<commit_message>
update test accroding to new configuration
</commit_message>
<xml_diff>
--- a/tests/regression_data/design_optimization.xlsx
+++ b/tests/regression_data/design_optimization.xlsx
@@ -499,7 +499,7 @@
         <v>1585000</v>
       </c>
       <c r="F2" t="n">
-        <v>3972.105864572915</v>
+        <v>3976.448895352781</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -647,70 +647,70 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.226938968589173</v>
+        <v>2.227042688033876</v>
       </c>
       <c r="C2" t="n">
-        <v>2.28391150791807</v>
+        <v>2.283911639304897</v>
       </c>
       <c r="D2" t="n">
-        <v>10.65999792392535</v>
+        <v>10.65999965361875</v>
       </c>
       <c r="E2" t="n">
-        <v>93.68342429346957</v>
+        <v>93.67808645241342</v>
       </c>
       <c r="F2" t="n">
-        <v>90.84026168250524</v>
+        <v>90.84031265372248</v>
       </c>
       <c r="G2" t="n">
-        <v>0.03034861964543415</v>
+        <v>0.03029282414017371</v>
       </c>
       <c r="H2" t="n">
-        <v>-89.87061030215068</v>
+        <v>-89.87060547786265</v>
       </c>
       <c r="I2" t="n">
-        <v>227072.0511165214</v>
+        <v>227072.2153732921</v>
       </c>
       <c r="J2" t="n">
-        <v>57.16666646319015</v>
+        <v>57.10427100890649</v>
       </c>
       <c r="K2" t="n">
-        <v>3972.105864572915</v>
+        <v>3976.448895352781</v>
       </c>
       <c r="L2" t="n">
-        <v>2.870498337071233</v>
+        <v>3.090530566745351</v>
       </c>
       <c r="M2" t="n">
-        <v>37.72667773428275</v>
+        <v>37.69198179992932</v>
       </c>
       <c r="N2" t="n">
         <v>216.5604229337033</v>
       </c>
       <c r="O2" t="n">
-        <v>185.3145011275188</v>
+        <v>185.5038172636049</v>
       </c>
       <c r="P2" t="n">
-        <v>0.8557173033608733</v>
+        <v>0.8565914988095222</v>
       </c>
       <c r="Q2" t="n">
         <v>497686.3106530505</v>
       </c>
       <c r="R2" t="n">
-        <v>476384.9883885424</v>
+        <v>476384.9764361954</v>
       </c>
       <c r="S2" t="n">
         <v>474237.1022624383</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9103156809626101</v>
+        <v>0.9113110780726753</v>
       </c>
       <c r="U2" t="n">
-        <v>0.6984722866202033</v>
+        <v>0.6989862158304685</v>
       </c>
       <c r="V2" t="n">
-        <v>0.8557173033608733</v>
+        <v>0.8565914988095222</v>
       </c>
       <c r="W2" t="n">
-        <v>1.012962320101543</v>
+        <v>1.014196781788576</v>
       </c>
     </row>
   </sheetData>
@@ -1362,10 +1362,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>12.38812096722824</v>
+        <v>12.38990724163974</v>
       </c>
       <c r="D2" t="n">
-        <v>12.38812096722824</v>
+        <v>12.38990724163974</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1374,10 +1374,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>12.38812096722824</v>
+        <v>12.38990724163974</v>
       </c>
       <c r="H2" t="n">
-        <v>12.38812096722824</v>
+        <v>12.38990724163974</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1386,102 +1386,102 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>463.0421461027376</v>
+        <v>463.0421150040211</v>
       </c>
       <c r="L2" t="n">
-        <v>3610331.183813308</v>
+        <v>3610328.398905194</v>
       </c>
       <c r="M2" t="n">
-        <v>125.8417393155188</v>
+        <v>125.8416444479905</v>
       </c>
       <c r="N2" t="n">
-        <v>468920.1207639751</v>
+        <v>468920.0991360247</v>
       </c>
       <c r="O2" t="n">
-        <v>497609.5778825011</v>
+        <v>497609.5557522508</v>
       </c>
       <c r="P2" t="n">
         <v>1837.707528152813</v>
       </c>
       <c r="Q2" t="n">
-        <v>-353326.4598625344</v>
+        <v>-353326.4248424391</v>
       </c>
       <c r="R2" t="n">
-        <v>962.2104995562338</v>
+        <v>962.210455394315</v>
       </c>
       <c r="S2" t="n">
-        <v>1093.997138446942</v>
+        <v>1093.997049278801</v>
       </c>
       <c r="T2" t="n">
-        <v>1.136962378763782</v>
+        <v>1.136962338276069</v>
       </c>
       <c r="U2" t="n">
-        <v>0.8943877066593975</v>
+        <v>0.8943877510689475</v>
       </c>
       <c r="V2" t="n">
-        <v>171.3352191216099</v>
+        <v>171.3352175015731</v>
       </c>
       <c r="W2" t="n">
-        <v>3694179.558997133</v>
+        <v>3694176.704229427</v>
       </c>
       <c r="X2" t="n">
-        <v>2.706961001840074e-07</v>
+        <v>2.706963093712084e-07</v>
       </c>
       <c r="Y2" t="n">
-        <v>3249166.048056762</v>
+        <v>3249163.65288824</v>
       </c>
       <c r="Z2" t="n">
-        <v>3.07771281987288e-07</v>
+        <v>3.077715088653912e-07</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.003320105106537163</v>
+        <v>0.003320104623385129</v>
       </c>
       <c r="AB2" t="n">
-        <v>2.133798734315975e-05</v>
+        <v>2.133798409767246e-05</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.02951130702197091</v>
+        <v>0.02951130243679343</v>
       </c>
       <c r="AD2" t="n">
-        <v>16.25810766468673</v>
+        <v>16.25585319706831</v>
       </c>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="n">
-        <v>3610331.183813308</v>
+        <v>3610328.398905194</v>
       </c>
       <c r="AH2" t="n">
-        <v>125.8417393155188</v>
+        <v>125.8416444479905</v>
       </c>
       <c r="AI2" t="n">
-        <v>125.8417393155188</v>
+        <v>125.8416444479905</v>
       </c>
       <c r="AJ2" t="n">
-        <v>468920.1207639751</v>
+        <v>468920.0991360247</v>
       </c>
       <c r="AK2" t="n">
-        <v>497609.5778825011</v>
+        <v>497609.5557522508</v>
       </c>
       <c r="AL2" t="n">
         <v>1837.707528152813</v>
       </c>
       <c r="AM2" t="n">
-        <v>962.2104995562338</v>
+        <v>962.210455394315</v>
       </c>
       <c r="AN2" t="n">
-        <v>1093.997138446942</v>
+        <v>1093.997049278801</v>
       </c>
       <c r="AO2" t="n">
-        <v>171.3352191216099</v>
+        <v>171.3352175015731</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.8943877066593975</v>
+        <v>0.8943877510689475</v>
       </c>
       <c r="AQ2" t="n">
-        <v>2.133798734315975e-05</v>
+        <v>2.133798409767246e-05</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.02951130702197091</v>
+        <v>0.02951130243679343</v>
       </c>
       <c r="AS2" t="n">
         <v>463.1499999987578</v>
@@ -1680,16 +1680,16 @@
         <v>0.02952721766241618</v>
       </c>
       <c r="DI2" t="n">
-        <v>0.07230341216907325</v>
+        <v>0.07231383846421409</v>
       </c>
       <c r="DJ2" t="n">
-        <v>0.07230341216907325</v>
+        <v>0.07231383846421409</v>
       </c>
       <c r="DK2" t="n">
-        <v>757470.9581053781</v>
+        <v>759317.1921973135</v>
       </c>
       <c r="DL2" t="n">
-        <v>10.6599999455916</v>
+        <v>10.65999997293771</v>
       </c>
       <c r="DM2" t="n">
         <v>497686.3106530505</v>
@@ -1711,358 +1711,358 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>119.0158128022878</v>
+        <v>119.0418871241251</v>
       </c>
       <c r="D3" t="n">
-        <v>22.67315499758701</v>
+        <v>22.67826107111551</v>
       </c>
       <c r="E3" t="n">
-        <v>116.8361747895086</v>
+        <v>116.8617446595047</v>
       </c>
       <c r="F3" t="n">
-        <v>79.01771978640866</v>
+        <v>79.01765174713842</v>
       </c>
       <c r="G3" t="n">
-        <v>119.0158128022878</v>
+        <v>119.0418871241251</v>
       </c>
       <c r="H3" t="n">
-        <v>22.67315499758701</v>
+        <v>22.67826107111551</v>
       </c>
       <c r="I3" t="n">
-        <v>116.8361747895086</v>
+        <v>116.8617446595047</v>
       </c>
       <c r="J3" t="n">
-        <v>79.01771978640866</v>
+        <v>79.01765174713842</v>
       </c>
       <c r="K3" t="n">
-        <v>453.2078194298383</v>
+        <v>453.2035767851328</v>
       </c>
       <c r="L3" t="n">
-        <v>2781503.179163435</v>
+        <v>2781184.474470288</v>
       </c>
       <c r="M3" t="n">
-        <v>97.41094440920666</v>
+        <v>97.40001062108095</v>
       </c>
       <c r="N3" t="n">
-        <v>462049.6098208613</v>
+        <v>462046.5729369614</v>
       </c>
       <c r="O3" t="n">
-        <v>490603.9288045559</v>
+        <v>490600.8252079395</v>
       </c>
       <c r="P3" t="n">
-        <v>1838.710694368773</v>
+        <v>1838.711065814871</v>
       </c>
       <c r="Q3" t="n">
-        <v>-342714.1355526394</v>
+        <v>-342709.6064937637</v>
       </c>
       <c r="R3" t="n">
-        <v>947.9655242476334</v>
+        <v>947.9593802929335</v>
       </c>
       <c r="S3" t="n">
-        <v>1066.064546081332</v>
+        <v>1066.053138041856</v>
       </c>
       <c r="T3" t="n">
-        <v>1.124581557886749</v>
+        <v>1.124576812260067</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9094910415027115</v>
+        <v>0.9094974307578179</v>
       </c>
       <c r="V3" t="n">
-        <v>171.1108493016974</v>
+        <v>171.1107948571363</v>
       </c>
       <c r="W3" t="n">
-        <v>2852087.516239766</v>
+        <v>2851765.571934444</v>
       </c>
       <c r="X3" t="n">
-        <v>3.506203769365446e-07</v>
+        <v>3.506599595147185e-07</v>
       </c>
       <c r="Y3" t="n">
-        <v>2536132.21401145</v>
+        <v>2535856.635887092</v>
       </c>
       <c r="Z3" t="n">
-        <v>3.943012097221384e-07</v>
+        <v>3.943440594583062e-07</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.003163678803647447</v>
+        <v>0.003163617434231275</v>
       </c>
       <c r="AB3" t="n">
-        <v>2.038626753246112e-05</v>
+        <v>2.038589962153135e-05</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.02810977154019901</v>
+        <v>0.02810919898684134</v>
       </c>
       <c r="AD3" t="n">
-        <v>3.139787371995992</v>
+        <v>3.139358796022666</v>
       </c>
       <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="n">
-        <v>2781503.179163435</v>
+        <v>2781184.474470288</v>
       </c>
       <c r="AH3" t="n">
-        <v>97.41094440920666</v>
+        <v>97.40001062108095</v>
       </c>
       <c r="AI3" t="n">
-        <v>97.41094440920666</v>
+        <v>97.40001062108095</v>
       </c>
       <c r="AJ3" t="n">
-        <v>462049.6098208613</v>
+        <v>462046.5729369614</v>
       </c>
       <c r="AK3" t="n">
-        <v>490603.9288045559</v>
+        <v>490600.8252079395</v>
       </c>
       <c r="AL3" t="n">
-        <v>1838.710694368773</v>
+        <v>1838.711065814871</v>
       </c>
       <c r="AM3" t="n">
-        <v>947.9655242476334</v>
+        <v>947.9593802929335</v>
       </c>
       <c r="AN3" t="n">
-        <v>1066.064546081332</v>
+        <v>1066.053138041856</v>
       </c>
       <c r="AO3" t="n">
-        <v>171.1108493016974</v>
+        <v>171.1107948571363</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.9094910415027115</v>
+        <v>0.9094974307578179</v>
       </c>
       <c r="AQ3" t="n">
-        <v>2.038626753246112e-05</v>
+        <v>2.038589962153135e-05</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.02810977154019901</v>
+        <v>0.02810919898684134</v>
       </c>
       <c r="AS3" t="n">
-        <v>462.9231882062415</v>
+        <v>462.923104892691</v>
       </c>
       <c r="AT3" t="n">
-        <v>3561895.056455894</v>
+        <v>3561873.731643836</v>
       </c>
       <c r="AU3" t="n">
-        <v>124.0170900335747</v>
+        <v>124.0163000864333</v>
       </c>
       <c r="AV3" t="n">
-        <v>468965.308930766</v>
+        <v>468965.2979380261</v>
       </c>
       <c r="AW3" t="n">
-        <v>497686.3106531222</v>
+        <v>497686.3106529787</v>
       </c>
       <c r="AX3" t="n">
-        <v>1838.710694368772</v>
+        <v>1838.71106581487</v>
       </c>
       <c r="AY3" t="n">
-        <v>-353495.506172982</v>
+        <v>-353495.5249345902</v>
       </c>
       <c r="AZ3" t="n">
-        <v>961.8097081693035</v>
+        <v>961.8095044357805</v>
       </c>
       <c r="BA3" t="n">
-        <v>1092.55545898897</v>
+        <v>1092.554816777956</v>
       </c>
       <c r="BB3" t="n">
-        <v>1.135937233435214</v>
+        <v>1.135936806341786</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.8956011874832537</v>
+        <v>0.8956016914470506</v>
       </c>
       <c r="BD3" t="n">
-        <v>171.4488132042876</v>
+        <v>171.4488533266321</v>
       </c>
       <c r="BE3" t="n">
-        <v>3645444.604429532</v>
+        <v>3645423.090372493</v>
       </c>
       <c r="BF3" t="n">
-        <v>2.743149625109961e-07</v>
+        <v>2.743165814253453e-07</v>
       </c>
       <c r="BG3" t="n">
-        <v>3209195.45299634</v>
+        <v>3209177.720116626</v>
       </c>
       <c r="BH3" t="n">
-        <v>3.116045796046254e-07</v>
+        <v>3.116063014309032e-07</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.00330371068699786</v>
+        <v>0.003303704050311836</v>
       </c>
       <c r="BJ3" t="n">
-        <v>2.129411966481703e-05</v>
+        <v>2.129409952281714e-05</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.02946683015074973</v>
+        <v>0.02946680802999982</v>
       </c>
       <c r="BL3" t="n">
-        <v>7.976917007659525</v>
+        <v>7.975887984568375</v>
       </c>
       <c r="BM3" t="inlineStr"/>
       <c r="BN3" t="inlineStr"/>
       <c r="BO3" t="n">
-        <v>3561895.056455894</v>
+        <v>3561873.731643836</v>
       </c>
       <c r="BP3" t="n">
-        <v>124.0170900335747</v>
+        <v>124.0163000864333</v>
       </c>
       <c r="BQ3" t="n">
-        <v>124.0170900335747</v>
+        <v>124.0163000864333</v>
       </c>
       <c r="BR3" t="n">
-        <v>468965.308930766</v>
+        <v>468965.2979380261</v>
       </c>
       <c r="BS3" t="n">
-        <v>497686.3106531222</v>
+        <v>497686.3106529787</v>
       </c>
       <c r="BT3" t="n">
-        <v>1838.710694368772</v>
+        <v>1838.71106581487</v>
       </c>
       <c r="BU3" t="n">
-        <v>961.8097081693035</v>
+        <v>961.8095044357805</v>
       </c>
       <c r="BV3" t="n">
-        <v>1092.55545898897</v>
+        <v>1092.554816777956</v>
       </c>
       <c r="BW3" t="n">
-        <v>171.4488132042876</v>
+        <v>171.4488533266321</v>
       </c>
       <c r="BX3" t="n">
-        <v>0.8956011874832537</v>
+        <v>0.8956016914470506</v>
       </c>
       <c r="BY3" t="n">
-        <v>2.129411966481703e-05</v>
+        <v>2.129409952281714e-05</v>
       </c>
       <c r="BZ3" t="n">
-        <v>0.02946683015074973</v>
+        <v>0.02946680802999982</v>
       </c>
       <c r="CA3" t="n">
-        <v>462.9231882062415</v>
+        <v>462.923104892691</v>
       </c>
       <c r="CB3" t="n">
-        <v>3561895.056455894</v>
+        <v>3561873.731643836</v>
       </c>
       <c r="CC3" t="n">
-        <v>124.0170900335747</v>
+        <v>124.0163000864333</v>
       </c>
       <c r="CD3" t="n">
-        <v>468965.308930766</v>
+        <v>468965.2979380261</v>
       </c>
       <c r="CE3" t="n">
-        <v>497686.3106531222</v>
+        <v>497686.3106529787</v>
       </c>
       <c r="CF3" t="n">
-        <v>1838.710694368772</v>
+        <v>1838.71106581487</v>
       </c>
       <c r="CG3" t="n">
-        <v>-353495.506172982</v>
+        <v>-353495.5249345902</v>
       </c>
       <c r="CH3" t="n">
-        <v>961.8097081693035</v>
+        <v>961.8095044357805</v>
       </c>
       <c r="CI3" t="n">
-        <v>1092.55545898897</v>
+        <v>1092.554816777956</v>
       </c>
       <c r="CJ3" t="n">
-        <v>1.135937233435214</v>
+        <v>1.135936806341786</v>
       </c>
       <c r="CK3" t="n">
-        <v>0.8956011874832537</v>
+        <v>0.8956016914470506</v>
       </c>
       <c r="CL3" t="n">
-        <v>171.4488132042876</v>
+        <v>171.4488533266321</v>
       </c>
       <c r="CM3" t="n">
-        <v>3645444.604429532</v>
+        <v>3645423.090372493</v>
       </c>
       <c r="CN3" t="n">
-        <v>2.743149625109961e-07</v>
+        <v>2.743165814253453e-07</v>
       </c>
       <c r="CO3" t="n">
-        <v>3209195.45299634</v>
+        <v>3209177.720116626</v>
       </c>
       <c r="CP3" t="n">
-        <v>3.116045796046254e-07</v>
+        <v>3.116063014309032e-07</v>
       </c>
       <c r="CQ3" t="n">
-        <v>0.00330371068699786</v>
+        <v>0.003303704050311836</v>
       </c>
       <c r="CR3" t="n">
-        <v>2.129411966481703e-05</v>
+        <v>2.129409952281714e-05</v>
       </c>
       <c r="CS3" t="n">
-        <v>0.02946683015074973</v>
+        <v>0.02946680802999982</v>
       </c>
       <c r="CT3" t="n">
-        <v>7.976917007659525</v>
+        <v>7.975887984568375</v>
       </c>
       <c r="CU3" t="inlineStr"/>
       <c r="CV3" t="inlineStr"/>
       <c r="CW3" t="n">
-        <v>3561895.056455894</v>
+        <v>3561873.731643836</v>
       </c>
       <c r="CX3" t="n">
-        <v>124.0170900335747</v>
+        <v>124.0163000864333</v>
       </c>
       <c r="CY3" t="n">
-        <v>124.0170900335747</v>
+        <v>124.0163000864333</v>
       </c>
       <c r="CZ3" t="n">
-        <v>468965.308930766</v>
+        <v>468965.2979380261</v>
       </c>
       <c r="DA3" t="n">
-        <v>497686.3106531222</v>
+        <v>497686.3106529787</v>
       </c>
       <c r="DB3" t="n">
-        <v>1838.710694368772</v>
+        <v>1838.71106581487</v>
       </c>
       <c r="DC3" t="n">
-        <v>961.8097081693035</v>
+        <v>961.8095044357805</v>
       </c>
       <c r="DD3" t="n">
-        <v>1092.55545898897</v>
+        <v>1092.554816777956</v>
       </c>
       <c r="DE3" t="n">
-        <v>171.4488132042876</v>
+        <v>171.4488533266321</v>
       </c>
       <c r="DF3" t="n">
-        <v>0.8956011874832537</v>
+        <v>0.8956016914470506</v>
       </c>
       <c r="DG3" t="n">
-        <v>2.129411966481703e-05</v>
+        <v>2.129409952281714e-05</v>
       </c>
       <c r="DH3" t="n">
-        <v>0.02946683015074973</v>
+        <v>0.02946680802999982</v>
       </c>
       <c r="DI3" t="n">
-        <v>0.6955480221621879</v>
+        <v>0.6957006261557926</v>
       </c>
       <c r="DJ3" t="n">
-        <v>0.6955480221621878</v>
+        <v>0.6957006261557926</v>
       </c>
       <c r="DK3" t="n">
-        <v>5896088.469719783</v>
+        <v>5910348.726371001</v>
       </c>
       <c r="DL3" t="n">
-        <v>10.65999993356908</v>
+        <v>10.66000004754654</v>
       </c>
       <c r="DM3" t="n">
         <v>497686.3106530505</v>
       </c>
       <c r="DN3" t="n">
-        <v>0.02229127449784395</v>
+        <v>0.02228041746933479</v>
       </c>
       <c r="DO3" t="n">
         <v>0</v>
       </c>
       <c r="DP3" t="n">
-        <v>0.01154788397553874</v>
+        <v>0.01154788426814579</v>
       </c>
       <c r="DQ3" t="n">
-        <v>0.04061695417700555</v>
+        <v>0.04062680325903407</v>
       </c>
       <c r="DR3" t="n">
         <v>0</v>
       </c>
       <c r="DS3" t="n">
-        <v>0.07445611265038825</v>
+        <v>0.07445510499651464</v>
       </c>
       <c r="DT3" t="n">
-        <v>-2.593142131579462e-09</v>
+        <v>-4.136982939551004e-08</v>
       </c>
       <c r="DU3" t="n">
         <v>0</v>
@@ -2073,340 +2073,340 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>185.3145011275188</v>
+        <v>185.5038172636049</v>
       </c>
       <c r="C4" t="n">
-        <v>119.0158128023331</v>
+        <v>119.0418871240997</v>
       </c>
       <c r="D4" t="n">
-        <v>22.67315499782513</v>
+        <v>22.67826107098182</v>
       </c>
       <c r="E4" t="n">
-        <v>116.8361747895085</v>
+        <v>116.8617446595047</v>
       </c>
       <c r="F4" t="n">
-        <v>79.01771978629611</v>
+        <v>79.01765174720158</v>
       </c>
       <c r="G4" t="n">
-        <v>72.13427157468514</v>
+        <v>72.29133873840054</v>
       </c>
       <c r="H4" t="n">
-        <v>22.67315499782513</v>
+        <v>22.67826107098182</v>
       </c>
       <c r="I4" t="n">
-        <v>-68.47832633801023</v>
+        <v>-68.64207260410019</v>
       </c>
       <c r="J4" t="n">
-        <v>-71.68030696607227</v>
+        <v>-71.71725745657214</v>
       </c>
       <c r="K4" t="n">
-        <v>453.2078194300026</v>
+        <v>453.2035767852385</v>
       </c>
       <c r="L4" t="n">
-        <v>2781503.179171203</v>
+        <v>2781184.474477571</v>
       </c>
       <c r="M4" t="n">
-        <v>97.41094440945442</v>
+        <v>97.40001062132806</v>
       </c>
       <c r="N4" t="n">
-        <v>462049.6098209947</v>
+        <v>462046.5729370393</v>
       </c>
       <c r="O4" t="n">
-        <v>490603.9288046965</v>
+        <v>490600.8252080198</v>
       </c>
       <c r="P4" t="n">
-        <v>1838.710694368907</v>
+        <v>1838.711065814882</v>
       </c>
       <c r="Q4" t="n">
-        <v>-342714.135552862</v>
+        <v>-342709.606493883</v>
       </c>
       <c r="R4" t="n">
-        <v>947.9655242478402</v>
+        <v>947.9593802930822</v>
       </c>
       <c r="S4" t="n">
-        <v>1066.064546081639</v>
+        <v>1066.05313804212</v>
       </c>
       <c r="T4" t="n">
-        <v>1.124581557886827</v>
+        <v>1.12457681226017</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9094910415026085</v>
+        <v>0.9094974307576799</v>
       </c>
       <c r="V4" t="n">
-        <v>171.1108493017177</v>
+        <v>171.1107948571404</v>
       </c>
       <c r="W4" t="n">
-        <v>2852087.516247699</v>
+        <v>2851765.571941813</v>
       </c>
       <c r="X4" t="n">
-        <v>3.506203769355694e-07</v>
+        <v>3.506599595138123e-07</v>
       </c>
       <c r="Y4" t="n">
-        <v>2536132.214018327</v>
+        <v>2535856.635893414</v>
       </c>
       <c r="Z4" t="n">
-        <v>3.943012097210693e-07</v>
+        <v>3.943440594573232e-07</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.003163678803647948</v>
+        <v>0.003163617434232532</v>
       </c>
       <c r="AB4" t="n">
-        <v>2.038626753247326e-05</v>
+        <v>2.038589962153989e-05</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.02810977154021816</v>
+        <v>0.02810919898685517</v>
       </c>
       <c r="AD4" t="n">
-        <v>3.139787372007381</v>
+        <v>3.139358796032601</v>
       </c>
       <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="n">
-        <v>2781503.179171203</v>
+        <v>2781184.474477571</v>
       </c>
       <c r="AH4" t="n">
-        <v>97.41094440945442</v>
+        <v>97.40001062132806</v>
       </c>
       <c r="AI4" t="n">
-        <v>97.41094440945442</v>
+        <v>97.40001062132806</v>
       </c>
       <c r="AJ4" t="n">
-        <v>462049.6098209947</v>
+        <v>462046.5729370393</v>
       </c>
       <c r="AK4" t="n">
-        <v>490603.9288046965</v>
+        <v>490600.8252080198</v>
       </c>
       <c r="AL4" t="n">
-        <v>1838.710694368907</v>
+        <v>1838.711065814882</v>
       </c>
       <c r="AM4" t="n">
-        <v>947.9655242478402</v>
+        <v>947.9593802930822</v>
       </c>
       <c r="AN4" t="n">
-        <v>1066.064546081639</v>
+        <v>1066.05313804212</v>
       </c>
       <c r="AO4" t="n">
-        <v>171.1108493017177</v>
+        <v>171.1107948571404</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.9094910415026085</v>
+        <v>0.9094974307576799</v>
       </c>
       <c r="AQ4" t="n">
-        <v>2.038626753247326e-05</v>
+        <v>2.038589962153989e-05</v>
       </c>
       <c r="AR4" t="n">
-        <v>0.02810977154021816</v>
+        <v>0.02810919898685517</v>
       </c>
       <c r="AS4" t="n">
-        <v>462.9231882061114</v>
+        <v>462.9231048926883</v>
       </c>
       <c r="AT4" t="n">
-        <v>3561895.056439299</v>
+        <v>3561873.731643156</v>
       </c>
       <c r="AU4" t="n">
-        <v>124.0170900329867</v>
+        <v>124.016300086408</v>
       </c>
       <c r="AV4" t="n">
-        <v>468965.3089306924</v>
+        <v>468965.2979380256</v>
       </c>
       <c r="AW4" t="n">
-        <v>497686.3106530508</v>
+        <v>497686.3106529787</v>
       </c>
       <c r="AX4" t="n">
-        <v>1838.710694368908</v>
+        <v>1838.711065814882</v>
       </c>
       <c r="AY4" t="n">
-        <v>-353495.5061728768</v>
+        <v>-353495.5249345907</v>
       </c>
       <c r="AZ4" t="n">
-        <v>961.8097081690879</v>
+        <v>961.8095044357738</v>
       </c>
       <c r="BA4" t="n">
-        <v>1092.555458988452</v>
+        <v>1092.554816777935</v>
       </c>
       <c r="BB4" t="n">
-        <v>1.135937233434931</v>
+        <v>1.135936806341772</v>
       </c>
       <c r="BC4" t="n">
-        <v>0.895601187483579</v>
+        <v>0.8956016914470669</v>
       </c>
       <c r="BD4" t="n">
-        <v>171.4488132042971</v>
+        <v>171.4488533266334</v>
       </c>
       <c r="BE4" t="n">
-        <v>3645444.604412652</v>
+        <v>3645423.090371807</v>
       </c>
       <c r="BF4" t="n">
-        <v>2.743149625122663e-07</v>
+        <v>2.74316581425397e-07</v>
       </c>
       <c r="BG4" t="n">
-        <v>3209195.452982281</v>
+        <v>3209177.72011606</v>
       </c>
       <c r="BH4" t="n">
-        <v>3.116045796059905e-07</v>
+        <v>3.116063014309581e-07</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.003303710686993916</v>
+        <v>0.003303704050311623</v>
       </c>
       <c r="BJ4" t="n">
-        <v>2.129411966479951e-05</v>
+        <v>2.129409952281705e-05</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.02946683015072706</v>
+        <v>0.0294668080299991</v>
       </c>
       <c r="BL4" t="n">
-        <v>7.976917006858202</v>
+        <v>7.975887984536678</v>
       </c>
       <c r="BM4" t="inlineStr"/>
       <c r="BN4" t="inlineStr"/>
       <c r="BO4" t="n">
-        <v>3561895.056439299</v>
+        <v>3561873.731643156</v>
       </c>
       <c r="BP4" t="n">
-        <v>124.0170900329867</v>
+        <v>124.016300086408</v>
       </c>
       <c r="BQ4" t="n">
-        <v>124.0170900329867</v>
+        <v>124.016300086408</v>
       </c>
       <c r="BR4" t="n">
-        <v>468965.3089306924</v>
+        <v>468965.2979380256</v>
       </c>
       <c r="BS4" t="n">
-        <v>497686.3106530508</v>
+        <v>497686.3106529787</v>
       </c>
       <c r="BT4" t="n">
-        <v>1838.710694368908</v>
+        <v>1838.711065814882</v>
       </c>
       <c r="BU4" t="n">
-        <v>961.8097081690879</v>
+        <v>961.8095044357738</v>
       </c>
       <c r="BV4" t="n">
-        <v>1092.555458988452</v>
+        <v>1092.554816777935</v>
       </c>
       <c r="BW4" t="n">
-        <v>171.4488132042971</v>
+        <v>171.4488533266334</v>
       </c>
       <c r="BX4" t="n">
-        <v>0.895601187483579</v>
+        <v>0.8956016914470669</v>
       </c>
       <c r="BY4" t="n">
-        <v>2.129411966479951e-05</v>
+        <v>2.129409952281705e-05</v>
       </c>
       <c r="BZ4" t="n">
-        <v>0.02946683015072706</v>
+        <v>0.0294668080299991</v>
       </c>
       <c r="CA4" t="n">
-        <v>456.7317968978804</v>
+        <v>456.7429629220757</v>
       </c>
       <c r="CB4" t="n">
-        <v>3046531.641631569</v>
+        <v>3047390.770152799</v>
       </c>
       <c r="CC4" t="n">
-        <v>106.4579699226598</v>
+        <v>106.487226582791</v>
       </c>
       <c r="CD4" t="n">
-        <v>464588.3807170556</v>
+        <v>464596.4138717342</v>
       </c>
       <c r="CE4" t="n">
-        <v>493205.6053724274</v>
+        <v>493213.8440363139</v>
       </c>
       <c r="CF4" t="n">
-        <v>1838.710694368907</v>
+        <v>1838.711065814882</v>
       </c>
       <c r="CG4" t="n">
-        <v>-346592.034042033</v>
+        <v>-346604.496121583</v>
       </c>
       <c r="CH4" t="n">
-        <v>952.9989785150415</v>
+        <v>953.0148291229207</v>
       </c>
       <c r="CI4" t="n">
-        <v>1075.408459857067</v>
+        <v>1075.4381811292</v>
       </c>
       <c r="CJ4" t="n">
-        <v>1.128446602883838</v>
+        <v>1.128459021061559</v>
       </c>
       <c r="CK4" t="n">
-        <v>0.9044619030102913</v>
+        <v>0.9044462866367438</v>
       </c>
       <c r="CL4" t="n">
-        <v>171.2048701559743</v>
+        <v>171.2052540470054</v>
       </c>
       <c r="CM4" t="n">
-        <v>3120401.007567819</v>
+        <v>3121272.550231584</v>
       </c>
       <c r="CN4" t="n">
-        <v>3.204716309136963e-07</v>
+        <v>3.203821466746967e-07</v>
       </c>
       <c r="CO4" t="n">
-        <v>2765218.132247797</v>
+        <v>2765960.032199801</v>
       </c>
       <c r="CP4" t="n">
-        <v>3.616351232252039e-07</v>
+        <v>3.615381236021288e-07</v>
       </c>
       <c r="CQ4" t="n">
-        <v>0.003212190528961387</v>
+        <v>0.003212343721804881</v>
       </c>
       <c r="CR4" t="n">
-        <v>2.069539505687771e-05</v>
+        <v>2.069639940915096e-05</v>
       </c>
       <c r="CS4" t="n">
-        <v>0.02858710372733998</v>
+        <v>0.02858863389510442</v>
       </c>
       <c r="CT4" t="n">
-        <v>3.596962471350485</v>
+        <v>3.598878927962373</v>
       </c>
       <c r="CU4" t="inlineStr"/>
       <c r="CV4" t="inlineStr"/>
       <c r="CW4" t="n">
-        <v>3046531.641631569</v>
+        <v>3047390.770152799</v>
       </c>
       <c r="CX4" t="n">
-        <v>106.4579699226598</v>
+        <v>106.487226582791</v>
       </c>
       <c r="CY4" t="n">
-        <v>106.4579699226598</v>
+        <v>106.487226582791</v>
       </c>
       <c r="CZ4" t="n">
-        <v>464588.3807170556</v>
+        <v>464596.4138717342</v>
       </c>
       <c r="DA4" t="n">
-        <v>493205.6053724274</v>
+        <v>493213.8440363139</v>
       </c>
       <c r="DB4" t="n">
-        <v>1838.710694368907</v>
+        <v>1838.711065814882</v>
       </c>
       <c r="DC4" t="n">
-        <v>952.9989785150415</v>
+        <v>953.0148291229207</v>
       </c>
       <c r="DD4" t="n">
-        <v>1075.408459857067</v>
+        <v>1075.4381811292</v>
       </c>
       <c r="DE4" t="n">
-        <v>171.2048701559743</v>
+        <v>171.2052540470054</v>
       </c>
       <c r="DF4" t="n">
-        <v>0.9044619030102913</v>
+        <v>0.9044462866367438</v>
       </c>
       <c r="DG4" t="n">
-        <v>2.069539505687771e-05</v>
+        <v>2.069639940915096e-05</v>
       </c>
       <c r="DH4" t="n">
-        <v>0.02858710372733998</v>
+        <v>0.02858863389510442</v>
       </c>
       <c r="DI4" t="n">
-        <v>0.6955480221623699</v>
+        <v>0.6957006261556274</v>
       </c>
       <c r="DJ4" t="n">
-        <v>0.4215645698040552</v>
+        <v>0.4224826306181106</v>
       </c>
       <c r="DK4" t="n">
-        <v>2906089.687979076</v>
+        <v>2913195.82880023</v>
       </c>
       <c r="DL4" t="n">
-        <v>10.6599999335962</v>
+        <v>10.66000004757358</v>
       </c>
       <c r="DM4" t="n">
-        <v>476034.8732083568</v>
+        <v>476008.0109265559</v>
       </c>
       <c r="DN4" t="inlineStr"/>
       <c r="DO4" t="inlineStr"/>
@@ -2422,361 +2422,361 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>185.3145011275188</v>
+        <v>185.5038172636049</v>
       </c>
       <c r="C5" t="n">
-        <v>37.72667773428275</v>
+        <v>37.69198179992932</v>
       </c>
       <c r="D5" t="n">
-        <v>37.6793411343868</v>
+        <v>37.63716237221433</v>
       </c>
       <c r="E5" t="n">
-        <v>1.889302661018917</v>
+        <v>2.032117263786063</v>
       </c>
       <c r="F5" t="n">
-        <v>2.870498337071233</v>
+        <v>3.090530566745351</v>
       </c>
       <c r="G5" t="n">
-        <v>187.2552701015284</v>
+        <v>187.2923401857533</v>
       </c>
       <c r="H5" t="n">
-        <v>37.6793411343868</v>
+        <v>37.63716237221433</v>
       </c>
       <c r="I5" t="n">
-        <v>-183.4251984664998</v>
+        <v>-183.4716999998188</v>
       </c>
       <c r="J5" t="n">
-        <v>-78.39174094925701</v>
+        <v>-78.40724266020219</v>
       </c>
       <c r="K5" t="n">
-        <v>433.5640351644821</v>
+        <v>433.56530857402</v>
       </c>
       <c r="L5" t="n">
-        <v>1585000.11380004</v>
+        <v>1585000.022619571</v>
       </c>
       <c r="M5" t="n">
-        <v>56.28856781638315</v>
+        <v>56.28835433983492</v>
       </c>
       <c r="N5" t="n">
-        <v>447514.8643401365</v>
+        <v>447516.0555754492</v>
       </c>
       <c r="O5" t="n">
-        <v>475673.3372821096</v>
+        <v>475674.6336900322</v>
       </c>
       <c r="P5" t="n">
-        <v>1841.025553341608</v>
+        <v>1841.028547192089</v>
       </c>
       <c r="Q5" t="n">
-        <v>-322529.1304656015</v>
+        <v>-322531.4764668855</v>
       </c>
       <c r="R5" t="n">
-        <v>919.4601191291863</v>
+        <v>919.4614595754555</v>
       </c>
       <c r="S5" t="n">
-        <v>1017.716035662872</v>
+        <v>1017.717043796976</v>
       </c>
       <c r="T5" t="n">
-        <v>1.106862619149532</v>
+        <v>1.106862101938333</v>
       </c>
       <c r="U5" t="n">
-        <v>0.9375185349113633</v>
+        <v>0.9375192830035907</v>
       </c>
       <c r="V5" t="n">
-        <v>170.9308572299604</v>
+        <v>170.9312099953958</v>
       </c>
       <c r="W5" t="n">
-        <v>1644603.234573759</v>
+        <v>1644603.785566514</v>
       </c>
       <c r="X5" t="n">
-        <v>6.080493939069599e-07</v>
+        <v>6.080491901917469e-07</v>
       </c>
       <c r="Y5" t="n">
-        <v>1485824.171962195</v>
+        <v>1485825.364050761</v>
       </c>
       <c r="Z5" t="n">
-        <v>6.73027144712143e-07</v>
+        <v>6.730266047375381e-07</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.002930077587493272</v>
+        <v>0.002930061598049747</v>
       </c>
       <c r="AB5" t="n">
-        <v>1.894954586459172e-05</v>
+        <v>1.894959181281052e-05</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.0256855039082108</v>
+        <v>0.02568561359144396</v>
       </c>
       <c r="AD5" t="n">
-        <v>2.254265723971397</v>
+        <v>2.254278124056925</v>
       </c>
       <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="inlineStr"/>
       <c r="AG5" t="n">
-        <v>1585000.11380004</v>
+        <v>1585000.022619571</v>
       </c>
       <c r="AH5" t="n">
-        <v>56.28856781638315</v>
+        <v>56.28835433983492</v>
       </c>
       <c r="AI5" t="n">
-        <v>56.28856781638315</v>
+        <v>56.28835433983492</v>
       </c>
       <c r="AJ5" t="n">
-        <v>447514.8643401365</v>
+        <v>447516.0555754492</v>
       </c>
       <c r="AK5" t="n">
-        <v>475673.3372821096</v>
+        <v>475674.6336900322</v>
       </c>
       <c r="AL5" t="n">
-        <v>1841.025553341608</v>
+        <v>1841.028547192089</v>
       </c>
       <c r="AM5" t="n">
-        <v>919.4601191291863</v>
+        <v>919.4614595754555</v>
       </c>
       <c r="AN5" t="n">
-        <v>1017.716035662872</v>
+        <v>1017.717043796976</v>
       </c>
       <c r="AO5" t="n">
-        <v>170.9308572299604</v>
+        <v>170.9312099953958</v>
       </c>
       <c r="AP5" t="n">
-        <v>0.9375185349113633</v>
+        <v>0.9375192830035907</v>
       </c>
       <c r="AQ5" t="n">
-        <v>1.894954586459172e-05</v>
+        <v>1.894959181281052e-05</v>
       </c>
       <c r="AR5" t="n">
-        <v>0.0256855039082108</v>
+        <v>0.02568561359144396</v>
       </c>
       <c r="AS5" t="n">
-        <v>434.4535040218728</v>
+        <v>434.4531369089998</v>
       </c>
       <c r="AT5" t="n">
-        <v>1625549.712416561</v>
+        <v>1625474.006138268</v>
       </c>
       <c r="AU5" t="n">
-        <v>57.67619749430219</v>
+        <v>57.67339111615116</v>
       </c>
       <c r="AV5" t="n">
-        <v>448200.9231582167</v>
+        <v>448200.8524462492</v>
       </c>
       <c r="AW5" t="n">
-        <v>476384.9883885424</v>
+        <v>476384.9764361954</v>
       </c>
       <c r="AX5" t="n">
-        <v>1841.025553341449</v>
+        <v>1841.02854719193</v>
       </c>
       <c r="AY5" t="n">
-        <v>-323455.0142544574</v>
+        <v>-323455.6510303572</v>
       </c>
       <c r="AZ5" t="n">
-        <v>920.7287858840798</v>
+        <v>920.7277799447118</v>
       </c>
       <c r="BA5" t="n">
-        <v>1019.645993601932</v>
+        <v>1019.64341447234</v>
       </c>
       <c r="BB5" t="n">
-        <v>1.107433599594556</v>
+        <v>1.107432008333199</v>
       </c>
       <c r="BC5" t="n">
-        <v>0.9364494614489639</v>
+        <v>0.9364522051094057</v>
       </c>
       <c r="BD5" t="n">
-        <v>170.9589059163501</v>
+        <v>170.959209779184</v>
       </c>
       <c r="BE5" t="n">
-        <v>1685699.196864374</v>
+        <v>1685623.167044072</v>
       </c>
       <c r="BF5" t="n">
-        <v>5.932256489533444e-07</v>
+        <v>5.932524063214031e-07</v>
       </c>
       <c r="BG5" t="n">
-        <v>1522167.286130318</v>
+        <v>1522100.819156484</v>
       </c>
       <c r="BH5" t="n">
-        <v>6.569580157922186e-07</v>
+        <v>6.569867037810144e-07</v>
       </c>
       <c r="BI5" t="n">
-        <v>0.002937185598809374</v>
+        <v>0.002937156152302595</v>
       </c>
       <c r="BJ5" t="n">
-        <v>1.900376954036744e-05</v>
+        <v>1.900371475341122e-05</v>
       </c>
       <c r="BK5" t="n">
-        <v>0.02578509101373902</v>
+        <v>0.02578501642097159</v>
       </c>
       <c r="BL5" t="n">
-        <v>2.27304552030751</v>
+        <v>2.273022698324746</v>
       </c>
       <c r="BM5" t="inlineStr"/>
       <c r="BN5" t="inlineStr"/>
       <c r="BO5" t="n">
-        <v>1625549.712416561</v>
+        <v>1625474.006138268</v>
       </c>
       <c r="BP5" t="n">
-        <v>57.67619749430219</v>
+        <v>57.67339111615116</v>
       </c>
       <c r="BQ5" t="n">
-        <v>57.67619749430219</v>
+        <v>57.67339111615116</v>
       </c>
       <c r="BR5" t="n">
-        <v>448200.9231582167</v>
+        <v>448200.8524462492</v>
       </c>
       <c r="BS5" t="n">
-        <v>476384.9883885424</v>
+        <v>476384.9764361954</v>
       </c>
       <c r="BT5" t="n">
-        <v>1841.025553341449</v>
+        <v>1841.02854719193</v>
       </c>
       <c r="BU5" t="n">
-        <v>920.7287858840798</v>
+        <v>920.7277799447118</v>
       </c>
       <c r="BV5" t="n">
-        <v>1019.645993601932</v>
+        <v>1019.64341447234</v>
       </c>
       <c r="BW5" t="n">
-        <v>170.9589059163501</v>
+        <v>170.959209779184</v>
       </c>
       <c r="BX5" t="n">
-        <v>0.9364494614489639</v>
+        <v>0.9364522051094057</v>
       </c>
       <c r="BY5" t="n">
-        <v>1.900376954036744e-05</v>
+        <v>1.900371475341122e-05</v>
       </c>
       <c r="BZ5" t="n">
-        <v>0.02578509101373902</v>
+        <v>0.02578501642097159</v>
       </c>
       <c r="CA5" t="n">
-        <v>456.2810456472773</v>
+        <v>456.2916095919634</v>
       </c>
       <c r="CB5" t="n">
-        <v>2936207.141287523</v>
+        <v>2936910.783454746</v>
       </c>
       <c r="CC5" t="n">
-        <v>102.3717759153861</v>
+        <v>102.3952918478925</v>
       </c>
       <c r="CD5" t="n">
-        <v>464523.8020625542</v>
+        <v>464531.755920069</v>
       </c>
       <c r="CE5" t="n">
-        <v>493205.6053724274</v>
+        <v>493213.8440361663</v>
       </c>
       <c r="CF5" t="n">
-        <v>1841.025553341449</v>
+        <v>1841.028547191931</v>
       </c>
       <c r="CG5" t="n">
-        <v>-346819.4591695665</v>
+        <v>-346832.0350667938</v>
       </c>
       <c r="CH5" t="n">
-        <v>951.8569877576319</v>
+        <v>951.8713741154153</v>
       </c>
       <c r="CI5" t="n">
-        <v>1071.993510323528</v>
+        <v>1072.018600656589</v>
       </c>
       <c r="CJ5" t="n">
-        <v>1.126212786280964</v>
+        <v>1.126222123921762</v>
       </c>
       <c r="CK5" t="n">
-        <v>0.9073984609336703</v>
+        <v>0.9073864632094164</v>
       </c>
       <c r="CL5" t="n">
-        <v>171.4752406577332</v>
+        <v>171.4759126461675</v>
       </c>
       <c r="CM5" t="n">
-        <v>3010114.94128522</v>
+        <v>3010829.996015432</v>
       </c>
       <c r="CN5" t="n">
-        <v>3.322132275696532e-07</v>
+        <v>3.321343288473318e-07</v>
       </c>
       <c r="CO5" t="n">
-        <v>2672776.386445914</v>
+        <v>2673389.140617338</v>
       </c>
       <c r="CP5" t="n">
-        <v>3.741427846606111e-07</v>
+        <v>3.740570292617708e-07</v>
       </c>
       <c r="CQ5" t="n">
-        <v>0.003175631638834513</v>
+        <v>0.003175737065024842</v>
       </c>
       <c r="CR5" t="n">
-        <v>2.059852970028682e-05</v>
+        <v>2.059938808697962e-05</v>
       </c>
       <c r="CS5" t="n">
-        <v>0.02847448699469209</v>
+        <v>0.02847585657092499</v>
       </c>
       <c r="CT5" t="n">
-        <v>3.395545443186674</v>
+        <v>3.396818904364442</v>
       </c>
       <c r="CU5" t="inlineStr"/>
       <c r="CV5" t="inlineStr"/>
       <c r="CW5" t="n">
-        <v>2936207.141287523</v>
+        <v>2936910.783454746</v>
       </c>
       <c r="CX5" t="n">
-        <v>102.3717759153861</v>
+        <v>102.3952918478925</v>
       </c>
       <c r="CY5" t="n">
-        <v>102.3717759153861</v>
+        <v>102.3952918478925</v>
       </c>
       <c r="CZ5" t="n">
-        <v>464523.8020625542</v>
+        <v>464531.755920069</v>
       </c>
       <c r="DA5" t="n">
-        <v>493205.6053724274</v>
+        <v>493213.8440361663</v>
       </c>
       <c r="DB5" t="n">
-        <v>1841.025553341449</v>
+        <v>1841.028547191931</v>
       </c>
       <c r="DC5" t="n">
-        <v>951.8569877576319</v>
+        <v>951.8713741154153</v>
       </c>
       <c r="DD5" t="n">
-        <v>1071.993510323528</v>
+        <v>1072.018600656589</v>
       </c>
       <c r="DE5" t="n">
-        <v>171.4752406577332</v>
+        <v>171.4759126461675</v>
       </c>
       <c r="DF5" t="n">
-        <v>0.9073984609336703</v>
+        <v>0.9073864632094164</v>
       </c>
       <c r="DG5" t="n">
-        <v>2.059852970028682e-05</v>
+        <v>2.059938808697962e-05</v>
       </c>
       <c r="DH5" t="n">
-        <v>0.02847448699469209</v>
+        <v>0.02847585657092499</v>
       </c>
       <c r="DI5" t="n">
-        <v>0.2207130903434684</v>
+        <v>0.2205096529822996</v>
       </c>
       <c r="DJ5" t="n">
-        <v>1.095503018800204</v>
+        <v>1.095717629277873</v>
       </c>
       <c r="DK5" t="n">
-        <v>4689783.23639762</v>
+        <v>4692378.083824161</v>
       </c>
       <c r="DL5" t="n">
-        <v>10.65999792392535</v>
+        <v>10.65999965361875</v>
       </c>
       <c r="DM5" t="n">
-        <v>476034.8732083568</v>
+        <v>476008.0109265559</v>
       </c>
       <c r="DN5" t="n">
-        <v>0.03399796747457478</v>
+        <v>0.03412930154663323</v>
       </c>
       <c r="DO5" t="n">
         <v>0</v>
       </c>
       <c r="DP5" t="n">
-        <v>0.0115964666997288</v>
+        <v>0.01159638030554655</v>
       </c>
       <c r="DQ5" t="n">
-        <v>0.009128034832231867</v>
+        <v>0.009111793222892966</v>
       </c>
       <c r="DR5" t="n">
-        <v>0.02692667968747732</v>
+        <v>0.0268839855469697</v>
       </c>
       <c r="DS5" t="n">
-        <v>0.08164914869401277</v>
+        <v>0.08172146062204244</v>
       </c>
       <c r="DT5" t="n">
-        <v>-2.98370024978678e-07</v>
+        <v>-1.000865281208796e-07</v>
       </c>
       <c r="DU5" t="n">
         <v>0</v>
@@ -3498,150 +3498,150 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.02229127449784395</v>
+        <v>0.02228041746933479</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01154788397553874</v>
+        <v>0.01154788426814579</v>
       </c>
       <c r="E2" t="n">
-        <v>0.04061695417700555</v>
+        <v>0.04062680325903407</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.07445611265038825</v>
+        <v>0.07445510499651464</v>
       </c>
       <c r="H2" t="n">
-        <v>-2.593142131579462e-09</v>
+        <v>-4.136982939551004e-08</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>118.9330244298916</v>
+        <v>118.9590493501572</v>
       </c>
       <c r="K2" t="n">
-        <v>22.28582646532928</v>
+        <v>22.29070304910059</v>
       </c>
       <c r="L2" t="n">
-        <v>116.8263935880862</v>
+        <v>116.8519575354643</v>
       </c>
       <c r="M2" t="n">
-        <v>79.19999999999996</v>
+        <v>79.19999999999999</v>
       </c>
       <c r="N2" t="n">
-        <v>118.9330244298916</v>
+        <v>118.9590493501572</v>
       </c>
       <c r="O2" t="n">
-        <v>22.28582646532928</v>
+        <v>22.29070304910059</v>
       </c>
       <c r="P2" t="n">
-        <v>116.8263935880862</v>
+        <v>116.8519575354643</v>
       </c>
       <c r="Q2" t="n">
-        <v>79.19999999999996</v>
+        <v>79.19999999999999</v>
       </c>
       <c r="R2" t="n">
-        <v>453.4076361974311</v>
+        <v>453.4034563245988</v>
       </c>
       <c r="S2" t="n">
-        <v>2827151.614117123</v>
+        <v>2826844.848028497</v>
       </c>
       <c r="T2" t="n">
-        <v>99.10395016504833</v>
+        <v>99.09345819806305</v>
       </c>
       <c r="U2" t="n">
-        <v>462086.6450294523</v>
+        <v>462083.6247543594</v>
       </c>
       <c r="V2" t="n">
-        <v>490613.7785030299</v>
+        <v>490610.682941978</v>
       </c>
       <c r="W2" t="n">
-        <v>1837.707528152813</v>
+        <v>1837.707528152812</v>
       </c>
       <c r="X2" t="n">
-        <v>-342616.8478589611</v>
+        <v>-342612.2620362422</v>
       </c>
       <c r="Y2" t="n">
-        <v>948.4640457739717</v>
+        <v>948.4580611086354</v>
       </c>
       <c r="Z2" t="n">
-        <v>1067.508372115067</v>
+        <v>1067.497370419139</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.125512745445139</v>
+        <v>1.1255082477462</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.9082247176006932</v>
+        <v>0.9082306934989498</v>
       </c>
       <c r="AC2" t="n">
-        <v>170.9918231929987</v>
+        <v>170.9917238401696</v>
       </c>
       <c r="AD2" t="n">
-        <v>2897621.472377524</v>
+        <v>2897311.339208968</v>
       </c>
       <c r="AE2" t="n">
-        <v>3.451106397204777e-07</v>
+        <v>3.451475809544937e-07</v>
       </c>
       <c r="AF2" t="n">
-        <v>2574490.146028082</v>
+        <v>2574224.884633902</v>
       </c>
       <c r="AG2" t="n">
-        <v>3.884264235941232e-07</v>
+        <v>3.884664490539321e-07</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.003179141084158335</v>
+        <v>0.003179084241090683</v>
       </c>
       <c r="AI2" t="n">
-        <v>2.042581512372908e-05</v>
+        <v>2.042545607351146e-05</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.0281570948814075</v>
+        <v>0.02815653470887956</v>
       </c>
       <c r="AK2" t="n">
-        <v>3.196941795383916</v>
+        <v>3.196496677810477</v>
       </c>
       <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="n">
-        <v>2827151.614117123</v>
+        <v>2826844.848028497</v>
       </c>
       <c r="AO2" t="n">
-        <v>99.10395016504833</v>
+        <v>99.09345819806305</v>
       </c>
       <c r="AP2" t="n">
-        <v>99.10395016504833</v>
+        <v>99.09345819806305</v>
       </c>
       <c r="AQ2" t="n">
-        <v>462086.6450294523</v>
+        <v>462083.6247543594</v>
       </c>
       <c r="AR2" t="n">
-        <v>490613.7785030299</v>
+        <v>490610.682941978</v>
       </c>
       <c r="AS2" t="n">
-        <v>1837.707528152813</v>
+        <v>1837.707528152812</v>
       </c>
       <c r="AT2" t="n">
-        <v>948.4640457739717</v>
+        <v>948.4580611086354</v>
       </c>
       <c r="AU2" t="n">
-        <v>1067.508372115067</v>
+        <v>1067.497370419139</v>
       </c>
       <c r="AV2" t="n">
-        <v>170.9918231929987</v>
+        <v>170.9917238401696</v>
       </c>
       <c r="AW2" t="n">
-        <v>0.9082247176006932</v>
+        <v>0.9082306934989498</v>
       </c>
       <c r="AX2" t="n">
-        <v>2.042581512372908e-05</v>
+        <v>2.042545607351146e-05</v>
       </c>
       <c r="AY2" t="n">
-        <v>0.0281570948814075</v>
+        <v>0.02815653470887956</v>
       </c>
       <c r="AZ2" t="n">
         <v>463.149999998658</v>
@@ -3840,7 +3840,7 @@
         <v>0.02952721766240145</v>
       </c>
       <c r="DP2" t="n">
-        <v>0.02240369737932484</v>
+        <v>0.02239282692506289</v>
       </c>
       <c r="DQ2" t="n">
         <v>0</v>
@@ -3849,28 +3849,28 @@
         <v>0.0115471027744396</v>
       </c>
       <c r="DS2" t="n">
-        <v>0.0406017154945208</v>
+        <v>0.04061155519819309</v>
       </c>
       <c r="DT2" t="n">
         <v>0</v>
       </c>
       <c r="DU2" t="n">
-        <v>0.07455251564828524</v>
+        <v>0.07455148489769559</v>
       </c>
       <c r="DV2" t="n">
-        <v>-0.07455251563700328</v>
+        <v>-0.07455148488641798</v>
       </c>
       <c r="DW2" t="n">
-        <v>0.6955480221744392</v>
+        <v>0.6957006261972732</v>
       </c>
       <c r="DX2" t="n">
-        <v>0.6955480221744392</v>
+        <v>0.6957006261972732</v>
       </c>
       <c r="DY2" t="n">
-        <v>5982783.970337747</v>
+        <v>5997287.761595534</v>
       </c>
       <c r="DZ2" t="n">
-        <v>10.65999990632622</v>
+        <v>10.6599999587826</v>
       </c>
       <c r="EA2" t="n">
         <v>497686.3106530505</v>
@@ -3879,25 +3879,25 @@
         <v>0</v>
       </c>
       <c r="EC2" t="n">
-        <v>454.4289176680613</v>
+        <v>454.5928436220274</v>
       </c>
       <c r="ED2" t="n">
-        <v>-14.39999999999999</v>
+        <v>-14.39999999999901</v>
       </c>
       <c r="EE2" t="n">
-        <v>0.005719523344981186</v>
+        <v>0.005718931413538502</v>
       </c>
       <c r="EF2" t="n">
         <v>0</v>
       </c>
       <c r="EG2" t="n">
-        <v>0.01042154936631747</v>
+        <v>0.01042807666012172</v>
       </c>
       <c r="EH2" t="n">
         <v>0</v>
       </c>
       <c r="EI2" t="n">
-        <v>0.002962970645290663</v>
+        <v>0.00296410775031038</v>
       </c>
     </row>
     <row r="3">
@@ -3905,406 +3905,406 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03399796747457478</v>
+        <v>0.03412930154663323</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0115964666997288</v>
+        <v>0.01159638030554655</v>
       </c>
       <c r="E3" t="n">
-        <v>0.009128034832231867</v>
+        <v>0.009111793222892966</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02692667968747732</v>
+        <v>0.0268839855469697</v>
       </c>
       <c r="G3" t="n">
-        <v>0.08164914869401277</v>
+        <v>0.08172146062204244</v>
       </c>
       <c r="H3" t="n">
-        <v>-2.98370024978678e-07</v>
+        <v>-1.000865281208796e-07</v>
       </c>
       <c r="I3" t="n">
-        <v>185.3145011275188</v>
+        <v>185.5038172636049</v>
       </c>
       <c r="J3" t="n">
-        <v>37.28058662248346</v>
+        <v>37.32616998900466</v>
       </c>
       <c r="K3" t="n">
-        <v>32.80935659201437</v>
+        <v>32.76350661959162</v>
       </c>
       <c r="L3" t="n">
-        <v>17.70277545851317</v>
+        <v>17.88282975471299</v>
       </c>
       <c r="M3" t="n">
-        <v>28.34973924324227</v>
+        <v>28.62639624978223</v>
       </c>
       <c r="N3" t="n">
-        <v>170.7926944038414</v>
+        <v>170.7929823484212</v>
       </c>
       <c r="O3" t="n">
-        <v>32.80935659201437</v>
+        <v>32.76350661959162</v>
       </c>
       <c r="P3" t="n">
-        <v>-167.6117256690056</v>
+        <v>-167.6209875088919</v>
       </c>
       <c r="Q3" t="n">
-        <v>-78.92460942446993</v>
+        <v>-78.94030107298144</v>
       </c>
       <c r="R3" t="n">
-        <v>437.5593110043699</v>
+        <v>437.5696701355757</v>
       </c>
       <c r="S3" t="n">
-        <v>1823783.855048422</v>
+        <v>1824302.817755626</v>
       </c>
       <c r="T3" t="n">
-        <v>64.643633228116</v>
+        <v>64.66139356458564</v>
       </c>
       <c r="U3" t="n">
-        <v>450407.640951275</v>
+        <v>450415.5537293874</v>
       </c>
       <c r="V3" t="n">
-        <v>478620.5331414867</v>
+        <v>478628.7226264273</v>
       </c>
       <c r="W3" t="n">
-        <v>1838.710694368907</v>
+        <v>1838.711065814882</v>
       </c>
       <c r="X3" t="n">
-        <v>-325924.4514229387</v>
+        <v>-325935.4719168234</v>
       </c>
       <c r="Y3" t="n">
-        <v>925.5550655299288</v>
+        <v>925.5698412401132</v>
       </c>
       <c r="Z3" t="n">
-        <v>1027.994473448428</v>
+        <v>1028.017721222832</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.110678890682585</v>
+        <v>1.110686277164622</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.9307535314919602</v>
+        <v>0.9307406250479749</v>
       </c>
       <c r="AC3" t="n">
-        <v>170.7926944154233</v>
+        <v>170.7929823175917</v>
       </c>
       <c r="AD3" t="n">
-        <v>1885664.120050585</v>
+        <v>1886188.550643211</v>
       </c>
       <c r="AE3" t="n">
-        <v>5.303171383317055e-07</v>
+        <v>5.301696904368278e-07</v>
       </c>
       <c r="AF3" t="n">
-        <v>1697758.133218614</v>
+        <v>1698219.010554721</v>
       </c>
       <c r="AG3" t="n">
-        <v>5.890120509122213e-07</v>
+        <v>5.888521997368004e-07</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.002985657828243262</v>
+        <v>0.002985750839304567</v>
       </c>
       <c r="AI3" t="n">
-        <v>1.922690650442412e-05</v>
+        <v>1.922757614672969e-05</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.02616713196378715</v>
+        <v>0.02616832879336677</v>
       </c>
       <c r="AK3" t="n">
-        <v>2.36076938236807</v>
+        <v>2.361041637648083</v>
       </c>
       <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="inlineStr"/>
       <c r="AN3" t="n">
-        <v>1823783.855048422</v>
+        <v>1824302.817755626</v>
       </c>
       <c r="AO3" t="n">
-        <v>64.643633228116</v>
+        <v>64.66139356458564</v>
       </c>
       <c r="AP3" t="n">
-        <v>64.643633228116</v>
+        <v>64.66139356458564</v>
       </c>
       <c r="AQ3" t="n">
-        <v>450407.640951275</v>
+        <v>450415.5537293874</v>
       </c>
       <c r="AR3" t="n">
-        <v>478620.5331414867</v>
+        <v>478628.7226264273</v>
       </c>
       <c r="AS3" t="n">
-        <v>1838.710694368907</v>
+        <v>1838.711065814882</v>
       </c>
       <c r="AT3" t="n">
-        <v>925.5550655299288</v>
+        <v>925.5698412401132</v>
       </c>
       <c r="AU3" t="n">
-        <v>1027.994473448428</v>
+        <v>1028.017721222832</v>
       </c>
       <c r="AV3" t="n">
-        <v>170.7926944154233</v>
+        <v>170.7929823175917</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.9307535314919602</v>
+        <v>0.9307406250479749</v>
       </c>
       <c r="AX3" t="n">
-        <v>1.922690650442412e-05</v>
+        <v>1.922757614672969e-05</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.02616713196378715</v>
+        <v>0.02616832879336677</v>
       </c>
       <c r="AZ3" t="n">
-        <v>438.4436929934603</v>
+        <v>438.4562480774021</v>
       </c>
       <c r="BA3" t="n">
-        <v>1869245.3997312</v>
+        <v>1869889.455706534</v>
       </c>
       <c r="BB3" t="n">
-        <v>66.20193884262284</v>
+        <v>66.22398141145847</v>
       </c>
       <c r="BC3" t="n">
-        <v>451079.9458195002</v>
+        <v>451089.5084523014</v>
       </c>
       <c r="BD3" t="n">
-        <v>479315.4542111023</v>
+        <v>479325.344109609</v>
       </c>
       <c r="BE3" t="n">
-        <v>1838.710694369046</v>
+        <v>1838.711065815021</v>
       </c>
       <c r="BF3" t="n">
-        <v>-326855.6529746322</v>
+        <v>-326869.0111060464</v>
       </c>
       <c r="BG3" t="n">
-        <v>926.8220299693231</v>
+        <v>926.8399518668405</v>
       </c>
       <c r="BH3" t="n">
-        <v>1030.007595332159</v>
+        <v>1030.036036644316</v>
       </c>
       <c r="BI3" t="n">
-        <v>1.111332663689761</v>
+        <v>1.111341860662802</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0.9296207261415116</v>
+        <v>0.9296048812146117</v>
       </c>
       <c r="BK3" t="n">
-        <v>170.8133122598472</v>
+        <v>170.8136405703442</v>
       </c>
       <c r="BL3" t="n">
-        <v>1931586.392085941</v>
+        <v>1932236.959915899</v>
       </c>
       <c r="BM3" t="n">
-        <v>5.177091763004652e-07</v>
+        <v>5.175348680026931e-07</v>
       </c>
       <c r="BN3" t="n">
-        <v>1738081.184145922</v>
+        <v>1738652.190032253</v>
       </c>
       <c r="BO3" t="n">
-        <v>5.753471179146281e-07</v>
+        <v>5.751581631639905e-07</v>
       </c>
       <c r="BP3" t="n">
-        <v>0.00299400751282472</v>
+        <v>0.002994123888756507</v>
       </c>
       <c r="BQ3" t="n">
-        <v>1.928484755229509e-05</v>
+        <v>1.9285670781927e-05</v>
       </c>
       <c r="BR3" t="n">
-        <v>0.02627007462645792</v>
+        <v>0.02627153652002328</v>
       </c>
       <c r="BS3" t="n">
-        <v>2.384817603784184</v>
+        <v>2.385165116738592</v>
       </c>
       <c r="BT3" t="inlineStr"/>
       <c r="BU3" t="inlineStr"/>
       <c r="BV3" t="n">
-        <v>1869245.3997312</v>
+        <v>1869889.455706534</v>
       </c>
       <c r="BW3" t="n">
-        <v>66.20193884262284</v>
+        <v>66.22398141145847</v>
       </c>
       <c r="BX3" t="n">
-        <v>66.20193884262284</v>
+        <v>66.22398141145847</v>
       </c>
       <c r="BY3" t="n">
-        <v>451079.9458195002</v>
+        <v>451089.5084523014</v>
       </c>
       <c r="BZ3" t="n">
-        <v>479315.4542111023</v>
+        <v>479325.344109609</v>
       </c>
       <c r="CA3" t="n">
-        <v>1838.710694369046</v>
+        <v>1838.711065815021</v>
       </c>
       <c r="CB3" t="n">
-        <v>926.8220299693231</v>
+        <v>926.8399518668405</v>
       </c>
       <c r="CC3" t="n">
-        <v>1030.007595332159</v>
+        <v>1030.036036644316</v>
       </c>
       <c r="CD3" t="n">
-        <v>170.8133122598472</v>
+        <v>170.8136405703442</v>
       </c>
       <c r="CE3" t="n">
-        <v>0.9296207261415116</v>
+        <v>0.9296048812146117</v>
       </c>
       <c r="CF3" t="n">
-        <v>1.928484755229509e-05</v>
+        <v>1.9285670781927e-05</v>
       </c>
       <c r="CG3" t="n">
-        <v>0.02627007462645792</v>
+        <v>0.02627153652002328</v>
       </c>
       <c r="CH3" t="n">
-        <v>456.7317968979807</v>
+        <v>456.7429629219752</v>
       </c>
       <c r="CI3" t="n">
-        <v>3046531.641639401</v>
+        <v>3047390.770144956</v>
       </c>
       <c r="CJ3" t="n">
-        <v>106.4579699229271</v>
+        <v>106.4872265825234</v>
       </c>
       <c r="CK3" t="n">
-        <v>464588.3807171274</v>
+        <v>464596.4138716624</v>
       </c>
       <c r="CL3" t="n">
-        <v>493205.605372501</v>
+        <v>493213.8440362404</v>
       </c>
       <c r="CM3" t="n">
-        <v>1838.710694368907</v>
+        <v>1838.711065814882</v>
       </c>
       <c r="CN3" t="n">
-        <v>-346592.0340421437</v>
+        <v>-346604.4961214722</v>
       </c>
       <c r="CO3" t="n">
-        <v>952.9989785151848</v>
+        <v>953.0148291227774</v>
       </c>
       <c r="CP3" t="n">
-        <v>1075.408459857337</v>
+        <v>1075.438181128929</v>
       </c>
       <c r="CQ3" t="n">
-        <v>1.128446602883953</v>
+        <v>1.128459021061444</v>
       </c>
       <c r="CR3" t="n">
-        <v>0.9044619030101475</v>
+        <v>0.9044462866368876</v>
       </c>
       <c r="CS3" t="n">
-        <v>171.2048701559773</v>
+        <v>171.2052540470023</v>
       </c>
       <c r="CT3" t="n">
-        <v>3120401.007575761</v>
+        <v>3121272.55022363</v>
       </c>
       <c r="CU3" t="n">
-        <v>3.204716309128806e-07</v>
+        <v>3.203821466755131e-07</v>
       </c>
       <c r="CV3" t="n">
-        <v>2765218.132254555</v>
+        <v>2765960.032193033</v>
       </c>
       <c r="CW3" t="n">
-        <v>3.616351232243199e-07</v>
+        <v>3.615381236030136e-07</v>
       </c>
       <c r="CX3" t="n">
-        <v>0.003212190528962811</v>
+        <v>0.003212343721803458</v>
       </c>
       <c r="CY3" t="n">
-        <v>2.069539505688694e-05</v>
+        <v>2.069639940914196e-05</v>
       </c>
       <c r="CZ3" t="n">
-        <v>0.02858710372735379</v>
+        <v>0.02858863389509057</v>
       </c>
       <c r="DA3" t="n">
-        <v>3.596962471367962</v>
+        <v>3.598878927944934</v>
       </c>
       <c r="DB3" t="inlineStr"/>
       <c r="DC3" t="inlineStr"/>
       <c r="DD3" t="n">
-        <v>3046531.641639401</v>
+        <v>3047390.770144956</v>
       </c>
       <c r="DE3" t="n">
-        <v>106.4579699229271</v>
+        <v>106.4872265825234</v>
       </c>
       <c r="DF3" t="n">
-        <v>106.4579699229271</v>
+        <v>106.4872265825234</v>
       </c>
       <c r="DG3" t="n">
-        <v>464588.3807171274</v>
+        <v>464596.4138716624</v>
       </c>
       <c r="DH3" t="n">
-        <v>493205.605372501</v>
+        <v>493213.8440362404</v>
       </c>
       <c r="DI3" t="n">
-        <v>1838.710694368907</v>
+        <v>1838.711065814882</v>
       </c>
       <c r="DJ3" t="n">
-        <v>952.9989785151848</v>
+        <v>953.0148291227774</v>
       </c>
       <c r="DK3" t="n">
-        <v>1075.408459857337</v>
+        <v>1075.438181128929</v>
       </c>
       <c r="DL3" t="n">
-        <v>171.2048701559773</v>
+        <v>171.2052540470023</v>
       </c>
       <c r="DM3" t="n">
-        <v>0.9044619030101475</v>
+        <v>0.9044462866368876</v>
       </c>
       <c r="DN3" t="n">
-        <v>2.069539505688694e-05</v>
+        <v>2.069639940914196e-05</v>
       </c>
       <c r="DO3" t="n">
-        <v>0.02858710372735379</v>
+        <v>0.02858863389509057</v>
       </c>
       <c r="DP3" t="n">
-        <v>0.02194057031036497</v>
+        <v>0.02199139760120455</v>
       </c>
       <c r="DQ3" t="n">
         <v>0</v>
       </c>
       <c r="DR3" t="n">
-        <v>0.01159352606036013</v>
+        <v>0.01159344036766186</v>
       </c>
       <c r="DS3" t="n">
-        <v>0.01040039022630374</v>
+        <v>0.01038675746226658</v>
       </c>
       <c r="DT3" t="n">
-        <v>0.03224772596587085</v>
+        <v>0.03221498031639532</v>
       </c>
       <c r="DU3" t="n">
-        <v>0.07618221256289968</v>
+        <v>0.07618657574752831</v>
       </c>
       <c r="DV3" t="n">
-        <v>-0.07618221256930489</v>
+        <v>-0.07618657574111612</v>
       </c>
       <c r="DW3" t="n">
-        <v>0.2182797499043195</v>
+        <v>0.2185462744575546</v>
       </c>
       <c r="DX3" t="n">
-        <v>0.9999999999321874</v>
+        <v>1.000000000180508</v>
       </c>
       <c r="DY3" t="n">
-        <v>4841533.722939144</v>
+        <v>4844453.94628886</v>
       </c>
       <c r="DZ3" t="n">
-        <v>10.65999724673028</v>
+        <v>10.65999997631805</v>
       </c>
       <c r="EA3" t="n">
-        <v>476034.8732083568</v>
+        <v>476008.0109265559</v>
       </c>
       <c r="EB3" t="n">
         <v>0</v>
       </c>
       <c r="EC3" t="n">
-        <v>1002.498749407823</v>
+        <v>1003.636092913803</v>
       </c>
       <c r="ED3" t="n">
-        <v>-55.48030696607228</v>
+        <v>-55.51725745657214</v>
       </c>
       <c r="EE3" t="n">
-        <v>0.01754868052616728</v>
+        <v>0.01762101826518644</v>
       </c>
       <c r="EF3" t="n">
         <v>0</v>
       </c>
       <c r="EG3" t="n">
-        <v>0.004711604222292333</v>
+        <v>0.004704434826766555</v>
       </c>
       <c r="EH3" t="n">
-        <v>0.01389870438047083</v>
+        <v>0.01388024890333254</v>
       </c>
       <c r="EI3" t="n">
-        <v>0.005985731044012167</v>
+        <v>0.005987231496515689</v>
       </c>
     </row>
   </sheetData>
@@ -4563,28 +4563,28 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.03499047623207872</v>
+        <v>0.03498796705530414</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05831746038679786</v>
+        <v>0.05831327842550691</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03842132997263242</v>
+        <v>0.03841832361712644</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05488660664624415</v>
+        <v>0.05488292186368462</v>
       </c>
       <c r="F2" t="n">
-        <v>0.007775897966184713</v>
+        <v>0.007793731569723754</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01036786395491293</v>
+        <v>0.01039164209296501</v>
       </c>
       <c r="H2" t="n">
-        <v>0.00145705798298816</v>
+        <v>0.001460399667063102</v>
       </c>
       <c r="I2" t="n">
-        <v>0.001876583375839241</v>
+        <v>0.001880887218826678</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -4592,13 +4592,13 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>14.39999999999999</v>
+        <v>14.39999999999901</v>
       </c>
       <c r="L2" t="n">
-        <v>79.19999999999996</v>
+        <v>79.19999999999999</v>
       </c>
       <c r="M2" t="n">
-        <v>46.79999999999998</v>
+        <v>46.7999999999995</v>
       </c>
       <c r="N2" t="n">
         <v>0.01200896</v>
@@ -4607,7 +4607,7 @@
         <v>45</v>
       </c>
       <c r="P2" t="n">
-        <v>7.285289914940803e-05</v>
+        <v>7.301998335315558e-05</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -4622,85 +4622,85 @@
         <v>2</v>
       </c>
       <c r="U2" t="n">
-        <v>0.00709729126499802</v>
+        <v>0.007113568520586003</v>
       </c>
       <c r="V2" t="n">
-        <v>0.04665396830943829</v>
+        <v>0.04665062274040553</v>
       </c>
       <c r="W2" t="n">
-        <v>0.04665396830943828</v>
+        <v>0.04665062274040553</v>
       </c>
       <c r="X2" t="n">
-        <v>0.04665396830943828</v>
+        <v>0.04665062274040553</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.03842132997263242</v>
+        <v>0.03841832361712644</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.05488660664624415</v>
+        <v>0.05488292186368462</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.05831746038679786</v>
+        <v>0.05831327842550691</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.05488660664624415</v>
+        <v>0.05488292186368462</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.05488660664624415</v>
+        <v>0.05488292186368462</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.6000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.7000128504985937</v>
+        <v>0.7000050710227835</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.7000128504985937</v>
+        <v>0.7000050710227835</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.006837967821587912</v>
+        <v>0.006836987151605674</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.004826557574735687</v>
+        <v>0.004826012604139102</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.0009044067032776634</v>
+        <v>0.0009043045859708626</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.01989613041416543</v>
+        <v>0.01989495480838048</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.02332698415471914</v>
+        <v>0.02332531137020277</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.01646527667361172</v>
+        <v>0.01646459824655819</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.01646527667361172</v>
+        <v>0.01646459824655819</v>
       </c>
       <c r="AN2" t="n">
-        <v>-0.4502822799102217</v>
+        <v>-0.4493285826979359</v>
       </c>
       <c r="AO2" t="n">
-        <v>1.919019240673718</v>
+        <v>1.914515014123618</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.7500000000000013</v>
+        <v>0.75</v>
       </c>
       <c r="AQ2" t="n">
-        <v>1.333333333333331</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.181</v>
+        <v>0.1810000000000012</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.05000000000000003</v>
+        <v>0.05000000000000031</v>
       </c>
       <c r="AT2" t="n">
         <v>0</v>
       </c>
       <c r="AU2" t="n">
-        <v>1.158286803552183</v>
+        <v>1.155636413626091</v>
       </c>
     </row>
     <row r="3">
@@ -4708,28 +4708,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0384213299727189</v>
+        <v>0.03841832361707791</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05488660664615769</v>
+        <v>0.05488292186373316</v>
       </c>
       <c r="D3" t="n">
-        <v>0.03808092204868911</v>
+        <v>0.03806731948749102</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05522701457018747</v>
+        <v>0.05523392599332005</v>
       </c>
       <c r="F3" t="n">
-        <v>0.006323515560279881</v>
+        <v>0.006325801395096079</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00843135408037317</v>
+        <v>0.008434401860128105</v>
       </c>
       <c r="H3" t="n">
-        <v>0.001214750300980719</v>
+        <v>0.001213489178727771</v>
       </c>
       <c r="I3" t="n">
-        <v>0.00150420214755084</v>
+        <v>0.001504911326106501</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -4737,13 +4737,13 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>-16.19999999999999</v>
+        <v>-16.2</v>
       </c>
       <c r="L3" t="n">
-        <v>-78.92460942446993</v>
+        <v>-78.94030107298144</v>
       </c>
       <c r="M3" t="n">
-        <v>-47.56230471223496</v>
+        <v>-47.57015053649072</v>
       </c>
       <c r="N3" t="n">
         <v>0.01200896</v>
@@ -4752,7 +4752,7 @@
         <v>45</v>
       </c>
       <c r="P3" t="n">
-        <v>6.073751504903593e-05</v>
+        <v>6.067445893638997e-05</v>
       </c>
       <c r="Q3" t="n">
         <v>0.0005</v>
@@ -4763,85 +4763,85 @@
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
-        <v>0.005689377201913756</v>
+        <v>0.005690581373715239</v>
       </c>
       <c r="V3" t="n">
-        <v>0.0466539683094383</v>
+        <v>0.04665062274040553</v>
       </c>
       <c r="W3" t="n">
-        <v>0.04665396830943829</v>
+        <v>0.04665062274040553</v>
       </c>
       <c r="X3" t="n">
-        <v>0.04665396830943829</v>
+        <v>0.04665062274040553</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.03808092204868911</v>
+        <v>0.03806731948749102</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.05522701457018747</v>
+        <v>0.05523392599332005</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.05538660664615769</v>
+        <v>0.05538292186373316</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.05572701457018747</v>
+        <v>0.05573392599332005</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.05572701457018747</v>
+        <v>0.05573392599332005</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.7000128505012718</v>
+        <v>0.7000050710212805</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.6895343220172157</v>
+        <v>0.689201768711767</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.6895343220172157</v>
+        <v>0.689201768711767</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.004826557574684998</v>
+        <v>0.00482601260416755</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.005026128887915242</v>
+        <v>0.00503178140922726</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.0009655217135407338</v>
+        <v>0.0009652551366146885</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.01680568459746858</v>
+        <v>0.01681560237624214</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.0164652766734388</v>
+        <v>0.01646459824665524</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.01714609252149836</v>
+        <v>0.01716660650582903</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.01714609252149836</v>
+        <v>0.01716660650582903</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.05976095000094357</v>
+        <v>0.06160354703910173</v>
       </c>
       <c r="AO3" t="n">
-        <v>1.993236725354649</v>
+        <v>1.993692339433627</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.7500000000000003</v>
+        <v>0.75</v>
       </c>
       <c r="AQ3" t="n">
         <v>1.333333333333333</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.1784057617805874</v>
+        <v>0.1784253763412268</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.05</v>
+        <v>0.05000000000000118</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.029751837665412</v>
+        <v>0.02973429014392153</v>
       </c>
       <c r="AU3" t="n">
-        <v>1.424321631557963</v>
+        <v>1.423806951476889</v>
       </c>
     </row>
   </sheetData>
@@ -4855,7 +4855,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4935,7 +4935,7 @@
         <v>26</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.6258330249200093</v>
+        <v>-6.258330249200093</v>
       </c>
       <c r="I2" t="n">
         <v>0.4546790801976228</v>
@@ -4955,19 +4955,19 @@
         <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.8606242378415749</v>
+        <v>-8.256412534726815</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8388433955625365</v>
+        <v>0.9364972605158474</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5355157924032202</v>
+        <v>0.7927659177547192</v>
       </c>
     </row>
     <row r="4">
@@ -4981,19 +4981,19 @@
         <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.836757919731961</v>
+        <v>-9.089999410175356</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2683473465429107</v>
+        <v>0.2630573109350501</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2544874384588238</v>
+        <v>0.5083279564860762</v>
       </c>
     </row>
     <row r="5">
@@ -5013,13 +5013,13 @@
         <v>105</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.8656493080763369</v>
+        <v>-9.217264126678476</v>
       </c>
       <c r="I5" t="n">
-        <v>0.01563444826037557</v>
+        <v>0.1836350977086266</v>
       </c>
       <c r="J5" t="n">
-        <v>0.10279529694778</v>
+        <v>0.1714943290008779</v>
       </c>
     </row>
     <row r="6">
@@ -5033,19 +5033,19 @@
         <v>5</v>
       </c>
       <c r="F6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G6" t="n">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.8713510110125913</v>
+        <v>-9.843958487607058</v>
       </c>
       <c r="I6" t="n">
-        <v>0.02658903491729347</v>
+        <v>0.2277899682862147</v>
       </c>
       <c r="J6" t="n">
-        <v>0.08650024459444909</v>
+        <v>0.3040637149052056</v>
       </c>
     </row>
     <row r="7">
@@ -5059,19 +5059,19 @@
         <v>6</v>
       </c>
       <c r="F7" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G7" t="n">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.8757193530859184</v>
+        <v>-9.160667685102833</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0209456262432397</v>
+        <v>0.05091719415218562</v>
       </c>
       <c r="J7" t="n">
-        <v>0.05382306531281141</v>
+        <v>0.26025666668855</v>
       </c>
     </row>
     <row r="8">
@@ -5085,19 +5085,19 @@
         <v>7</v>
       </c>
       <c r="F8" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G8" t="n">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.8810766500233271</v>
+        <v>-9.120404803262669</v>
       </c>
       <c r="I8" t="n">
-        <v>0.02763384543885584</v>
+        <v>0.02781704588931895</v>
       </c>
       <c r="J8" t="n">
-        <v>0.06143367864870554</v>
+        <v>0.04253520404710044</v>
       </c>
     </row>
     <row r="9">
@@ -5111,19 +5111,19 @@
         <v>8</v>
       </c>
       <c r="F9" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G9" t="n">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.8894916613256395</v>
+        <v>-9.079952656632887</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0398971385187273</v>
+        <v>0.00170973687966177</v>
       </c>
       <c r="J9" t="n">
-        <v>0.08510170561737131</v>
+        <v>0.05745285774544549</v>
       </c>
     </row>
     <row r="10">
@@ -5137,19 +5137,19 @@
         <v>9</v>
       </c>
       <c r="F10" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G10" t="n">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.9015607349631903</v>
+        <v>-9.07666302833068</v>
       </c>
       <c r="I10" t="n">
-        <v>0.02936352372231872</v>
+        <v>0.001678276230825639</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0887291815673564</v>
+        <v>0.03754798166184733</v>
       </c>
     </row>
     <row r="11">
@@ -5163,19 +5163,19 @@
         <v>10</v>
       </c>
       <c r="F11" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G11" t="n">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.9054381047875829</v>
+        <v>-9.078812463347054</v>
       </c>
       <c r="I11" t="n">
-        <v>0.002308109611607809</v>
+        <v>0.0001436823098264067</v>
       </c>
       <c r="J11" t="n">
-        <v>0.04667029250635509</v>
+        <v>0.1014157260613982</v>
       </c>
     </row>
     <row r="12">
@@ -5189,19 +5189,19 @@
         <v>11</v>
       </c>
       <c r="F12" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G12" t="n">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.9047950201626921</v>
+        <v>-9.079966446301285</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0001730756865757034</v>
+        <v>0.0001548143536957425</v>
       </c>
       <c r="J12" t="n">
-        <v>0.02116795602240608</v>
+        <v>0.07256156811878461</v>
       </c>
     </row>
     <row r="13">
@@ -5215,19 +5215,19 @@
         <v>12</v>
       </c>
       <c r="F13" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G13" t="n">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.9055288820343665</v>
+        <v>-9.08072294854491</v>
       </c>
       <c r="I13" t="n">
-        <v>0.000869199137731702</v>
+        <v>0.000144402403583696</v>
       </c>
       <c r="J13" t="n">
-        <v>0.04638894214426629</v>
+        <v>0.0543663971902397</v>
       </c>
     </row>
     <row r="14">
@@ -5241,19 +5241,19 @@
         <v>13</v>
       </c>
       <c r="F14" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G14" t="n">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.9060449610288466</v>
+        <v>-9.081341394961781</v>
       </c>
       <c r="I14" t="n">
-        <v>0.001408231732708081</v>
+        <v>8.205237989726974e-05</v>
       </c>
       <c r="J14" t="n">
-        <v>0.05414331910836844</v>
+        <v>0.03582227549941989</v>
       </c>
     </row>
     <row r="15">
@@ -5267,19 +5267,19 @@
         <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G15" t="n">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.9062177584866956</v>
+        <v>-9.081584540108077</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0001640024231051563</v>
+        <v>7.240306721313949e-05</v>
       </c>
       <c r="J15" t="n">
-        <v>0.02201898573428753</v>
+        <v>0.01299018682397973</v>
       </c>
     </row>
     <row r="16">
@@ -5293,19 +5293,19 @@
         <v>15</v>
       </c>
       <c r="F16" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G16" t="n">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.9069852160720315</v>
+        <v>-9.081657277117952</v>
       </c>
       <c r="I16" t="n">
-        <v>0.002220144623424175</v>
+        <v>4.912159532383057e-05</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1046562815090653</v>
+        <v>0.01134746486340791</v>
       </c>
     </row>
     <row r="17">
@@ -5325,13 +5325,13 @@
         <v>422</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.906960492197756</v>
+        <v>-9.08180690643341</v>
       </c>
       <c r="I17" t="n">
-        <v>4.193157796819613e-05</v>
+        <v>0.0001029334331751468</v>
       </c>
       <c r="J17" t="n">
-        <v>0.01023444554361871</v>
+        <v>0.0144843600145345</v>
       </c>
     </row>
     <row r="18">
@@ -5345,19 +5345,19 @@
         <v>17</v>
       </c>
       <c r="F18" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G18" t="n">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.907136136581531</v>
+        <v>-9.081942941550185</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0003106463222229137</v>
+        <v>0.000166006446628394</v>
       </c>
       <c r="J18" t="n">
-        <v>0.0353072064404836</v>
+        <v>0.01341719670262314</v>
       </c>
     </row>
     <row r="19">
@@ -5371,19 +5371,19 @@
         <v>18</v>
       </c>
       <c r="F19" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G19" t="n">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.9071786512892958</v>
+        <v>-9.082115202188264</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0001231191194618523</v>
+        <v>0.0002110268388439394</v>
       </c>
       <c r="J19" t="n">
-        <v>0.02474299358969597</v>
+        <v>0.01835201160963716</v>
       </c>
     </row>
     <row r="20">
@@ -5397,19 +5397,19 @@
         <v>19</v>
       </c>
       <c r="F20" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G20" t="n">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.9072611582911615</v>
+        <v>-9.082246599412928</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0003968566503906338</v>
+        <v>0.0002634822194884516</v>
       </c>
       <c r="J20" t="n">
-        <v>0.03611592175736992</v>
+        <v>0.01282192719564129</v>
       </c>
     </row>
     <row r="21">
@@ -5423,19 +5423,19 @@
         <v>20</v>
       </c>
       <c r="F21" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G21" t="n">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.9073254445944304</v>
+        <v>-9.082408159524388</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0005125943027001524</v>
+        <v>0.0002871026196866519</v>
       </c>
       <c r="J21" t="n">
-        <v>0.02663666171143221</v>
+        <v>0.01578214532393193</v>
       </c>
     </row>
     <row r="22">
@@ -5449,19 +5449,19 @@
         <v>21</v>
       </c>
       <c r="F22" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G22" t="n">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.907379473429063</v>
+        <v>-9.082569949639479</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0005365174029782386</v>
+        <v>0.0003465392486870578</v>
       </c>
       <c r="J22" t="n">
-        <v>0.02022819031352086</v>
+        <v>0.01313543255874142</v>
       </c>
     </row>
     <row r="23">
@@ -5475,19 +5475,19 @@
         <v>22</v>
       </c>
       <c r="F23" t="n">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G23" t="n">
-        <v>582</v>
+        <v>587</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.9074209176173667</v>
+        <v>-9.082769402139686</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0005140728329228173</v>
+        <v>0.0004168500989024224</v>
       </c>
       <c r="J23" t="n">
-        <v>0.01329277099021195</v>
+        <v>0.01422813365634195</v>
       </c>
     </row>
     <row r="24">
@@ -5501,19 +5501,19 @@
         <v>23</v>
       </c>
       <c r="F24" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G24" t="n">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.9074499058110174</v>
+        <v>-9.083014622853554</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0004926973089961486</v>
+        <v>0.0004768834418942844</v>
       </c>
       <c r="J24" t="n">
-        <v>0.009054515995986495</v>
+        <v>0.01274373436523665</v>
       </c>
     </row>
     <row r="25">
@@ -5527,19 +5527,19 @@
         <v>24</v>
       </c>
       <c r="F25" t="n">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G25" t="n">
-        <v>636</v>
+        <v>642</v>
       </c>
       <c r="H25" t="n">
-        <v>-0.9074714838815384</v>
+        <v>-9.083238511961669</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0004995854672758903</v>
+        <v>0.0004066109234916906</v>
       </c>
       <c r="J25" t="n">
-        <v>0.007803750336328675</v>
+        <v>0.01658070655874211</v>
       </c>
     </row>
     <row r="26">
@@ -5553,19 +5553,19 @@
         <v>25</v>
       </c>
       <c r="F26" t="n">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G26" t="n">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.9074951559485309</v>
+        <v>-9.08334541165566</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0005137210171628863</v>
+        <v>0.0004172497670762339</v>
       </c>
       <c r="J26" t="n">
-        <v>0.009821760994066496</v>
+        <v>0.00614461473853484</v>
       </c>
     </row>
     <row r="27">
@@ -5579,19 +5579,19 @@
         <v>26</v>
       </c>
       <c r="F27" t="n">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="G27" t="n">
-        <v>690</v>
+        <v>699</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.9075078054165977</v>
+        <v>-9.08336925076874</v>
       </c>
       <c r="I27" t="n">
-        <v>0.000529579673357427</v>
+        <v>0.0004070688553406457</v>
       </c>
       <c r="J27" t="n">
-        <v>0.006249703059017525</v>
+        <v>0.001282374122382684</v>
       </c>
     </row>
     <row r="28">
@@ -5605,19 +5605,19 @@
         <v>27</v>
       </c>
       <c r="F28" t="n">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G28" t="n">
-        <v>717</v>
+        <v>725</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.9075264582692979</v>
+        <v>-9.083439105361558</v>
       </c>
       <c r="I28" t="n">
-        <v>0.0006455125822065045</v>
+        <v>1.070180232903839e-06</v>
       </c>
       <c r="J28" t="n">
-        <v>0.008349911523472597</v>
+        <v>0.00574989523083606</v>
       </c>
     </row>
     <row r="29">
@@ -5631,19 +5631,19 @@
         <v>28</v>
       </c>
       <c r="F29" t="n">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G29" t="n">
-        <v>744</v>
+        <v>752</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.9075450676158506</v>
+        <v>-9.083665407261968</v>
       </c>
       <c r="I29" t="n">
-        <v>0.00074794003126734</v>
+        <v>3.184987008920948e-05</v>
       </c>
       <c r="J29" t="n">
-        <v>0.008218824261957133</v>
+        <v>0.01543794457007689</v>
       </c>
     </row>
     <row r="30">
@@ -5657,19 +5657,19 @@
         <v>29</v>
       </c>
       <c r="F30" t="n">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="G30" t="n">
-        <v>772</v>
+        <v>778</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.9075571652217479</v>
+        <v>-9.083535232719674</v>
       </c>
       <c r="I30" t="n">
-        <v>0.0007946875943754963</v>
+        <v>2.19970531423197e-06</v>
       </c>
       <c r="J30" t="n">
-        <v>0.005390224122110888</v>
+        <v>0.007324279260261699</v>
       </c>
     </row>
     <row r="31">
@@ -5683,19 +5683,19 @@
         <v>30</v>
       </c>
       <c r="F31" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G31" t="n">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.9075695118121635</v>
+        <v>-9.083672363841837</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0008490262374252344</v>
+        <v>2.770028558428395e-05</v>
       </c>
       <c r="J31" t="n">
-        <v>0.005335864143034753</v>
+        <v>0.02394207299141612</v>
       </c>
     </row>
     <row r="32">
@@ -5709,19 +5709,19 @@
         <v>31</v>
       </c>
       <c r="F32" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G32" t="n">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.907583931013333</v>
+        <v>-9.083616478679565</v>
       </c>
       <c r="I32" t="n">
-        <v>0.0009075580284853145</v>
+        <v>5.43856616505578e-07</v>
       </c>
       <c r="J32" t="n">
-        <v>0.006016902089750241</v>
+        <v>0.003100851469937611</v>
       </c>
     </row>
     <row r="33">
@@ -5735,19 +5735,19 @@
         <v>32</v>
       </c>
       <c r="F33" t="n">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="G33" t="n">
-        <v>856</v>
+        <v>862</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.9075994770995056</v>
+        <v>-9.083616479147675</v>
       </c>
       <c r="I33" t="n">
-        <v>0.0009755325485349505</v>
+        <v>5.438444161121048e-07</v>
       </c>
       <c r="J33" t="n">
-        <v>0.006111010390485761</v>
+        <v>1.551025206175806e-07</v>
       </c>
     </row>
     <row r="34">
@@ -5761,19 +5761,19 @@
         <v>33</v>
       </c>
       <c r="F34" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G34" t="n">
-        <v>884</v>
+        <v>888</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.9076163911071141</v>
+        <v>-9.732843571512268</v>
       </c>
       <c r="I34" t="n">
-        <v>0.001045952981667831</v>
+        <v>0.144434172252016</v>
       </c>
       <c r="J34" t="n">
-        <v>0.006520656430918746</v>
+        <v>0.2375421917851947</v>
       </c>
     </row>
     <row r="35">
@@ -5787,19 +5787,19 @@
         <v>34</v>
       </c>
       <c r="F35" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G35" t="n">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="H35" t="n">
-        <v>-0.9076357072419647</v>
+        <v>-9.117530334469242</v>
       </c>
       <c r="I35" t="n">
-        <v>0.00112435420184982</v>
+        <v>0.02255177478702066</v>
       </c>
       <c r="J35" t="n">
-        <v>0.007286720484505645</v>
+        <v>0.2788665945867921</v>
       </c>
     </row>
     <row r="36">
@@ -5813,19 +5813,19 @@
         <v>35</v>
       </c>
       <c r="F36" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G36" t="n">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.9076555544998308</v>
+        <v>-9.107688063423769</v>
       </c>
       <c r="I36" t="n">
-        <v>0.001203651271272753</v>
+        <v>0.01395344405971485</v>
       </c>
       <c r="J36" t="n">
-        <v>0.007393919387531206</v>
+        <v>0.1797553805133415</v>
       </c>
     </row>
     <row r="37">
@@ -5839,19 +5839,19 @@
         <v>36</v>
       </c>
       <c r="F37" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G37" t="n">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="H37" t="n">
-        <v>-0.907679430266693</v>
+        <v>-9.097459315225183</v>
       </c>
       <c r="I37" t="n">
-        <v>0.001303781382501257</v>
+        <v>0.01284823643320517</v>
       </c>
       <c r="J37" t="n">
-        <v>0.008799164908406609</v>
+        <v>0.06063376458664391</v>
       </c>
     </row>
     <row r="38">
@@ -5865,19 +5865,19 @@
         <v>37</v>
       </c>
       <c r="F38" t="n">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G38" t="n">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="H38" t="n">
-        <v>-0.907698054343935</v>
+        <v>-9.084479828153999</v>
       </c>
       <c r="I38" t="n">
-        <v>0.001376453208317262</v>
+        <v>0.000482898925693505</v>
       </c>
       <c r="J38" t="n">
-        <v>0.007403739177829111</v>
+        <v>0.01798458190849382</v>
       </c>
     </row>
     <row r="39">
@@ -5891,19 +5891,19 @@
         <v>38</v>
       </c>
       <c r="F39" t="n">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G39" t="n">
-        <v>1024</v>
+        <v>1019</v>
       </c>
       <c r="H39" t="n">
-        <v>-0.9077214913023924</v>
+        <v>-9.084193180411106</v>
       </c>
       <c r="I39" t="n">
-        <v>0.001467494877110526</v>
+        <v>0.0001181464120189046</v>
       </c>
       <c r="J39" t="n">
-        <v>0.00899460461463884</v>
+        <v>0.01675343240250649</v>
       </c>
     </row>
     <row r="40">
@@ -5917,19 +5917,19 @@
         <v>39</v>
       </c>
       <c r="F40" t="n">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G40" t="n">
-        <v>1052</v>
+        <v>1045</v>
       </c>
       <c r="H40" t="n">
-        <v>-0.9077465572172886</v>
+        <v>-9.083944531093127</v>
       </c>
       <c r="I40" t="n">
-        <v>0.001550243566079819</v>
+        <v>2.226940050099879e-05</v>
       </c>
       <c r="J40" t="n">
-        <v>0.009498819029326923</v>
+        <v>0.02458814978882919</v>
       </c>
     </row>
     <row r="41">
@@ -5943,19 +5943,19 @@
         <v>40</v>
       </c>
       <c r="F41" t="n">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G41" t="n">
-        <v>1080</v>
+        <v>1072</v>
       </c>
       <c r="H41" t="n">
-        <v>-0.9077722877027463</v>
+        <v>-9.08401171099854</v>
       </c>
       <c r="I41" t="n">
-        <v>0.001635543022979196</v>
+        <v>1.852559133454224e-05</v>
       </c>
       <c r="J41" t="n">
-        <v>0.01010355605821438</v>
+        <v>0.0119387803431142</v>
       </c>
     </row>
     <row r="42">
@@ -5969,19 +5969,19 @@
         <v>41</v>
       </c>
       <c r="F42" t="n">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G42" t="n">
-        <v>1108</v>
+        <v>1100</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.9078005954563898</v>
+        <v>-9.084018733975931</v>
       </c>
       <c r="I42" t="n">
-        <v>0.001729073286329987</v>
+        <v>1.682621054362177e-05</v>
       </c>
       <c r="J42" t="n">
-        <v>0.01129304958777255</v>
+        <v>0.001848148665591283</v>
       </c>
     </row>
     <row r="43">
@@ -5995,19 +5995,19 @@
         <v>42</v>
       </c>
       <c r="F43" t="n">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G43" t="n">
-        <v>1135</v>
+        <v>1129</v>
       </c>
       <c r="H43" t="n">
-        <v>-0.9078522151968822</v>
+        <v>-9.084019894523855</v>
       </c>
       <c r="I43" t="n">
-        <v>0.002054395901175705</v>
+        <v>1.657391141361708e-05</v>
       </c>
       <c r="J43" t="n">
-        <v>0.02008993407398506</v>
+        <v>0.0001891616384545366</v>
       </c>
     </row>
     <row r="44">
@@ -6021,19 +6021,19 @@
         <v>43</v>
       </c>
       <c r="F44" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G44" t="n">
-        <v>1162</v>
+        <v>1155</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.9078928090744349</v>
+        <v>-9.083993497256534</v>
       </c>
       <c r="I44" t="n">
-        <v>0.002241312290522992</v>
+        <v>1.191697099903188e-06</v>
       </c>
       <c r="J44" t="n">
-        <v>0.01748005330374545</v>
+        <v>0.002133605762493981</v>
       </c>
     </row>
     <row r="45">
@@ -6047,19 +6047,19 @@
         <v>44</v>
       </c>
       <c r="F45" t="n">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G45" t="n">
-        <v>1189</v>
+        <v>1181</v>
       </c>
       <c r="H45" t="n">
-        <v>-0.9079257579328071</v>
+        <v>-9.084013294140009</v>
       </c>
       <c r="I45" t="n">
-        <v>0.002322365897205202</v>
+        <v>2.849347304692504e-06</v>
       </c>
       <c r="J45" t="n">
-        <v>0.01542805094113075</v>
+        <v>0.002147951568342412</v>
       </c>
     </row>
     <row r="46">
@@ -6073,19 +6073,19 @@
         <v>45</v>
       </c>
       <c r="F46" t="n">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="G46" t="n">
-        <v>1216</v>
+        <v>1207</v>
       </c>
       <c r="H46" t="n">
-        <v>-0.9079588288976033</v>
+        <v>-9.084017210274235</v>
       </c>
       <c r="I46" t="n">
-        <v>0.002331617477070128</v>
+        <v>7.551696224877835e-07</v>
       </c>
       <c r="J46" t="n">
-        <v>0.01585272798414813</v>
+        <v>0.001119833865891155</v>
       </c>
     </row>
     <row r="47">
@@ -6099,19 +6099,19 @@
         <v>46</v>
       </c>
       <c r="F47" t="n">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="G47" t="n">
-        <v>1243</v>
+        <v>1233</v>
       </c>
       <c r="H47" t="n">
-        <v>-0.907987164681083</v>
+        <v>-9.084023801589989</v>
       </c>
       <c r="I47" t="n">
-        <v>0.002306808000683654</v>
+        <v>5.044237878504276e-07</v>
       </c>
       <c r="J47" t="n">
-        <v>0.0151835352769963</v>
+        <v>0.002163701717047986</v>
       </c>
     </row>
     <row r="48">
@@ -6125,19 +6125,19 @@
         <v>47</v>
       </c>
       <c r="F48" t="n">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="G48" t="n">
-        <v>1270</v>
+        <v>1260</v>
       </c>
       <c r="H48" t="n">
-        <v>-0.9080116482673481</v>
+        <v>-9.084042119394896</v>
       </c>
       <c r="I48" t="n">
-        <v>0.002245399976540558</v>
+        <v>2.443342505598078e-06</v>
       </c>
       <c r="J48" t="n">
-        <v>0.01446341623065327</v>
+        <v>0.003881622795160715</v>
       </c>
     </row>
     <row r="49">
@@ -6151,19 +6151,19 @@
         <v>48</v>
       </c>
       <c r="F49" t="n">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G49" t="n">
-        <v>1297</v>
+        <v>1286</v>
       </c>
       <c r="H49" t="n">
-        <v>-0.9080387056610546</v>
+        <v>-9.084033201173645</v>
       </c>
       <c r="I49" t="n">
-        <v>0.002133715804780129</v>
+        <v>6.732448429164206e-07</v>
       </c>
       <c r="J49" t="n">
-        <v>0.01688287165102741</v>
+        <v>0.002768131726134983</v>
       </c>
     </row>
     <row r="50">
@@ -6177,19 +6177,19 @@
         <v>49</v>
       </c>
       <c r="F50" t="n">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="G50" t="n">
-        <v>1324</v>
+        <v>1312</v>
       </c>
       <c r="H50" t="n">
-        <v>-0.9080642471119511</v>
+        <v>-9.084031265372248</v>
       </c>
       <c r="I50" t="n">
-        <v>0.001940106334653553</v>
+        <v>1.000865281208796e-07</v>
       </c>
       <c r="J50" t="n">
-        <v>0.01815433401465724</v>
+        <v>0.0008758053270857481</v>
       </c>
     </row>
     <row r="51">
@@ -6200,360 +6200,22 @@
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F51" t="n">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G51" t="n">
-        <v>1351</v>
+        <v>1316</v>
       </c>
       <c r="H51" t="n">
-        <v>-0.9080826732575424</v>
+        <v>-9.084031265372248</v>
       </c>
       <c r="I51" t="n">
-        <v>0.001626003972098506</v>
+        <v>1.000865281208796e-07</v>
       </c>
       <c r="J51" t="n">
-        <v>0.01750873811872088</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="n">
-        <v>51</v>
-      </c>
-      <c r="F52" t="n">
-        <v>102</v>
-      </c>
-      <c r="G52" t="n">
-        <v>1377</v>
-      </c>
-      <c r="H52" t="n">
-        <v>-0.9081019454565965</v>
-      </c>
-      <c r="I52" t="n">
-        <v>0.001058290593243108</v>
-      </c>
-      <c r="J52" t="n">
-        <v>0.02367843621183904</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="inlineStr"/>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="n">
-        <v>52</v>
-      </c>
-      <c r="F53" t="n">
-        <v>103</v>
-      </c>
-      <c r="G53" t="n">
-        <v>1403</v>
-      </c>
-      <c r="H53" t="n">
-        <v>-0.9081122891836452</v>
-      </c>
-      <c r="I53" t="n">
-        <v>4.759447498517422e-06</v>
-      </c>
-      <c r="J53" t="n">
-        <v>0.005503615967341307</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="n">
-        <v>53</v>
-      </c>
-      <c r="F54" t="n">
-        <v>104</v>
-      </c>
-      <c r="G54" t="n">
-        <v>1429</v>
-      </c>
-      <c r="H54" t="n">
-        <v>-0.9081805698281455</v>
-      </c>
-      <c r="I54" t="n">
-        <v>6.991776063479969e-05</v>
-      </c>
-      <c r="J54" t="n">
-        <v>0.02490879058720893</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="n">
-        <v>54</v>
-      </c>
-      <c r="F55" t="n">
-        <v>105</v>
-      </c>
-      <c r="G55" t="n">
-        <v>1455</v>
-      </c>
-      <c r="H55" t="n">
-        <v>-0.9082710869646423</v>
-      </c>
-      <c r="I55" t="n">
-        <v>0.0001907875135563007</v>
-      </c>
-      <c r="J55" t="n">
-        <v>0.05097804902395375</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="n">
-        <v>55</v>
-      </c>
-      <c r="F56" t="n">
-        <v>106</v>
-      </c>
-      <c r="G56" t="n">
-        <v>1481</v>
-      </c>
-      <c r="H56" t="n">
-        <v>-0.9083387481589102</v>
-      </c>
-      <c r="I56" t="n">
-        <v>1.102156937567156e-05</v>
-      </c>
-      <c r="J56" t="n">
-        <v>0.02973430791308585</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="n">
-        <v>56</v>
-      </c>
-      <c r="F57" t="n">
-        <v>107</v>
-      </c>
-      <c r="G57" t="n">
-        <v>1507</v>
-      </c>
-      <c r="H57" t="n">
-        <v>-0.9083854933286061</v>
-      </c>
-      <c r="I57" t="n">
-        <v>8.653457927940108e-05</v>
-      </c>
-      <c r="J57" t="n">
-        <v>0.01078536770545768</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="inlineStr"/>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="n">
-        <v>57</v>
-      </c>
-      <c r="F58" t="n">
-        <v>108</v>
-      </c>
-      <c r="G58" t="n">
-        <v>1533</v>
-      </c>
-      <c r="H58" t="n">
-        <v>-0.9083701483344296</v>
-      </c>
-      <c r="I58" t="n">
-        <v>1.071538564934027e-06</v>
-      </c>
-      <c r="J58" t="n">
-        <v>0.005565576860952455</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="n">
-        <v>58</v>
-      </c>
-      <c r="F59" t="n">
-        <v>109</v>
-      </c>
-      <c r="G59" t="n">
-        <v>1559</v>
-      </c>
-      <c r="H59" t="n">
-        <v>-0.9084083159942263</v>
-      </c>
-      <c r="I59" t="n">
-        <v>3.241064778029823e-05</v>
-      </c>
-      <c r="J59" t="n">
-        <v>0.02870436309450362</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="inlineStr"/>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="n">
-        <v>59</v>
-      </c>
-      <c r="F60" t="n">
-        <v>110</v>
-      </c>
-      <c r="G60" t="n">
-        <v>1585</v>
-      </c>
-      <c r="H60" t="n">
-        <v>-0.9084050415181634</v>
-      </c>
-      <c r="I60" t="n">
-        <v>2.059530452372097e-05</v>
-      </c>
-      <c r="J60" t="n">
-        <v>0.00882282138633555</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="n">
-        <v>60</v>
-      </c>
-      <c r="F61" t="n">
-        <v>112</v>
-      </c>
-      <c r="G61" t="n">
-        <v>1612</v>
-      </c>
-      <c r="H61" t="n">
-        <v>-0.9084049761231163</v>
-      </c>
-      <c r="I61" t="n">
-        <v>1.222123902882236e-05</v>
-      </c>
-      <c r="J61" t="n">
-        <v>0.002190961735600912</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="inlineStr"/>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="n">
-        <v>61</v>
-      </c>
-      <c r="F62" t="n">
-        <v>113</v>
-      </c>
-      <c r="G62" t="n">
-        <v>1638</v>
-      </c>
-      <c r="H62" t="n">
-        <v>-0.9084022159273509</v>
-      </c>
-      <c r="I62" t="n">
-        <v>4.993569938620937e-07</v>
-      </c>
-      <c r="J62" t="n">
-        <v>0.0008335132633354456</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="inlineStr"/>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="n">
-        <v>62</v>
-      </c>
-      <c r="F63" t="n">
-        <v>117</v>
-      </c>
-      <c r="G63" t="n">
-        <v>1667</v>
-      </c>
-      <c r="H63" t="n">
-        <v>-0.9084025206304137</v>
-      </c>
-      <c r="I63" t="n">
-        <v>7.163792600239915e-07</v>
-      </c>
-      <c r="J63" t="n">
-        <v>0.0002693064057895489</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="n">
-        <v>62</v>
-      </c>
-      <c r="F64" t="n">
-        <v>118</v>
-      </c>
-      <c r="G64" t="n">
-        <v>1668</v>
-      </c>
-      <c r="H64" t="n">
-        <v>-0.9084026168250524</v>
-      </c>
-      <c r="I64" t="n">
-        <v>2.98370024978678e-07</v>
-      </c>
-      <c r="J64" t="n">
-        <v>0.0003909110944457294</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final updates config checks
</commit_message>
<xml_diff>
--- a/tests/regression_data/design_optimization.xlsx
+++ b/tests/regression_data/design_optimization.xlsx
@@ -499,7 +499,7 @@
         <v>1585000</v>
       </c>
       <c r="F2" t="n">
-        <v>3976.448895352781</v>
+        <v>3977.764947514536</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -647,70 +647,70 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.227042688033876</v>
+        <v>2.227151947864928</v>
       </c>
       <c r="C2" t="n">
-        <v>2.283911639304897</v>
+        <v>2.2839116530672</v>
       </c>
       <c r="D2" t="n">
-        <v>10.65999965361875</v>
+        <v>10.66000002256525</v>
       </c>
       <c r="E2" t="n">
-        <v>93.67808645241342</v>
+        <v>93.79581776406162</v>
       </c>
       <c r="F2" t="n">
-        <v>90.84031265372248</v>
+        <v>90.96022570562324</v>
       </c>
       <c r="G2" t="n">
-        <v>0.03029282414017371</v>
+        <v>0.03023154044641057</v>
       </c>
       <c r="H2" t="n">
-        <v>-89.87060547786265</v>
+        <v>-89.99045724606965</v>
       </c>
       <c r="I2" t="n">
-        <v>227072.2153732921</v>
+        <v>227371.9681637993</v>
       </c>
       <c r="J2" t="n">
-        <v>57.10427100890649</v>
+        <v>57.16073502680701</v>
       </c>
       <c r="K2" t="n">
-        <v>3976.448895352781</v>
+        <v>3977.764947514536</v>
       </c>
       <c r="L2" t="n">
-        <v>3.090530566745351</v>
+        <v>2.475340382755529</v>
       </c>
       <c r="M2" t="n">
-        <v>37.69198179992932</v>
+        <v>37.6538362427284</v>
       </c>
       <c r="N2" t="n">
         <v>216.5604229337033</v>
       </c>
       <c r="O2" t="n">
-        <v>185.5038172636049</v>
+        <v>185.7269854854344</v>
       </c>
       <c r="P2" t="n">
-        <v>0.8565914988095222</v>
+        <v>0.8576220113048632</v>
       </c>
       <c r="Q2" t="n">
         <v>497686.3106530505</v>
       </c>
       <c r="R2" t="n">
-        <v>476384.9764361954</v>
+        <v>476356.8577747677</v>
       </c>
       <c r="S2" t="n">
         <v>474237.1022624383</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9113110780726753</v>
+        <v>0.911612702883369</v>
       </c>
       <c r="U2" t="n">
-        <v>0.6989862158304685</v>
+        <v>0.7000366906688344</v>
       </c>
       <c r="V2" t="n">
-        <v>0.8565914988095222</v>
+        <v>0.8576220113048632</v>
       </c>
       <c r="W2" t="n">
-        <v>1.014196781788576</v>
+        <v>1.015207331940892</v>
       </c>
     </row>
   </sheetData>
@@ -1362,10 +1362,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>12.38990724163974</v>
+        <v>12.36821977728593</v>
       </c>
       <c r="D2" t="n">
-        <v>12.38990724163974</v>
+        <v>12.36821977728593</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1374,10 +1374,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>12.38990724163974</v>
+        <v>12.36821977728593</v>
       </c>
       <c r="H2" t="n">
-        <v>12.38990724163974</v>
+        <v>12.36821977728593</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1386,102 +1386,102 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>463.0421150040211</v>
+        <v>463.0424922746769</v>
       </c>
       <c r="L2" t="n">
-        <v>3610328.398905194</v>
+        <v>3610362.183828706</v>
       </c>
       <c r="M2" t="n">
-        <v>125.8416444479905</v>
+        <v>125.8427953268424</v>
       </c>
       <c r="N2" t="n">
-        <v>468920.0991360247</v>
+        <v>468920.3615129316</v>
       </c>
       <c r="O2" t="n">
-        <v>497609.5557522508</v>
+        <v>497609.8242227497</v>
       </c>
       <c r="P2" t="n">
         <v>1837.707528152813</v>
       </c>
       <c r="Q2" t="n">
-        <v>-353326.4248424391</v>
+        <v>-353326.8496850646</v>
       </c>
       <c r="R2" t="n">
-        <v>962.210455394315</v>
+        <v>962.2109911396508</v>
       </c>
       <c r="S2" t="n">
-        <v>1093.997049278801</v>
+        <v>1093.998131013886</v>
       </c>
       <c r="T2" t="n">
-        <v>1.136962338276069</v>
+        <v>1.136962829449854</v>
       </c>
       <c r="U2" t="n">
-        <v>0.8943877510689475</v>
+        <v>0.8943872123197021</v>
       </c>
       <c r="V2" t="n">
-        <v>171.3352175015731</v>
+        <v>171.3352371551619</v>
       </c>
       <c r="W2" t="n">
-        <v>3694176.704229427</v>
+        <v>3694211.336663066</v>
       </c>
       <c r="X2" t="n">
-        <v>2.706963093712084e-07</v>
+        <v>2.706937716517559e-07</v>
       </c>
       <c r="Y2" t="n">
-        <v>3249163.65288824</v>
+        <v>3249192.709712944</v>
       </c>
       <c r="Z2" t="n">
-        <v>3.077715088653912e-07</v>
+        <v>3.07768756531633e-07</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.003320104623385129</v>
+        <v>0.003320110484701121</v>
       </c>
       <c r="AB2" t="n">
-        <v>2.133798409767246e-05</v>
+        <v>2.133802347008626e-05</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.02951130243679343</v>
+        <v>0.02951135806146724</v>
       </c>
       <c r="AD2" t="n">
-        <v>16.25585319706831</v>
+        <v>16.28328319945192</v>
       </c>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="n">
-        <v>3610328.398905194</v>
+        <v>3610362.183828706</v>
       </c>
       <c r="AH2" t="n">
-        <v>125.8416444479905</v>
+        <v>125.8427953268424</v>
       </c>
       <c r="AI2" t="n">
-        <v>125.8416444479905</v>
+        <v>125.8427953268424</v>
       </c>
       <c r="AJ2" t="n">
-        <v>468920.0991360247</v>
+        <v>468920.3615129316</v>
       </c>
       <c r="AK2" t="n">
-        <v>497609.5557522508</v>
+        <v>497609.8242227497</v>
       </c>
       <c r="AL2" t="n">
         <v>1837.707528152813</v>
       </c>
       <c r="AM2" t="n">
-        <v>962.210455394315</v>
+        <v>962.2109911396508</v>
       </c>
       <c r="AN2" t="n">
-        <v>1093.997049278801</v>
+        <v>1093.998131013886</v>
       </c>
       <c r="AO2" t="n">
-        <v>171.3352175015731</v>
+        <v>171.3352371551619</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.8943877510689475</v>
+        <v>0.8943872123197021</v>
       </c>
       <c r="AQ2" t="n">
-        <v>2.133798409767246e-05</v>
+        <v>2.133802347008626e-05</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.02951130243679343</v>
+        <v>0.02951135806146724</v>
       </c>
       <c r="AS2" t="n">
         <v>463.1499999987578</v>
@@ -1680,16 +1680,16 @@
         <v>0.02952721766241618</v>
       </c>
       <c r="DI2" t="n">
-        <v>0.07231383846421409</v>
+        <v>0.0721872510444843</v>
       </c>
       <c r="DJ2" t="n">
-        <v>0.07231383846421409</v>
+        <v>0.0721872510444843</v>
       </c>
       <c r="DK2" t="n">
-        <v>759317.1921973135</v>
+        <v>757455.2056797787</v>
       </c>
       <c r="DL2" t="n">
-        <v>10.65999997293771</v>
+        <v>10.6600001303714</v>
       </c>
       <c r="DM2" t="n">
         <v>497686.3106530505</v>
@@ -1711,358 +1711,358 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>119.0418871241251</v>
+        <v>118.6407351946236</v>
       </c>
       <c r="D3" t="n">
-        <v>22.67826107111551</v>
+        <v>22.59486093300653</v>
       </c>
       <c r="E3" t="n">
-        <v>116.8617446595047</v>
+        <v>116.4692934079145</v>
       </c>
       <c r="F3" t="n">
-        <v>79.01765174713842</v>
+        <v>79.02108454732277</v>
       </c>
       <c r="G3" t="n">
-        <v>119.0418871241251</v>
+        <v>118.6407351946236</v>
       </c>
       <c r="H3" t="n">
-        <v>22.67826107111551</v>
+        <v>22.59486093300653</v>
       </c>
       <c r="I3" t="n">
-        <v>116.8617446595047</v>
+        <v>116.4692934079145</v>
       </c>
       <c r="J3" t="n">
-        <v>79.01765174713842</v>
+        <v>79.02108454732277</v>
       </c>
       <c r="K3" t="n">
-        <v>453.2035767851328</v>
+        <v>453.2711658668854</v>
       </c>
       <c r="L3" t="n">
-        <v>2781184.474470288</v>
+        <v>2786661.134696331</v>
       </c>
       <c r="M3" t="n">
-        <v>97.40001062108095</v>
+        <v>97.58952243095221</v>
       </c>
       <c r="N3" t="n">
-        <v>462046.5729369614</v>
+        <v>462093.5773091174</v>
       </c>
       <c r="O3" t="n">
-        <v>490600.8252079395</v>
+        <v>490648.4986293645</v>
       </c>
       <c r="P3" t="n">
-        <v>1838.711065814871</v>
+        <v>1838.69231077327</v>
       </c>
       <c r="Q3" t="n">
-        <v>-342709.6064937637</v>
+        <v>-342777.7087453131</v>
       </c>
       <c r="R3" t="n">
-        <v>947.9593802929335</v>
+        <v>948.059967048864</v>
       </c>
       <c r="S3" t="n">
-        <v>1066.053138041856</v>
+        <v>1066.24663035286</v>
       </c>
       <c r="T3" t="n">
-        <v>1.124576812260067</v>
+        <v>1.12466159041805</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9094974307578179</v>
+        <v>0.9093831190317795</v>
       </c>
       <c r="V3" t="n">
-        <v>171.1107948571363</v>
+        <v>171.1100850911274</v>
       </c>
       <c r="W3" t="n">
-        <v>2851765.571934444</v>
+        <v>2857290.565866986</v>
       </c>
       <c r="X3" t="n">
-        <v>3.506599595147185e-07</v>
+        <v>3.499819066166869e-07</v>
       </c>
       <c r="Y3" t="n">
-        <v>2535856.635887092</v>
+        <v>2540578.063846652</v>
       </c>
       <c r="Z3" t="n">
-        <v>3.943440594583062e-07</v>
+        <v>3.936112077130645e-07</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.003163617434231275</v>
+        <v>0.003164758053624418</v>
       </c>
       <c r="AB3" t="n">
-        <v>2.038589962153135e-05</v>
+        <v>2.039204973153515e-05</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.02810919898684134</v>
+        <v>0.02811858515351782</v>
       </c>
       <c r="AD3" t="n">
-        <v>3.139358796022666</v>
+        <v>3.146670114868681</v>
       </c>
       <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="n">
-        <v>2781184.474470288</v>
+        <v>2786661.134696331</v>
       </c>
       <c r="AH3" t="n">
-        <v>97.40001062108095</v>
+        <v>97.58952243095221</v>
       </c>
       <c r="AI3" t="n">
-        <v>97.40001062108095</v>
+        <v>97.58952243095221</v>
       </c>
       <c r="AJ3" t="n">
-        <v>462046.5729369614</v>
+        <v>462093.5773091174</v>
       </c>
       <c r="AK3" t="n">
-        <v>490600.8252079395</v>
+        <v>490648.4986293645</v>
       </c>
       <c r="AL3" t="n">
-        <v>1838.711065814871</v>
+        <v>1838.69231077327</v>
       </c>
       <c r="AM3" t="n">
-        <v>947.9593802929335</v>
+        <v>948.059967048864</v>
       </c>
       <c r="AN3" t="n">
-        <v>1066.053138041856</v>
+        <v>1066.24663035286</v>
       </c>
       <c r="AO3" t="n">
-        <v>171.1107948571363</v>
+        <v>171.1100850911274</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.9094974307578179</v>
+        <v>0.9093831190317795</v>
       </c>
       <c r="AQ3" t="n">
-        <v>2.038589962153135e-05</v>
+        <v>2.039204973153515e-05</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.02810919898684134</v>
+        <v>0.02811858515351782</v>
       </c>
       <c r="AS3" t="n">
-        <v>462.923104892691</v>
+        <v>462.9273121629154</v>
       </c>
       <c r="AT3" t="n">
-        <v>3561873.731643836</v>
+        <v>3562950.636844302</v>
       </c>
       <c r="AU3" t="n">
-        <v>124.0163000864333</v>
+        <v>124.0561930398347</v>
       </c>
       <c r="AV3" t="n">
-        <v>468965.2979380261</v>
+        <v>468965.8530156869</v>
       </c>
       <c r="AW3" t="n">
-        <v>497686.3106529787</v>
+        <v>497686.310652979</v>
       </c>
       <c r="AX3" t="n">
-        <v>1838.71106581487</v>
+        <v>1838.692310773269</v>
       </c>
       <c r="AY3" t="n">
-        <v>-353495.5249345902</v>
+        <v>-353494.5786679107</v>
       </c>
       <c r="AZ3" t="n">
-        <v>961.8095044357805</v>
+        <v>961.8197925965275</v>
       </c>
       <c r="BA3" t="n">
-        <v>1092.554816777956</v>
+        <v>1092.587248908932</v>
       </c>
       <c r="BB3" t="n">
-        <v>1.135936806341786</v>
+        <v>1.135958375278788</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.8956016914470506</v>
+        <v>0.8955762431372412</v>
       </c>
       <c r="BD3" t="n">
-        <v>171.4488533266321</v>
+        <v>171.4468276035726</v>
       </c>
       <c r="BE3" t="n">
-        <v>3645423.090372493</v>
+        <v>3646509.561259492</v>
       </c>
       <c r="BF3" t="n">
-        <v>2.743165814253453e-07</v>
+        <v>2.742348492991756e-07</v>
       </c>
       <c r="BG3" t="n">
-        <v>3209177.720116626</v>
+        <v>3210073.22153381</v>
       </c>
       <c r="BH3" t="n">
-        <v>3.116063014309032e-07</v>
+        <v>3.115193738547149e-07</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.003303704050311836</v>
+        <v>0.003304039199726039</v>
       </c>
       <c r="BJ3" t="n">
-        <v>2.129409952281714e-05</v>
+        <v>2.129511678122448e-05</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.02946680802999982</v>
+        <v>0.02946792516800589</v>
       </c>
       <c r="BL3" t="n">
-        <v>7.975887984568375</v>
+        <v>8.028534606518111</v>
       </c>
       <c r="BM3" t="inlineStr"/>
       <c r="BN3" t="inlineStr"/>
       <c r="BO3" t="n">
-        <v>3561873.731643836</v>
+        <v>3562950.636844302</v>
       </c>
       <c r="BP3" t="n">
-        <v>124.0163000864333</v>
+        <v>124.0561930398347</v>
       </c>
       <c r="BQ3" t="n">
-        <v>124.0163000864333</v>
+        <v>124.0561930398347</v>
       </c>
       <c r="BR3" t="n">
-        <v>468965.2979380261</v>
+        <v>468965.8530156869</v>
       </c>
       <c r="BS3" t="n">
-        <v>497686.3106529787</v>
+        <v>497686.310652979</v>
       </c>
       <c r="BT3" t="n">
-        <v>1838.71106581487</v>
+        <v>1838.692310773269</v>
       </c>
       <c r="BU3" t="n">
-        <v>961.8095044357805</v>
+        <v>961.8197925965275</v>
       </c>
       <c r="BV3" t="n">
-        <v>1092.554816777956</v>
+        <v>1092.587248908932</v>
       </c>
       <c r="BW3" t="n">
-        <v>171.4488533266321</v>
+        <v>171.4468276035726</v>
       </c>
       <c r="BX3" t="n">
-        <v>0.8956016914470506</v>
+        <v>0.8955762431372412</v>
       </c>
       <c r="BY3" t="n">
-        <v>2.129409952281714e-05</v>
+        <v>2.129511678122448e-05</v>
       </c>
       <c r="BZ3" t="n">
-        <v>0.02946680802999982</v>
+        <v>0.02946792516800589</v>
       </c>
       <c r="CA3" t="n">
-        <v>462.923104892691</v>
+        <v>462.9273121629154</v>
       </c>
       <c r="CB3" t="n">
-        <v>3561873.731643836</v>
+        <v>3562950.636844302</v>
       </c>
       <c r="CC3" t="n">
-        <v>124.0163000864333</v>
+        <v>124.0561930398347</v>
       </c>
       <c r="CD3" t="n">
-        <v>468965.2979380261</v>
+        <v>468965.8530156869</v>
       </c>
       <c r="CE3" t="n">
-        <v>497686.3106529787</v>
+        <v>497686.310652979</v>
       </c>
       <c r="CF3" t="n">
-        <v>1838.71106581487</v>
+        <v>1838.692310773269</v>
       </c>
       <c r="CG3" t="n">
-        <v>-353495.5249345902</v>
+        <v>-353494.5786679107</v>
       </c>
       <c r="CH3" t="n">
-        <v>961.8095044357805</v>
+        <v>961.8197925965275</v>
       </c>
       <c r="CI3" t="n">
-        <v>1092.554816777956</v>
+        <v>1092.587248908932</v>
       </c>
       <c r="CJ3" t="n">
-        <v>1.135936806341786</v>
+        <v>1.135958375278788</v>
       </c>
       <c r="CK3" t="n">
-        <v>0.8956016914470506</v>
+        <v>0.8955762431372412</v>
       </c>
       <c r="CL3" t="n">
-        <v>171.4488533266321</v>
+        <v>171.4468276035726</v>
       </c>
       <c r="CM3" t="n">
-        <v>3645423.090372493</v>
+        <v>3646509.561259492</v>
       </c>
       <c r="CN3" t="n">
-        <v>2.743165814253453e-07</v>
+        <v>2.742348492991756e-07</v>
       </c>
       <c r="CO3" t="n">
-        <v>3209177.720116626</v>
+        <v>3210073.22153381</v>
       </c>
       <c r="CP3" t="n">
-        <v>3.116063014309032e-07</v>
+        <v>3.115193738547149e-07</v>
       </c>
       <c r="CQ3" t="n">
-        <v>0.003303704050311836</v>
+        <v>0.003304039199726039</v>
       </c>
       <c r="CR3" t="n">
-        <v>2.129409952281714e-05</v>
+        <v>2.129511678122448e-05</v>
       </c>
       <c r="CS3" t="n">
-        <v>0.02946680802999982</v>
+        <v>0.02946792516800589</v>
       </c>
       <c r="CT3" t="n">
-        <v>7.975887984568375</v>
+        <v>8.028534606518111</v>
       </c>
       <c r="CU3" t="inlineStr"/>
       <c r="CV3" t="inlineStr"/>
       <c r="CW3" t="n">
-        <v>3561873.731643836</v>
+        <v>3562950.636844302</v>
       </c>
       <c r="CX3" t="n">
-        <v>124.0163000864333</v>
+        <v>124.0561930398347</v>
       </c>
       <c r="CY3" t="n">
-        <v>124.0163000864333</v>
+        <v>124.0561930398347</v>
       </c>
       <c r="CZ3" t="n">
-        <v>468965.2979380261</v>
+        <v>468965.8530156869</v>
       </c>
       <c r="DA3" t="n">
-        <v>497686.3106529787</v>
+        <v>497686.310652979</v>
       </c>
       <c r="DB3" t="n">
-        <v>1838.71106581487</v>
+        <v>1838.692310773269</v>
       </c>
       <c r="DC3" t="n">
-        <v>961.8095044357805</v>
+        <v>961.8197925965275</v>
       </c>
       <c r="DD3" t="n">
-        <v>1092.554816777956</v>
+        <v>1092.587248908932</v>
       </c>
       <c r="DE3" t="n">
-        <v>171.4488533266321</v>
+        <v>171.4468276035726</v>
       </c>
       <c r="DF3" t="n">
-        <v>0.8956016914470506</v>
+        <v>0.8955762431372412</v>
       </c>
       <c r="DG3" t="n">
-        <v>2.129409952281714e-05</v>
+        <v>2.129511678122448e-05</v>
       </c>
       <c r="DH3" t="n">
-        <v>0.02946680802999982</v>
+        <v>0.02946792516800589</v>
       </c>
       <c r="DI3" t="n">
-        <v>0.6957006261557926</v>
+        <v>0.6933591034768029</v>
       </c>
       <c r="DJ3" t="n">
-        <v>0.6957006261557926</v>
+        <v>0.6933591034768029</v>
       </c>
       <c r="DK3" t="n">
-        <v>5910348.726371001</v>
+        <v>5895922.049525524</v>
       </c>
       <c r="DL3" t="n">
-        <v>10.66000004754654</v>
+        <v>10.66000017013204</v>
       </c>
       <c r="DM3" t="n">
         <v>497686.3106530505</v>
       </c>
       <c r="DN3" t="n">
-        <v>0.02228041746933479</v>
+        <v>0.01980004381651392</v>
       </c>
       <c r="DO3" t="n">
         <v>0</v>
       </c>
       <c r="DP3" t="n">
-        <v>0.01154788426814579</v>
+        <v>0.01172080958049171</v>
       </c>
       <c r="DQ3" t="n">
-        <v>0.04062680325903407</v>
+        <v>0.04196894844846946</v>
       </c>
       <c r="DR3" t="n">
         <v>0</v>
       </c>
       <c r="DS3" t="n">
-        <v>0.07445510499651464</v>
+        <v>0.0734898018454751</v>
       </c>
       <c r="DT3" t="n">
-        <v>-4.136982939551004e-08</v>
+        <v>1.838855456792743e-09</v>
       </c>
       <c r="DU3" t="n">
         <v>0</v>
@@ -2073,340 +2073,340 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>185.5038172636049</v>
+        <v>185.7269854854344</v>
       </c>
       <c r="C4" t="n">
-        <v>119.0418871240997</v>
+        <v>118.6407351946266</v>
       </c>
       <c r="D4" t="n">
-        <v>22.67826107098182</v>
+        <v>22.59486093302263</v>
       </c>
       <c r="E4" t="n">
-        <v>116.8617446595047</v>
+        <v>116.4692934079145</v>
       </c>
       <c r="F4" t="n">
-        <v>79.01765174720158</v>
+        <v>79.02108454731514</v>
       </c>
       <c r="G4" t="n">
-        <v>72.29133873840054</v>
+        <v>72.85022753902139</v>
       </c>
       <c r="H4" t="n">
-        <v>22.67826107098182</v>
+        <v>22.59486093302263</v>
       </c>
       <c r="I4" t="n">
-        <v>-68.64207260410019</v>
+        <v>-69.25769207751988</v>
       </c>
       <c r="J4" t="n">
-        <v>-71.71725745657214</v>
+        <v>-71.93142939380483</v>
       </c>
       <c r="K4" t="n">
-        <v>453.2035767852385</v>
+        <v>453.2711658667434</v>
       </c>
       <c r="L4" t="n">
-        <v>2781184.474477571</v>
+        <v>2786661.134695223</v>
       </c>
       <c r="M4" t="n">
-        <v>97.40001062132806</v>
+        <v>97.58952243095351</v>
       </c>
       <c r="N4" t="n">
-        <v>462046.5729370393</v>
+        <v>462093.5773089828</v>
       </c>
       <c r="O4" t="n">
-        <v>490600.8252080198</v>
+        <v>490648.4986292182</v>
       </c>
       <c r="P4" t="n">
-        <v>1838.711065814882</v>
+        <v>1838.692310772972</v>
       </c>
       <c r="Q4" t="n">
-        <v>-342709.606493883</v>
+        <v>-342777.7087450634</v>
       </c>
       <c r="R4" t="n">
-        <v>947.9593802930822</v>
+        <v>948.0599670487237</v>
       </c>
       <c r="S4" t="n">
-        <v>1066.05313804212</v>
+        <v>1066.24663035276</v>
       </c>
       <c r="T4" t="n">
-        <v>1.12457681226017</v>
+        <v>1.124661590418112</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9094974307576799</v>
+        <v>0.9093831190316906</v>
       </c>
       <c r="V4" t="n">
-        <v>171.1107948571404</v>
+        <v>171.1100850910873</v>
       </c>
       <c r="W4" t="n">
-        <v>2851765.571941813</v>
+        <v>2857290.565865685</v>
       </c>
       <c r="X4" t="n">
-        <v>3.506599595138123e-07</v>
+        <v>3.499819066168462e-07</v>
       </c>
       <c r="Y4" t="n">
-        <v>2535856.635893414</v>
+        <v>2540578.063845356</v>
       </c>
       <c r="Z4" t="n">
-        <v>3.943440594573232e-07</v>
+        <v>3.936112077132653e-07</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.003163617434232532</v>
+        <v>0.003164758053626289</v>
       </c>
       <c r="AB4" t="n">
-        <v>2.038589962153989e-05</v>
+        <v>2.039204973152943e-05</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.02810919898685517</v>
+        <v>0.02811858515350499</v>
       </c>
       <c r="AD4" t="n">
-        <v>3.139358796032601</v>
+        <v>3.146670114865183</v>
       </c>
       <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="n">
-        <v>2781184.474477571</v>
+        <v>2786661.134695223</v>
       </c>
       <c r="AH4" t="n">
-        <v>97.40001062132806</v>
+        <v>97.58952243095351</v>
       </c>
       <c r="AI4" t="n">
-        <v>97.40001062132806</v>
+        <v>97.58952243095351</v>
       </c>
       <c r="AJ4" t="n">
-        <v>462046.5729370393</v>
+        <v>462093.5773089828</v>
       </c>
       <c r="AK4" t="n">
-        <v>490600.8252080198</v>
+        <v>490648.4986292182</v>
       </c>
       <c r="AL4" t="n">
-        <v>1838.711065814882</v>
+        <v>1838.692310772972</v>
       </c>
       <c r="AM4" t="n">
-        <v>947.9593802930822</v>
+        <v>948.0599670487237</v>
       </c>
       <c r="AN4" t="n">
-        <v>1066.05313804212</v>
+        <v>1066.24663035276</v>
       </c>
       <c r="AO4" t="n">
-        <v>171.1107948571404</v>
+        <v>171.1100850910873</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.9094974307576799</v>
+        <v>0.9093831190316906</v>
       </c>
       <c r="AQ4" t="n">
-        <v>2.038589962153989e-05</v>
+        <v>2.039204973152943e-05</v>
       </c>
       <c r="AR4" t="n">
-        <v>0.02810919898685517</v>
+        <v>0.02811858515350499</v>
       </c>
       <c r="AS4" t="n">
-        <v>462.9231048926883</v>
+        <v>462.9273121628818</v>
       </c>
       <c r="AT4" t="n">
-        <v>3561873.731643156</v>
+        <v>3562950.636852475</v>
       </c>
       <c r="AU4" t="n">
-        <v>124.016300086408</v>
+        <v>124.0561930401644</v>
       </c>
       <c r="AV4" t="n">
-        <v>468965.2979380256</v>
+        <v>468965.8530156256</v>
       </c>
       <c r="AW4" t="n">
-        <v>497686.3106529787</v>
+        <v>497686.3106529073</v>
       </c>
       <c r="AX4" t="n">
-        <v>1838.711065814882</v>
+        <v>1838.692310772971</v>
       </c>
       <c r="AY4" t="n">
-        <v>-353495.5249345907</v>
+        <v>-353494.5786677827</v>
       </c>
       <c r="AZ4" t="n">
-        <v>961.8095044357738</v>
+        <v>961.8197925965482</v>
       </c>
       <c r="BA4" t="n">
-        <v>1092.554816777935</v>
+        <v>1092.587248909161</v>
       </c>
       <c r="BB4" t="n">
-        <v>1.135936806341772</v>
+        <v>1.135958375279001</v>
       </c>
       <c r="BC4" t="n">
-        <v>0.8956016914470669</v>
+        <v>0.8955762431369805</v>
       </c>
       <c r="BD4" t="n">
-        <v>171.4488533266334</v>
+        <v>171.4468276035354</v>
       </c>
       <c r="BE4" t="n">
-        <v>3645423.090371807</v>
+        <v>3646509.5612676</v>
       </c>
       <c r="BF4" t="n">
-        <v>2.74316581425397e-07</v>
+        <v>2.742348492985659e-07</v>
       </c>
       <c r="BG4" t="n">
-        <v>3209177.72011606</v>
+        <v>3210073.221540345</v>
       </c>
       <c r="BH4" t="n">
-        <v>3.116063014309581e-07</v>
+        <v>3.115193738540807e-07</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.003303704050311623</v>
+        <v>0.003304039199729813</v>
       </c>
       <c r="BJ4" t="n">
-        <v>2.129409952281705e-05</v>
+        <v>2.129511678123073e-05</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.0294668080299991</v>
+        <v>0.0294679251680089</v>
       </c>
       <c r="BL4" t="n">
-        <v>7.975887984536678</v>
+        <v>8.028534606919878</v>
       </c>
       <c r="BM4" t="inlineStr"/>
       <c r="BN4" t="inlineStr"/>
       <c r="BO4" t="n">
-        <v>3561873.731643156</v>
+        <v>3562950.636852475</v>
       </c>
       <c r="BP4" t="n">
-        <v>124.016300086408</v>
+        <v>124.0561930401644</v>
       </c>
       <c r="BQ4" t="n">
-        <v>124.016300086408</v>
+        <v>124.0561930401644</v>
       </c>
       <c r="BR4" t="n">
-        <v>468965.2979380256</v>
+        <v>468965.8530156256</v>
       </c>
       <c r="BS4" t="n">
-        <v>497686.3106529787</v>
+        <v>497686.3106529073</v>
       </c>
       <c r="BT4" t="n">
-        <v>1838.711065814882</v>
+        <v>1838.692310772971</v>
       </c>
       <c r="BU4" t="n">
-        <v>961.8095044357738</v>
+        <v>961.8197925965482</v>
       </c>
       <c r="BV4" t="n">
-        <v>1092.554816777935</v>
+        <v>1092.587248909161</v>
       </c>
       <c r="BW4" t="n">
-        <v>171.4488533266334</v>
+        <v>171.4468276035354</v>
       </c>
       <c r="BX4" t="n">
-        <v>0.8956016914470669</v>
+        <v>0.8955762431369805</v>
       </c>
       <c r="BY4" t="n">
-        <v>2.129409952281705e-05</v>
+        <v>2.129511678123073e-05</v>
       </c>
       <c r="BZ4" t="n">
-        <v>0.0294668080299991</v>
+        <v>0.0294679251680089</v>
       </c>
       <c r="CA4" t="n">
-        <v>456.7429629220757</v>
+        <v>456.8670989261845</v>
       </c>
       <c r="CB4" t="n">
-        <v>3047390.770152799</v>
+        <v>3057715.885893652</v>
       </c>
       <c r="CC4" t="n">
-        <v>106.487226582791</v>
+        <v>106.8422115224492</v>
       </c>
       <c r="CD4" t="n">
-        <v>464596.4138717342</v>
+        <v>464683.0892375571</v>
       </c>
       <c r="CE4" t="n">
-        <v>493213.8440363139</v>
+        <v>493302.0764554618</v>
       </c>
       <c r="CF4" t="n">
-        <v>1838.711065814882</v>
+        <v>1838.692310772972</v>
       </c>
       <c r="CG4" t="n">
-        <v>-346604.496121583</v>
+        <v>-346735.9453852685</v>
       </c>
       <c r="CH4" t="n">
-        <v>953.0148291229207</v>
+        <v>953.1960415863164</v>
       </c>
       <c r="CI4" t="n">
-        <v>1075.4381811292</v>
+        <v>1075.791138820839</v>
       </c>
       <c r="CJ4" t="n">
-        <v>1.128459021061559</v>
+        <v>1.12861477795323</v>
       </c>
       <c r="CK4" t="n">
-        <v>0.9044462866367438</v>
+        <v>0.90424973514617</v>
       </c>
       <c r="CL4" t="n">
-        <v>171.2052540470054</v>
+        <v>171.2067265336125</v>
       </c>
       <c r="CM4" t="n">
-        <v>3121272.550231584</v>
+        <v>3131731.46817248</v>
       </c>
       <c r="CN4" t="n">
-        <v>3.203821466746967e-07</v>
+        <v>3.193121792730044e-07</v>
       </c>
       <c r="CO4" t="n">
-        <v>2765960.032199801</v>
+        <v>2774845.349670105</v>
       </c>
       <c r="CP4" t="n">
-        <v>3.615381236021288e-07</v>
+        <v>3.603804443079639e-07</v>
       </c>
       <c r="CQ4" t="n">
-        <v>0.003212343721804881</v>
+        <v>0.003214353612700892</v>
       </c>
       <c r="CR4" t="n">
-        <v>2.069639940915096e-05</v>
+        <v>2.070815687562728e-05</v>
       </c>
       <c r="CS4" t="n">
-        <v>0.02858863389510442</v>
+        <v>0.02860617330842331</v>
       </c>
       <c r="CT4" t="n">
-        <v>3.598878927962373</v>
+        <v>3.622024986330358</v>
       </c>
       <c r="CU4" t="inlineStr"/>
       <c r="CV4" t="inlineStr"/>
       <c r="CW4" t="n">
-        <v>3047390.770152799</v>
+        <v>3057715.885893652</v>
       </c>
       <c r="CX4" t="n">
-        <v>106.487226582791</v>
+        <v>106.8422115224492</v>
       </c>
       <c r="CY4" t="n">
-        <v>106.487226582791</v>
+        <v>106.8422115224492</v>
       </c>
       <c r="CZ4" t="n">
-        <v>464596.4138717342</v>
+        <v>464683.0892375571</v>
       </c>
       <c r="DA4" t="n">
-        <v>493213.8440363139</v>
+        <v>493302.0764554618</v>
       </c>
       <c r="DB4" t="n">
-        <v>1838.711065814882</v>
+        <v>1838.692310772972</v>
       </c>
       <c r="DC4" t="n">
-        <v>953.0148291229207</v>
+        <v>953.1960415863164</v>
       </c>
       <c r="DD4" t="n">
-        <v>1075.4381811292</v>
+        <v>1075.791138820839</v>
       </c>
       <c r="DE4" t="n">
-        <v>171.2052540470054</v>
+        <v>171.2067265336125</v>
       </c>
       <c r="DF4" t="n">
-        <v>0.9044462866367438</v>
+        <v>0.90424973514617</v>
       </c>
       <c r="DG4" t="n">
-        <v>2.069639940915096e-05</v>
+        <v>2.070815687562728e-05</v>
       </c>
       <c r="DH4" t="n">
-        <v>0.02858863389510442</v>
+        <v>0.02860617330842331</v>
       </c>
       <c r="DI4" t="n">
-        <v>0.6957006261556274</v>
+        <v>0.693359103476983</v>
       </c>
       <c r="DJ4" t="n">
-        <v>0.4224826306181106</v>
+        <v>0.4257506359151239</v>
       </c>
       <c r="DK4" t="n">
-        <v>2913195.82880023</v>
+        <v>2941179.927099155</v>
       </c>
       <c r="DL4" t="n">
-        <v>10.66000004757358</v>
+        <v>10.66000017013219</v>
       </c>
       <c r="DM4" t="n">
-        <v>476008.0109265559</v>
+        <v>476054.8198867084</v>
       </c>
       <c r="DN4" t="inlineStr"/>
       <c r="DO4" t="inlineStr"/>
@@ -2422,361 +2422,361 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>185.5038172636049</v>
+        <v>185.7269854854344</v>
       </c>
       <c r="C5" t="n">
-        <v>37.69198179992932</v>
+        <v>37.6538362427284</v>
       </c>
       <c r="D5" t="n">
-        <v>37.63716237221433</v>
+        <v>37.61870154095219</v>
       </c>
       <c r="E5" t="n">
-        <v>2.032117263786063</v>
+        <v>1.626246650102019</v>
       </c>
       <c r="F5" t="n">
-        <v>3.090530566745351</v>
+        <v>2.475340382755529</v>
       </c>
       <c r="G5" t="n">
-        <v>187.2923401857533</v>
+        <v>187.9048928190602</v>
       </c>
       <c r="H5" t="n">
-        <v>37.63716237221433</v>
+        <v>37.61870154095219</v>
       </c>
       <c r="I5" t="n">
-        <v>-183.4716999998188</v>
+        <v>-184.1007388353324</v>
       </c>
       <c r="J5" t="n">
-        <v>-78.40724266020219</v>
+        <v>-78.45130107866638</v>
       </c>
       <c r="K5" t="n">
-        <v>433.56530857402</v>
+        <v>433.5390911433603</v>
       </c>
       <c r="L5" t="n">
-        <v>1585000.022619571</v>
+        <v>1585000.013068741</v>
       </c>
       <c r="M5" t="n">
-        <v>56.28835433983492</v>
+        <v>56.29267838384589</v>
       </c>
       <c r="N5" t="n">
-        <v>447516.0555754492</v>
+        <v>447491.5370999126</v>
       </c>
       <c r="O5" t="n">
-        <v>475674.6336900322</v>
+        <v>475647.9520827105</v>
       </c>
       <c r="P5" t="n">
-        <v>1841.028547192089</v>
+        <v>1840.967005726803</v>
       </c>
       <c r="Q5" t="n">
-        <v>-322531.4764668855</v>
+        <v>-322483.2104050012</v>
       </c>
       <c r="R5" t="n">
-        <v>919.4614595754555</v>
+        <v>919.4338460015102</v>
       </c>
       <c r="S5" t="n">
-        <v>1017.717043796976</v>
+        <v>1017.6962315835</v>
       </c>
       <c r="T5" t="n">
-        <v>1.106862101938333</v>
+        <v>1.106872708688416</v>
       </c>
       <c r="U5" t="n">
-        <v>0.9375192830035907</v>
+        <v>0.9375039534055785</v>
       </c>
       <c r="V5" t="n">
-        <v>170.9312099953958</v>
+        <v>170.923957038721</v>
       </c>
       <c r="W5" t="n">
-        <v>1644603.785566514</v>
+        <v>1644590.547745029</v>
       </c>
       <c r="X5" t="n">
-        <v>6.080491901917469e-07</v>
+        <v>6.080540845690404e-07</v>
       </c>
       <c r="Y5" t="n">
-        <v>1485825.364050761</v>
+        <v>1485799.166277917</v>
       </c>
       <c r="Z5" t="n">
-        <v>6.730266047375381e-07</v>
+        <v>6.73038471615989e-07</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.002930061598049747</v>
+        <v>0.002930389986183424</v>
       </c>
       <c r="AB5" t="n">
-        <v>1.894959181281052e-05</v>
+        <v>1.894864477612411e-05</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.02568561359144396</v>
+        <v>0.02568335436178383</v>
       </c>
       <c r="AD5" t="n">
-        <v>2.254278124056925</v>
+        <v>2.254022372326611</v>
       </c>
       <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="inlineStr"/>
       <c r="AG5" t="n">
-        <v>1585000.022619571</v>
+        <v>1585000.013068741</v>
       </c>
       <c r="AH5" t="n">
-        <v>56.28835433983492</v>
+        <v>56.29267838384589</v>
       </c>
       <c r="AI5" t="n">
-        <v>56.28835433983492</v>
+        <v>56.29267838384589</v>
       </c>
       <c r="AJ5" t="n">
-        <v>447516.0555754492</v>
+        <v>447491.5370999126</v>
       </c>
       <c r="AK5" t="n">
-        <v>475674.6336900322</v>
+        <v>475647.9520827105</v>
       </c>
       <c r="AL5" t="n">
-        <v>1841.028547192089</v>
+        <v>1840.967005726803</v>
       </c>
       <c r="AM5" t="n">
-        <v>919.4614595754555</v>
+        <v>919.4338460015102</v>
       </c>
       <c r="AN5" t="n">
-        <v>1017.717043796976</v>
+        <v>1017.6962315835</v>
       </c>
       <c r="AO5" t="n">
-        <v>170.9312099953958</v>
+        <v>170.923957038721</v>
       </c>
       <c r="AP5" t="n">
-        <v>0.9375192830035907</v>
+        <v>0.9375039534055785</v>
       </c>
       <c r="AQ5" t="n">
-        <v>1.894959181281052e-05</v>
+        <v>1.894864477612411e-05</v>
       </c>
       <c r="AR5" t="n">
-        <v>0.02568561359144396</v>
+        <v>0.02568335436178383</v>
       </c>
       <c r="AS5" t="n">
-        <v>434.4531369089998</v>
+        <v>434.4251852488196</v>
       </c>
       <c r="AT5" t="n">
-        <v>1625474.006138268</v>
+        <v>1625394.263480629</v>
       </c>
       <c r="AU5" t="n">
-        <v>57.67339111615116</v>
+        <v>57.67510469093092</v>
       </c>
       <c r="AV5" t="n">
-        <v>448200.8524462492</v>
+        <v>448174.95377666</v>
       </c>
       <c r="AW5" t="n">
-        <v>476384.9764361954</v>
+        <v>476356.8577747677</v>
       </c>
       <c r="AX5" t="n">
-        <v>1841.02854719193</v>
+        <v>1840.967005726644</v>
       </c>
       <c r="AY5" t="n">
-        <v>-323455.6510303572</v>
+        <v>-323405.5747249946</v>
       </c>
       <c r="AZ5" t="n">
-        <v>920.7277799447118</v>
+        <v>920.6978234389131</v>
       </c>
       <c r="BA5" t="n">
-        <v>1019.64341447234</v>
+        <v>1019.61912689835</v>
       </c>
       <c r="BB5" t="n">
-        <v>1.107432008333199</v>
+        <v>1.107441661032666</v>
       </c>
       <c r="BC5" t="n">
-        <v>0.9364522051094057</v>
+        <v>0.9364386913406459</v>
       </c>
       <c r="BD5" t="n">
-        <v>170.959209779184</v>
+        <v>170.9518683613519</v>
       </c>
       <c r="BE5" t="n">
-        <v>1685623.167044072</v>
+        <v>1685528.478804902</v>
       </c>
       <c r="BF5" t="n">
-        <v>5.932524063214031e-07</v>
+        <v>5.932857335694703e-07</v>
       </c>
       <c r="BG5" t="n">
-        <v>1522100.819156484</v>
+        <v>1522002.050413367</v>
       </c>
       <c r="BH5" t="n">
-        <v>6.569867037810144e-07</v>
+        <v>6.570293382511581e-07</v>
       </c>
       <c r="BI5" t="n">
-        <v>0.002937156152302595</v>
+        <v>0.002937473752266581</v>
       </c>
       <c r="BJ5" t="n">
-        <v>1.900371475341122e-05</v>
+        <v>1.900266402401556e-05</v>
       </c>
       <c r="BK5" t="n">
-        <v>0.02578501642097159</v>
+        <v>0.02578256199850107</v>
       </c>
       <c r="BL5" t="n">
-        <v>2.273022698324746</v>
+        <v>2.272726193506659</v>
       </c>
       <c r="BM5" t="inlineStr"/>
       <c r="BN5" t="inlineStr"/>
       <c r="BO5" t="n">
-        <v>1625474.006138268</v>
+        <v>1625394.263480629</v>
       </c>
       <c r="BP5" t="n">
-        <v>57.67339111615116</v>
+        <v>57.67510469093092</v>
       </c>
       <c r="BQ5" t="n">
-        <v>57.67339111615116</v>
+        <v>57.67510469093092</v>
       </c>
       <c r="BR5" t="n">
-        <v>448200.8524462492</v>
+        <v>448174.95377666</v>
       </c>
       <c r="BS5" t="n">
-        <v>476384.9764361954</v>
+        <v>476356.8577747677</v>
       </c>
       <c r="BT5" t="n">
-        <v>1841.02854719193</v>
+        <v>1840.967005726644</v>
       </c>
       <c r="BU5" t="n">
-        <v>920.7277799447118</v>
+        <v>920.6978234389131</v>
       </c>
       <c r="BV5" t="n">
-        <v>1019.64341447234</v>
+        <v>1019.61912689835</v>
       </c>
       <c r="BW5" t="n">
-        <v>170.959209779184</v>
+        <v>170.9518683613519</v>
       </c>
       <c r="BX5" t="n">
-        <v>0.9364522051094057</v>
+        <v>0.9364386913406459</v>
       </c>
       <c r="BY5" t="n">
-        <v>1.900371475341122e-05</v>
+        <v>1.900266402401556e-05</v>
       </c>
       <c r="BZ5" t="n">
-        <v>0.02578501642097159</v>
+        <v>0.02578256199850107</v>
       </c>
       <c r="CA5" t="n">
-        <v>456.2916095919634</v>
+        <v>456.422700920908</v>
       </c>
       <c r="CB5" t="n">
-        <v>2936910.783454746</v>
+        <v>2948845.213964269</v>
       </c>
       <c r="CC5" t="n">
-        <v>102.3952918478925</v>
+        <v>102.8097167581872</v>
       </c>
       <c r="CD5" t="n">
-        <v>464531.755920069</v>
+        <v>464619.522831663</v>
       </c>
       <c r="CE5" t="n">
-        <v>493213.8440361663</v>
+        <v>493302.0764554618</v>
       </c>
       <c r="CF5" t="n">
-        <v>1841.028547191931</v>
+        <v>1840.967005726646</v>
       </c>
       <c r="CG5" t="n">
-        <v>-346832.0350667938</v>
+        <v>-346957.0566045704</v>
       </c>
       <c r="CH5" t="n">
-        <v>951.8713741154153</v>
+        <v>952.0709739740486</v>
       </c>
       <c r="CI5" t="n">
-        <v>1072.018600656589</v>
+        <v>1072.422932497658</v>
       </c>
       <c r="CJ5" t="n">
-        <v>1.126222123921762</v>
+        <v>1.126410700266648</v>
       </c>
       <c r="CK5" t="n">
-        <v>0.9073864632094164</v>
+        <v>0.9071405710098366</v>
       </c>
       <c r="CL5" t="n">
-        <v>171.4759126461675</v>
+        <v>171.4722239592743</v>
       </c>
       <c r="CM5" t="n">
-        <v>3010829.996015432</v>
+        <v>3022885.684159829</v>
       </c>
       <c r="CN5" t="n">
-        <v>3.321343288473318e-07</v>
+        <v>3.308097309931641e-07</v>
       </c>
       <c r="CO5" t="n">
-        <v>2673389.140617338</v>
+        <v>2683644.325683554</v>
       </c>
       <c r="CP5" t="n">
-        <v>3.740570292617708e-07</v>
+        <v>3.726276207430315e-07</v>
       </c>
       <c r="CQ5" t="n">
-        <v>0.003175737065024842</v>
+        <v>0.003178319597851342</v>
       </c>
       <c r="CR5" t="n">
-        <v>2.059938808697962e-05</v>
+        <v>2.061241255071784e-05</v>
       </c>
       <c r="CS5" t="n">
-        <v>0.02847585657092499</v>
+        <v>0.02849499565103307</v>
       </c>
       <c r="CT5" t="n">
-        <v>3.396818904364442</v>
+        <v>3.417848086121974</v>
       </c>
       <c r="CU5" t="inlineStr"/>
       <c r="CV5" t="inlineStr"/>
       <c r="CW5" t="n">
-        <v>2936910.783454746</v>
+        <v>2948845.213964269</v>
       </c>
       <c r="CX5" t="n">
-        <v>102.3952918478925</v>
+        <v>102.8097167581872</v>
       </c>
       <c r="CY5" t="n">
-        <v>102.3952918478925</v>
+        <v>102.8097167581872</v>
       </c>
       <c r="CZ5" t="n">
-        <v>464531.755920069</v>
+        <v>464619.522831663</v>
       </c>
       <c r="DA5" t="n">
-        <v>493213.8440361663</v>
+        <v>493302.0764554618</v>
       </c>
       <c r="DB5" t="n">
-        <v>1841.028547191931</v>
+        <v>1840.967005726646</v>
       </c>
       <c r="DC5" t="n">
-        <v>951.8713741154153</v>
+        <v>952.0709739740486</v>
       </c>
       <c r="DD5" t="n">
-        <v>1072.018600656589</v>
+        <v>1072.422932497658</v>
       </c>
       <c r="DE5" t="n">
-        <v>171.4759126461675</v>
+        <v>171.4722239592743</v>
       </c>
       <c r="DF5" t="n">
-        <v>0.9073864632094164</v>
+        <v>0.9071405710098366</v>
       </c>
       <c r="DG5" t="n">
-        <v>2.059938808697962e-05</v>
+        <v>2.061241255071784e-05</v>
       </c>
       <c r="DH5" t="n">
-        <v>0.02847585657092499</v>
+        <v>0.02849499565103307</v>
       </c>
       <c r="DI5" t="n">
-        <v>0.2205096529822996</v>
+        <v>0.2202958373716934</v>
       </c>
       <c r="DJ5" t="n">
-        <v>1.095717629277873</v>
+        <v>1.099347897594556</v>
       </c>
       <c r="DK5" t="n">
-        <v>4692378.083824161</v>
+        <v>4709341.849148807</v>
       </c>
       <c r="DL5" t="n">
-        <v>10.65999965361875</v>
+        <v>10.66000002256525</v>
       </c>
       <c r="DM5" t="n">
-        <v>476008.0109265559</v>
+        <v>476054.8198867084</v>
       </c>
       <c r="DN5" t="n">
-        <v>0.03412930154663323</v>
+        <v>0.03281173715281153</v>
       </c>
       <c r="DO5" t="n">
         <v>0</v>
       </c>
       <c r="DP5" t="n">
-        <v>0.01159638030554655</v>
+        <v>0.01172194538417859</v>
       </c>
       <c r="DQ5" t="n">
-        <v>0.009111793222892966</v>
+        <v>0.00898903580870326</v>
       </c>
       <c r="DR5" t="n">
-        <v>0.0268839855469697</v>
+        <v>0.0263037632265502</v>
       </c>
       <c r="DS5" t="n">
-        <v>0.08172146062204244</v>
+        <v>0.07982648157224359</v>
       </c>
       <c r="DT5" t="n">
-        <v>-1.000865281208796e-07</v>
+        <v>-2.140032434178041e-07</v>
       </c>
       <c r="DU5" t="n">
         <v>0</v>
@@ -3498,150 +3498,150 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.02228041746933479</v>
+        <v>0.01980004381651392</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01154788426814579</v>
+        <v>0.01172080958049171</v>
       </c>
       <c r="E2" t="n">
-        <v>0.04062680325903407</v>
+        <v>0.04196894844846946</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.07445510499651464</v>
+        <v>0.0734898018454751</v>
       </c>
       <c r="H2" t="n">
-        <v>-4.136982939551004e-08</v>
+        <v>1.838855456792743e-09</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>118.9590493501572</v>
+        <v>118.5597259550003</v>
       </c>
       <c r="K2" t="n">
-        <v>22.29070304910059</v>
+        <v>22.21587730637121</v>
       </c>
       <c r="L2" t="n">
-        <v>116.8519575354643</v>
+        <v>116.459707255484</v>
       </c>
       <c r="M2" t="n">
-        <v>79.19999999999999</v>
+        <v>79.20000000000002</v>
       </c>
       <c r="N2" t="n">
-        <v>118.9590493501572</v>
+        <v>118.5597259550003</v>
       </c>
       <c r="O2" t="n">
-        <v>22.29070304910059</v>
+        <v>22.21587730637121</v>
       </c>
       <c r="P2" t="n">
-        <v>116.8519575354643</v>
+        <v>116.459707255484</v>
       </c>
       <c r="Q2" t="n">
-        <v>79.19999999999999</v>
+        <v>79.20000000000002</v>
       </c>
       <c r="R2" t="n">
-        <v>453.4034563245988</v>
+        <v>453.4674988769447</v>
       </c>
       <c r="S2" t="n">
-        <v>2826844.848028497</v>
+        <v>2831548.010050902</v>
       </c>
       <c r="T2" t="n">
-        <v>99.09345819806305</v>
+        <v>99.25431368764492</v>
       </c>
       <c r="U2" t="n">
-        <v>462083.6247543594</v>
+        <v>462129.8952782032</v>
       </c>
       <c r="V2" t="n">
-        <v>490610.682941978</v>
+        <v>490658.1063437881</v>
       </c>
       <c r="W2" t="n">
         <v>1837.707528152812</v>
       </c>
       <c r="X2" t="n">
-        <v>-342612.2620362422</v>
+        <v>-342682.530115</v>
       </c>
       <c r="Y2" t="n">
-        <v>948.4580611086354</v>
+        <v>948.5497546943964</v>
       </c>
       <c r="Z2" t="n">
-        <v>1067.497370419139</v>
+        <v>1067.665980566446</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.1255082477462</v>
+        <v>1.125577203813022</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.9082306934989498</v>
+        <v>0.9081391249928659</v>
       </c>
       <c r="AC2" t="n">
-        <v>170.9917238401696</v>
+        <v>170.9932491693386</v>
       </c>
       <c r="AD2" t="n">
-        <v>2897311.339208968</v>
+        <v>2902066.234283884</v>
       </c>
       <c r="AE2" t="n">
-        <v>3.451475809544937e-07</v>
+        <v>3.445820733470478e-07</v>
       </c>
       <c r="AF2" t="n">
-        <v>2574224.884633902</v>
+        <v>2578291.586265964</v>
       </c>
       <c r="AG2" t="n">
-        <v>3.884664490539321e-07</v>
+        <v>3.878537266020636e-07</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.003179084241090683</v>
+        <v>0.003179955621716659</v>
       </c>
       <c r="AI2" t="n">
-        <v>2.042545607351146e-05</v>
+        <v>2.043096046810692e-05</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.02815653470887956</v>
+        <v>0.02816511994251491</v>
       </c>
       <c r="AK2" t="n">
-        <v>3.196496677810477</v>
+        <v>3.203345775658089</v>
       </c>
       <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="n">
-        <v>2826844.848028497</v>
+        <v>2831548.010050902</v>
       </c>
       <c r="AO2" t="n">
-        <v>99.09345819806305</v>
+        <v>99.25431368764492</v>
       </c>
       <c r="AP2" t="n">
-        <v>99.09345819806305</v>
+        <v>99.25431368764492</v>
       </c>
       <c r="AQ2" t="n">
-        <v>462083.6247543594</v>
+        <v>462129.8952782032</v>
       </c>
       <c r="AR2" t="n">
-        <v>490610.682941978</v>
+        <v>490658.1063437881</v>
       </c>
       <c r="AS2" t="n">
         <v>1837.707528152812</v>
       </c>
       <c r="AT2" t="n">
-        <v>948.4580611086354</v>
+        <v>948.5497546943964</v>
       </c>
       <c r="AU2" t="n">
-        <v>1067.497370419139</v>
+        <v>1067.665980566446</v>
       </c>
       <c r="AV2" t="n">
-        <v>170.9917238401696</v>
+        <v>170.9932491693386</v>
       </c>
       <c r="AW2" t="n">
-        <v>0.9082306934989498</v>
+        <v>0.9081391249928659</v>
       </c>
       <c r="AX2" t="n">
-        <v>2.042545607351146e-05</v>
+        <v>2.043096046810692e-05</v>
       </c>
       <c r="AY2" t="n">
-        <v>0.02815653470887956</v>
+        <v>0.02816511994251491</v>
       </c>
       <c r="AZ2" t="n">
         <v>463.149999998658</v>
@@ -3840,37 +3840,37 @@
         <v>0.02952721766240145</v>
       </c>
       <c r="DP2" t="n">
-        <v>0.02239282692506289</v>
+        <v>0.01990831620277725</v>
       </c>
       <c r="DQ2" t="n">
         <v>0</v>
       </c>
       <c r="DR2" t="n">
-        <v>0.0115471027744396</v>
+        <v>0.01171926198267625</v>
       </c>
       <c r="DS2" t="n">
-        <v>0.04061155519819309</v>
+        <v>0.04195349286721551</v>
       </c>
       <c r="DT2" t="n">
         <v>0</v>
       </c>
       <c r="DU2" t="n">
-        <v>0.07455148489769559</v>
+        <v>0.07358107105266901</v>
       </c>
       <c r="DV2" t="n">
-        <v>-0.07455148488641798</v>
+        <v>-0.07358107104132414</v>
       </c>
       <c r="DW2" t="n">
-        <v>0.6957006261972732</v>
+        <v>0.6933591035374028</v>
       </c>
       <c r="DX2" t="n">
-        <v>0.6957006261972732</v>
+        <v>0.6933591035374028</v>
       </c>
       <c r="DY2" t="n">
-        <v>5997287.761595534</v>
+        <v>5980994.274455138</v>
       </c>
       <c r="DZ2" t="n">
-        <v>10.6599999587826</v>
+        <v>10.66000001140312</v>
       </c>
       <c r="EA2" t="n">
         <v>497686.3106530505</v>
@@ -3879,25 +3879,25 @@
         <v>0</v>
       </c>
       <c r="EC2" t="n">
-        <v>454.5928436220274</v>
+        <v>446.167482614168</v>
       </c>
       <c r="ED2" t="n">
-        <v>-14.39999999999901</v>
+        <v>-20.45482481504649</v>
       </c>
       <c r="EE2" t="n">
-        <v>0.005718931413538502</v>
+        <v>0.005053341098554821</v>
       </c>
       <c r="EF2" t="n">
         <v>0</v>
       </c>
       <c r="EG2" t="n">
-        <v>0.01042807666012172</v>
+        <v>0.01071125973372314</v>
       </c>
       <c r="EH2" t="n">
         <v>0</v>
       </c>
       <c r="EI2" t="n">
-        <v>0.00296410775031038</v>
+        <v>0.002991369580305403</v>
       </c>
     </row>
     <row r="3">
@@ -3905,406 +3905,406 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03412930154663323</v>
+        <v>0.03281173715281153</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01159638030554655</v>
+        <v>0.01172194538417859</v>
       </c>
       <c r="E3" t="n">
-        <v>0.009111793222892966</v>
+        <v>0.00898903580870326</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0268839855469697</v>
+        <v>0.0263037632265502</v>
       </c>
       <c r="G3" t="n">
-        <v>0.08172146062204244</v>
+        <v>0.07982648157224359</v>
       </c>
       <c r="H3" t="n">
-        <v>-1.000865281208796e-07</v>
+        <v>-2.140032434178041e-07</v>
       </c>
       <c r="I3" t="n">
-        <v>185.5038172636049</v>
+        <v>185.7269854854344</v>
       </c>
       <c r="J3" t="n">
-        <v>37.32616998900466</v>
+        <v>37.31472068893063</v>
       </c>
       <c r="K3" t="n">
-        <v>32.76350661959162</v>
+        <v>32.64119739861184</v>
       </c>
       <c r="L3" t="n">
-        <v>17.88282975471299</v>
+        <v>18.08149917672102</v>
       </c>
       <c r="M3" t="n">
-        <v>28.62639624978223</v>
+        <v>28.98413701803451</v>
       </c>
       <c r="N3" t="n">
-        <v>170.7929823484212</v>
+        <v>170.7936089181915</v>
       </c>
       <c r="O3" t="n">
-        <v>32.76350661959162</v>
+        <v>32.64119739861184</v>
       </c>
       <c r="P3" t="n">
-        <v>-167.6209875088919</v>
+        <v>-167.6454863087134</v>
       </c>
       <c r="Q3" t="n">
-        <v>-78.94030107298144</v>
+        <v>-78.98214644821354</v>
       </c>
       <c r="R3" t="n">
-        <v>437.5696701355757</v>
+        <v>437.6841392241788</v>
       </c>
       <c r="S3" t="n">
-        <v>1824302.817755626</v>
+        <v>1830542.222542533</v>
       </c>
       <c r="T3" t="n">
-        <v>64.66139356458564</v>
+        <v>64.87683310172842</v>
       </c>
       <c r="U3" t="n">
-        <v>450415.5537293874</v>
+        <v>450501.1948468437</v>
       </c>
       <c r="V3" t="n">
-        <v>478628.7226264273</v>
+        <v>478716.8480318905</v>
       </c>
       <c r="W3" t="n">
-        <v>1838.711065814882</v>
+        <v>1838.692310772849</v>
       </c>
       <c r="X3" t="n">
-        <v>-325935.4719168234</v>
+        <v>-326049.6133068401</v>
       </c>
       <c r="Y3" t="n">
-        <v>925.5698412401132</v>
+        <v>925.7370752676075</v>
       </c>
       <c r="Z3" t="n">
-        <v>1028.017721222832</v>
+        <v>1028.289799532081</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.110686277164622</v>
+        <v>1.110779536657131</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.9307406250479749</v>
+        <v>0.9305791393308286</v>
       </c>
       <c r="AC3" t="n">
-        <v>170.7929823175917</v>
+        <v>170.7936088914001</v>
       </c>
       <c r="AD3" t="n">
-        <v>1886188.550643211</v>
+        <v>1892486.859789735</v>
       </c>
       <c r="AE3" t="n">
-        <v>5.301696904368278e-07</v>
+        <v>5.284052540851487e-07</v>
       </c>
       <c r="AF3" t="n">
-        <v>1698219.010554721</v>
+        <v>1703746.600774746</v>
       </c>
       <c r="AG3" t="n">
-        <v>5.888521997368004e-07</v>
+        <v>5.869417432998953e-07</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.002985750839304567</v>
+        <v>0.002987002019409811</v>
       </c>
       <c r="AI3" t="n">
-        <v>1.922757614672969e-05</v>
+        <v>1.923527098137095e-05</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.02616832879336677</v>
+        <v>0.02618185202890959</v>
       </c>
       <c r="AK3" t="n">
-        <v>2.361041637648083</v>
+        <v>2.364217385293886</v>
       </c>
       <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="inlineStr"/>
       <c r="AN3" t="n">
-        <v>1824302.817755626</v>
+        <v>1830542.222542533</v>
       </c>
       <c r="AO3" t="n">
-        <v>64.66139356458564</v>
+        <v>64.87683310172842</v>
       </c>
       <c r="AP3" t="n">
-        <v>64.66139356458564</v>
+        <v>64.87683310172842</v>
       </c>
       <c r="AQ3" t="n">
-        <v>450415.5537293874</v>
+        <v>450501.1948468437</v>
       </c>
       <c r="AR3" t="n">
-        <v>478628.7226264273</v>
+        <v>478716.8480318905</v>
       </c>
       <c r="AS3" t="n">
-        <v>1838.711065814882</v>
+        <v>1838.692310772849</v>
       </c>
       <c r="AT3" t="n">
-        <v>925.5698412401132</v>
+        <v>925.7370752676075</v>
       </c>
       <c r="AU3" t="n">
-        <v>1028.017721222832</v>
+        <v>1028.289799532081</v>
       </c>
       <c r="AV3" t="n">
-        <v>170.7929823175917</v>
+        <v>170.7936088914001</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.9307406250479749</v>
+        <v>0.9305791393308286</v>
       </c>
       <c r="AX3" t="n">
-        <v>1.922757614672969e-05</v>
+        <v>1.923527098137095e-05</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.02616832879336677</v>
+        <v>0.02618185202890959</v>
       </c>
       <c r="AZ3" t="n">
-        <v>438.4562480774021</v>
+        <v>438.5705446342649</v>
       </c>
       <c r="BA3" t="n">
-        <v>1869889.455706534</v>
+        <v>1876252.351671242</v>
       </c>
       <c r="BB3" t="n">
-        <v>66.22398141145847</v>
+        <v>66.44364365269342</v>
       </c>
       <c r="BC3" t="n">
-        <v>451089.5084523014</v>
+        <v>451174.7902458925</v>
       </c>
       <c r="BD3" t="n">
-        <v>479325.344109609</v>
+        <v>479413.0422219366</v>
       </c>
       <c r="BE3" t="n">
-        <v>1838.711065815021</v>
+        <v>1838.692310773106</v>
       </c>
       <c r="BF3" t="n">
-        <v>-326869.0111060464</v>
+        <v>-326983.2459286597</v>
       </c>
       <c r="BG3" t="n">
-        <v>926.8399518668405</v>
+        <v>927.0069910937846</v>
       </c>
       <c r="BH3" t="n">
-        <v>1030.036036644316</v>
+        <v>1030.309956803415</v>
       </c>
       <c r="BI3" t="n">
-        <v>1.111341860662802</v>
+        <v>1.111437094544177</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0.9296048812146117</v>
+        <v>0.9294421468567994</v>
       </c>
       <c r="BK3" t="n">
-        <v>170.8136405703442</v>
+        <v>170.8141329377099</v>
       </c>
       <c r="BL3" t="n">
-        <v>1932236.959915899</v>
+        <v>1938657.28722813</v>
       </c>
       <c r="BM3" t="n">
-        <v>5.175348680026931e-07</v>
+        <v>5.158209274986341e-07</v>
       </c>
       <c r="BN3" t="n">
-        <v>1738652.190032253</v>
+        <v>1744279.812815869</v>
       </c>
       <c r="BO3" t="n">
-        <v>5.751581631639905e-07</v>
+        <v>5.733025129641642e-07</v>
       </c>
       <c r="BP3" t="n">
-        <v>0.002994123888756507</v>
+        <v>0.002995403326322593</v>
       </c>
       <c r="BQ3" t="n">
-        <v>1.9285670781927e-05</v>
+        <v>1.929346090078699e-05</v>
       </c>
       <c r="BR3" t="n">
-        <v>0.02627153652002328</v>
+        <v>0.02628514220530958</v>
       </c>
       <c r="BS3" t="n">
-        <v>2.385165116738592</v>
+        <v>2.388503707776606</v>
       </c>
       <c r="BT3" t="inlineStr"/>
       <c r="BU3" t="inlineStr"/>
       <c r="BV3" t="n">
-        <v>1869889.455706534</v>
+        <v>1876252.351671242</v>
       </c>
       <c r="BW3" t="n">
-        <v>66.22398141145847</v>
+        <v>66.44364365269342</v>
       </c>
       <c r="BX3" t="n">
-        <v>66.22398141145847</v>
+        <v>66.44364365269342</v>
       </c>
       <c r="BY3" t="n">
-        <v>451089.5084523014</v>
+        <v>451174.7902458925</v>
       </c>
       <c r="BZ3" t="n">
-        <v>479325.344109609</v>
+        <v>479413.0422219366</v>
       </c>
       <c r="CA3" t="n">
-        <v>1838.711065815021</v>
+        <v>1838.692310773106</v>
       </c>
       <c r="CB3" t="n">
-        <v>926.8399518668405</v>
+        <v>927.0069910937846</v>
       </c>
       <c r="CC3" t="n">
-        <v>1030.036036644316</v>
+        <v>1030.309956803415</v>
       </c>
       <c r="CD3" t="n">
-        <v>170.8136405703442</v>
+        <v>170.8141329377099</v>
       </c>
       <c r="CE3" t="n">
-        <v>0.9296048812146117</v>
+        <v>0.9294421468567994</v>
       </c>
       <c r="CF3" t="n">
-        <v>1.9285670781927e-05</v>
+        <v>1.929346090078699e-05</v>
       </c>
       <c r="CG3" t="n">
-        <v>0.02627153652002328</v>
+        <v>0.02628514220530958</v>
       </c>
       <c r="CH3" t="n">
-        <v>456.7429629219752</v>
+        <v>456.8670989261845</v>
       </c>
       <c r="CI3" t="n">
-        <v>3047390.770144956</v>
+        <v>3057715.885893652</v>
       </c>
       <c r="CJ3" t="n">
-        <v>106.4872265825234</v>
+        <v>106.8422115224492</v>
       </c>
       <c r="CK3" t="n">
-        <v>464596.4138716624</v>
+        <v>464683.0892375571</v>
       </c>
       <c r="CL3" t="n">
-        <v>493213.8440362404</v>
+        <v>493302.0764554618</v>
       </c>
       <c r="CM3" t="n">
-        <v>1838.711065814882</v>
+        <v>1838.692310772972</v>
       </c>
       <c r="CN3" t="n">
-        <v>-346604.4961214722</v>
+        <v>-346735.9453852685</v>
       </c>
       <c r="CO3" t="n">
-        <v>953.0148291227774</v>
+        <v>953.1960415863164</v>
       </c>
       <c r="CP3" t="n">
-        <v>1075.438181128929</v>
+        <v>1075.791138820839</v>
       </c>
       <c r="CQ3" t="n">
-        <v>1.128459021061444</v>
+        <v>1.12861477795323</v>
       </c>
       <c r="CR3" t="n">
-        <v>0.9044462866368876</v>
+        <v>0.90424973514617</v>
       </c>
       <c r="CS3" t="n">
-        <v>171.2052540470023</v>
+        <v>171.2067265336125</v>
       </c>
       <c r="CT3" t="n">
-        <v>3121272.55022363</v>
+        <v>3131731.46817248</v>
       </c>
       <c r="CU3" t="n">
-        <v>3.203821466755131e-07</v>
+        <v>3.193121792730044e-07</v>
       </c>
       <c r="CV3" t="n">
-        <v>2765960.032193033</v>
+        <v>2774845.349670105</v>
       </c>
       <c r="CW3" t="n">
-        <v>3.615381236030136e-07</v>
+        <v>3.603804443079639e-07</v>
       </c>
       <c r="CX3" t="n">
-        <v>0.003212343721803458</v>
+        <v>0.003214353612700892</v>
       </c>
       <c r="CY3" t="n">
-        <v>2.069639940914196e-05</v>
+        <v>2.070815687562728e-05</v>
       </c>
       <c r="CZ3" t="n">
-        <v>0.02858863389509057</v>
+        <v>0.02860617330842331</v>
       </c>
       <c r="DA3" t="n">
-        <v>3.598878927944934</v>
+        <v>3.622024986330358</v>
       </c>
       <c r="DB3" t="inlineStr"/>
       <c r="DC3" t="inlineStr"/>
       <c r="DD3" t="n">
-        <v>3047390.770144956</v>
+        <v>3057715.885893652</v>
       </c>
       <c r="DE3" t="n">
-        <v>106.4872265825234</v>
+        <v>106.8422115224492</v>
       </c>
       <c r="DF3" t="n">
-        <v>106.4872265825234</v>
+        <v>106.8422115224492</v>
       </c>
       <c r="DG3" t="n">
-        <v>464596.4138716624</v>
+        <v>464683.0892375571</v>
       </c>
       <c r="DH3" t="n">
-        <v>493213.8440362404</v>
+        <v>493302.0764554618</v>
       </c>
       <c r="DI3" t="n">
-        <v>1838.711065814882</v>
+        <v>1838.692310772972</v>
       </c>
       <c r="DJ3" t="n">
-        <v>953.0148291227774</v>
+        <v>953.1960415863164</v>
       </c>
       <c r="DK3" t="n">
-        <v>1075.438181128929</v>
+        <v>1075.791138820839</v>
       </c>
       <c r="DL3" t="n">
-        <v>171.2052540470023</v>
+        <v>171.2067265336125</v>
       </c>
       <c r="DM3" t="n">
-        <v>0.9044462866368876</v>
+        <v>0.90424973514617</v>
       </c>
       <c r="DN3" t="n">
-        <v>2.069639940914196e-05</v>
+        <v>2.070815687562728e-05</v>
       </c>
       <c r="DO3" t="n">
-        <v>0.02858863389509057</v>
+        <v>0.02860617330842331</v>
       </c>
       <c r="DP3" t="n">
-        <v>0.02199139760120455</v>
+        <v>0.02062880338743957</v>
       </c>
       <c r="DQ3" t="n">
         <v>0</v>
       </c>
       <c r="DR3" t="n">
-        <v>0.01159344036766186</v>
+        <v>0.01171733603980618</v>
       </c>
       <c r="DS3" t="n">
-        <v>0.01038675746226658</v>
+        <v>0.01025163958462825</v>
       </c>
       <c r="DT3" t="n">
-        <v>0.03221498031639532</v>
+        <v>0.03161933431089667</v>
       </c>
       <c r="DU3" t="n">
-        <v>0.07618657574752831</v>
+        <v>0.07421711332277067</v>
       </c>
       <c r="DV3" t="n">
-        <v>-0.07618657574111612</v>
+        <v>-0.07421711332277067</v>
       </c>
       <c r="DW3" t="n">
-        <v>0.2185462744575546</v>
+        <v>0.2184784368170204</v>
       </c>
       <c r="DX3" t="n">
-        <v>1.000000000180508</v>
+        <v>1.000000000156865</v>
       </c>
       <c r="DY3" t="n">
-        <v>4844453.94628886</v>
+        <v>4859720.791660261</v>
       </c>
       <c r="DZ3" t="n">
-        <v>10.65999997631805</v>
+        <v>10.6600002682561</v>
       </c>
       <c r="EA3" t="n">
-        <v>476008.0109265559</v>
+        <v>476054.8198867084</v>
       </c>
       <c r="EB3" t="n">
         <v>0</v>
       </c>
       <c r="EC3" t="n">
-        <v>1003.636092913803</v>
+        <v>985.0676128327614</v>
       </c>
       <c r="ED3" t="n">
-        <v>-55.51725745657214</v>
+        <v>-51.59049224650101</v>
       </c>
       <c r="EE3" t="n">
-        <v>0.01762101826518644</v>
+        <v>0.01702118925470615</v>
       </c>
       <c r="EF3" t="n">
         <v>0</v>
       </c>
       <c r="EG3" t="n">
-        <v>0.004704434826766555</v>
+        <v>0.0046630898877647</v>
       </c>
       <c r="EH3" t="n">
-        <v>0.01388024890333254</v>
+        <v>0.01364515782583999</v>
       </c>
       <c r="EI3" t="n">
-        <v>0.005987231496515689</v>
+        <v>0.006080795109634621</v>
       </c>
     </row>
   </sheetData>
@@ -4563,28 +4563,28 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.03498796705530414</v>
+        <v>0.03501846915341564</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05831327842550691</v>
+        <v>0.05836411525569274</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03841832361712644</v>
+        <v>0.03845183525768956</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05488292186368462</v>
+        <v>0.05493074915141882</v>
       </c>
       <c r="F2" t="n">
-        <v>0.007793731569723754</v>
+        <v>0.007788195703852473</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01039164209296501</v>
+        <v>0.01038426093846996</v>
       </c>
       <c r="H2" t="n">
-        <v>0.001460399667063102</v>
+        <v>0.001459362349238768</v>
       </c>
       <c r="I2" t="n">
-        <v>0.001880887218826678</v>
+        <v>0.00233197822466819</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -4592,13 +4592,13 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>14.39999999999901</v>
+        <v>20.45482481504649</v>
       </c>
       <c r="L2" t="n">
-        <v>79.19999999999999</v>
+        <v>79.20000000000002</v>
       </c>
       <c r="M2" t="n">
-        <v>46.7999999999995</v>
+        <v>-29.37258759247675</v>
       </c>
       <c r="N2" t="n">
         <v>0.01200896</v>
@@ -4607,7 +4607,7 @@
         <v>45</v>
       </c>
       <c r="P2" t="n">
-        <v>7.301998335315558e-05</v>
+        <v>7.296811746193841e-05</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -4622,67 +4622,67 @@
         <v>2</v>
       </c>
       <c r="U2" t="n">
-        <v>0.007113568520586003</v>
+        <v>0.009049349426384919</v>
       </c>
       <c r="V2" t="n">
-        <v>0.04665062274040553</v>
+        <v>0.04669129220455419</v>
       </c>
       <c r="W2" t="n">
-        <v>0.04665062274040553</v>
+        <v>0.04669129220455419</v>
       </c>
       <c r="X2" t="n">
-        <v>0.04665062274040553</v>
+        <v>0.04669129220455419</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.03841832361712644</v>
+        <v>0.03845183525768956</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.05488292186368462</v>
+        <v>0.05493074915141882</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.05831327842550691</v>
+        <v>0.05836411525569274</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.05488292186368462</v>
+        <v>0.05493074915141882</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.05488292186368462</v>
+        <v>0.05493074915141882</v>
       </c>
       <c r="AD2" t="n">
         <v>0.6</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.7000050710227835</v>
+        <v>0.7000056589742756</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.7000050710227835</v>
+        <v>0.7000056589742756</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.006836987151605674</v>
+        <v>0.006848913157765688</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.004826012604139102</v>
+        <v>0.004834419647158179</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.0009043045859708626</v>
+        <v>0.0009058799087435539</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.01989495480838048</v>
+        <v>0.01991227999800318</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.02332531137020277</v>
+        <v>0.02334564610227709</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.01646459824655819</v>
+        <v>0.01647891389372926</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.01646459824655819</v>
+        <v>0.01647891389372926</v>
       </c>
       <c r="AN2" t="n">
-        <v>-0.4493285826979359</v>
+        <v>-0.3626267605338406</v>
       </c>
       <c r="AO2" t="n">
-        <v>1.914515014123618</v>
+        <v>1.917544263957709</v>
       </c>
       <c r="AP2" t="n">
         <v>0.75</v>
@@ -4691,16 +4691,16 @@
         <v>1.333333333333333</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.1810000000000012</v>
+        <v>0.2245685310188081</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.05000000000000031</v>
+        <v>0.05</v>
       </c>
       <c r="AT2" t="n">
         <v>0</v>
       </c>
       <c r="AU2" t="n">
-        <v>1.155636413626091</v>
+        <v>1.156457842417183</v>
       </c>
     </row>
     <row r="3">
@@ -4708,28 +4708,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03841832361707791</v>
+        <v>0.03845183525769544</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05488292186373316</v>
+        <v>0.05493074915141296</v>
       </c>
       <c r="D3" t="n">
-        <v>0.03806731948749102</v>
+        <v>0.03811191556079215</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05523392599332005</v>
+        <v>0.05527066884831626</v>
       </c>
       <c r="F3" t="n">
-        <v>0.006325801395096079</v>
+        <v>0.006327171889564677</v>
       </c>
       <c r="G3" t="n">
-        <v>0.008434401860128105</v>
+        <v>0.008436229186086237</v>
       </c>
       <c r="H3" t="n">
-        <v>0.001213489178727771</v>
+        <v>0.001209216597332706</v>
       </c>
       <c r="I3" t="n">
-        <v>0.001504911326106501</v>
+        <v>0.001891013289459357</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -4737,13 +4737,13 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>-16.2</v>
+        <v>-20.34093714730382</v>
       </c>
       <c r="L3" t="n">
-        <v>-78.94030107298144</v>
+        <v>-78.98214644821354</v>
       </c>
       <c r="M3" t="n">
-        <v>-47.57015053649072</v>
+        <v>29.32060465045486</v>
       </c>
       <c r="N3" t="n">
         <v>0.01200896</v>
@@ -4752,7 +4752,7 @@
         <v>45</v>
       </c>
       <c r="P3" t="n">
-        <v>6.067445893638997e-05</v>
+        <v>6.046082986663532e-05</v>
       </c>
       <c r="Q3" t="n">
         <v>0.0005</v>
@@ -4763,67 +4763,67 @@
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
-        <v>0.005690581373715239</v>
+        <v>0.007355491070390359</v>
       </c>
       <c r="V3" t="n">
-        <v>0.04665062274040553</v>
+        <v>0.0466912922045542</v>
       </c>
       <c r="W3" t="n">
-        <v>0.04665062274040553</v>
+        <v>0.0466912922045542</v>
       </c>
       <c r="X3" t="n">
-        <v>0.04665062274040553</v>
+        <v>0.0466912922045542</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.03806731948749102</v>
+        <v>0.03811191556079215</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.05523392599332005</v>
+        <v>0.05527066884831626</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.05538292186373316</v>
+        <v>0.05543074915141296</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.05573392599332005</v>
+        <v>0.05577066884831626</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.05573392599332005</v>
+        <v>0.05577066884831626</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.7000050710212805</v>
+        <v>0.7000056589744573</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.689201768711767</v>
+        <v>0.6895504678147778</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.689201768711767</v>
+        <v>0.6895504678147778</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.00482601260416755</v>
+        <v>0.004834419647154736</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.00503178140922726</v>
+        <v>0.005033864158093129</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.0009652551366146885</v>
+        <v>0.0009620462656820981</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.01681560237624214</v>
+        <v>0.01681883359062082</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.01646459824665524</v>
+        <v>0.01647891389371752</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.01716660650582903</v>
+        <v>0.01715875328752411</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.01716660650582903</v>
+        <v>0.01715875328752411</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.06160354703910173</v>
+        <v>0.04618019660586769</v>
       </c>
       <c r="AO3" t="n">
-        <v>1.993692339433627</v>
+        <v>1.993643512952434</v>
       </c>
       <c r="AP3" t="n">
         <v>0.75</v>
@@ -4832,16 +4832,16 @@
         <v>1.333333333333333</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.1784253763412268</v>
+        <v>0.2241538544943967</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.05000000000000118</v>
+        <v>0.05</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.02973429014392153</v>
+        <v>0.02972857762733497</v>
       </c>
       <c r="AU3" t="n">
-        <v>1.423806951476889</v>
+        <v>1.423498548356916</v>
       </c>
     </row>
   </sheetData>
@@ -4855,7 +4855,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4935,10 +4935,10 @@
         <v>26</v>
       </c>
       <c r="H2" t="n">
-        <v>-6.258330249200093</v>
+        <v>-6.189646350986211</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4546790801976228</v>
+        <v>0.5071288016892547</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -4961,13 +4961,13 @@
         <v>52</v>
       </c>
       <c r="H3" t="n">
-        <v>-8.256412534726815</v>
+        <v>-7.752241401862241</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9364972605158474</v>
+        <v>1.567658567410162</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7927659177547192</v>
+        <v>0.6718379361474457</v>
       </c>
     </row>
     <row r="4">
@@ -4987,13 +4987,13 @@
         <v>78</v>
       </c>
       <c r="H4" t="n">
-        <v>-9.089999410175356</v>
+        <v>-9.496681167675767</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2630573109350501</v>
+        <v>0.7263584805820325</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5083279564860762</v>
+        <v>0.5604141555651215</v>
       </c>
     </row>
     <row r="5">
@@ -5007,19 +5007,19 @@
         <v>4</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H5" t="n">
-        <v>-9.217264126678476</v>
+        <v>-9.300263675083597</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1836350977086266</v>
+        <v>0.1496678225891009</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1714943290008779</v>
+        <v>0.2445503358458909</v>
       </c>
     </row>
     <row r="6">
@@ -5039,13 +5039,13 @@
         <v>131</v>
       </c>
       <c r="H6" t="n">
-        <v>-9.843958487607058</v>
+        <v>-9.890889008353167</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2277899682862147</v>
+        <v>0.1483108946310957</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3040637149052056</v>
+        <v>0.3465300081295161</v>
       </c>
     </row>
     <row r="7">
@@ -5065,13 +5065,13 @@
         <v>157</v>
       </c>
       <c r="H7" t="n">
-        <v>-9.160667685102833</v>
+        <v>-9.195105233675728</v>
       </c>
       <c r="I7" t="n">
-        <v>0.05091719415218562</v>
+        <v>0.03076324969639546</v>
       </c>
       <c r="J7" t="n">
-        <v>0.26025666668855</v>
+        <v>0.3406266508564865</v>
       </c>
     </row>
     <row r="8">
@@ -5085,19 +5085,19 @@
         <v>7</v>
       </c>
       <c r="F8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" t="n">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H8" t="n">
-        <v>-9.120404803262669</v>
+        <v>-9.081531617520348</v>
       </c>
       <c r="I8" t="n">
-        <v>0.02781704588931895</v>
+        <v>0.006286733515888293</v>
       </c>
       <c r="J8" t="n">
-        <v>0.04253520404710044</v>
+        <v>0.1413709544783197</v>
       </c>
     </row>
     <row r="9">
@@ -5111,19 +5111,19 @@
         <v>8</v>
       </c>
       <c r="F9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" t="n">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H9" t="n">
-        <v>-9.079952656632887</v>
+        <v>-9.06590253858932</v>
       </c>
       <c r="I9" t="n">
-        <v>0.00170973687966177</v>
+        <v>0.00102944946504707</v>
       </c>
       <c r="J9" t="n">
-        <v>0.05745285774544549</v>
+        <v>0.05793206929450177</v>
       </c>
     </row>
     <row r="10">
@@ -5143,13 +5143,13 @@
         <v>236</v>
       </c>
       <c r="H10" t="n">
-        <v>-9.07666302833068</v>
+        <v>-9.070622359159794</v>
       </c>
       <c r="I10" t="n">
-        <v>0.001678276230825639</v>
+        <v>0.001475100257618176</v>
       </c>
       <c r="J10" t="n">
-        <v>0.03754798166184733</v>
+        <v>0.04788031134677607</v>
       </c>
     </row>
     <row r="11">
@@ -5163,19 +5163,19 @@
         <v>10</v>
       </c>
       <c r="F11" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G11" t="n">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H11" t="n">
-        <v>-9.078812463347054</v>
+        <v>-9.077875183592001</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0001436823098264067</v>
+        <v>0.001836303600281859</v>
       </c>
       <c r="J11" t="n">
-        <v>0.1014157260613982</v>
+        <v>0.04556309085715757</v>
       </c>
     </row>
     <row r="12">
@@ -5189,19 +5189,19 @@
         <v>11</v>
       </c>
       <c r="F12" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G12" t="n">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="H12" t="n">
-        <v>-9.079966446301285</v>
+        <v>-9.082116416384093</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0001548143536957425</v>
+        <v>0.001841614343665628</v>
       </c>
       <c r="J12" t="n">
-        <v>0.07256156811878461</v>
+        <v>0.01983936589461483</v>
       </c>
     </row>
     <row r="13">
@@ -5215,19 +5215,19 @@
         <v>12</v>
       </c>
       <c r="F13" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G13" t="n">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H13" t="n">
-        <v>-9.08072294854491</v>
+        <v>-9.085263995600993</v>
       </c>
       <c r="I13" t="n">
-        <v>0.000144402403583696</v>
+        <v>0.001594988456161688</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0543663971902397</v>
+        <v>0.04356405300670656</v>
       </c>
     </row>
     <row r="14">
@@ -5241,19 +5241,19 @@
         <v>13</v>
       </c>
       <c r="F14" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G14" t="n">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H14" t="n">
-        <v>-9.081341394961781</v>
+        <v>-9.086501873525645</v>
       </c>
       <c r="I14" t="n">
-        <v>8.205237989726974e-05</v>
+        <v>0.001632993030477531</v>
       </c>
       <c r="J14" t="n">
-        <v>0.03582227549941989</v>
+        <v>0.02717900287357426</v>
       </c>
     </row>
     <row r="15">
@@ -5267,19 +5267,19 @@
         <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G15" t="n">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="H15" t="n">
-        <v>-9.081584540108077</v>
+        <v>-9.088408665613809</v>
       </c>
       <c r="I15" t="n">
-        <v>7.240306721313949e-05</v>
+        <v>0.001928486725397289</v>
       </c>
       <c r="J15" t="n">
-        <v>0.01299018682397973</v>
+        <v>0.03780797442089298</v>
       </c>
     </row>
     <row r="16">
@@ -5293,19 +5293,19 @@
         <v>15</v>
       </c>
       <c r="F16" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G16" t="n">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="H16" t="n">
-        <v>-9.081657277117952</v>
+        <v>-9.09017787268912</v>
       </c>
       <c r="I16" t="n">
-        <v>4.912159532383057e-05</v>
+        <v>0.002023580817964962</v>
       </c>
       <c r="J16" t="n">
-        <v>0.01134746486340791</v>
+        <v>0.03288958240280306</v>
       </c>
     </row>
     <row r="17">
@@ -5319,19 +5319,19 @@
         <v>16</v>
       </c>
       <c r="F17" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G17" t="n">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="H17" t="n">
-        <v>-9.08180690643341</v>
+        <v>-9.091399764010456</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0001029334331751468</v>
+        <v>0.00203286958733823</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0144843600145345</v>
+        <v>0.02021499614941741</v>
       </c>
     </row>
     <row r="18">
@@ -5345,19 +5345,19 @@
         <v>17</v>
       </c>
       <c r="F18" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G18" t="n">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="H18" t="n">
-        <v>-9.081942941550185</v>
+        <v>-9.092032036160104</v>
       </c>
       <c r="I18" t="n">
-        <v>0.000166006446628394</v>
+        <v>0.002010472187275882</v>
       </c>
       <c r="J18" t="n">
-        <v>0.01341719670262314</v>
+        <v>0.009861536603102279</v>
       </c>
     </row>
     <row r="19">
@@ -5371,19 +5371,19 @@
         <v>18</v>
       </c>
       <c r="F19" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G19" t="n">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="H19" t="n">
-        <v>-9.082115202188264</v>
+        <v>-9.09330659198983</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0002110268388439394</v>
+        <v>0.003420453499451466</v>
       </c>
       <c r="J19" t="n">
-        <v>0.01835201160963716</v>
+        <v>0.04122928416919467</v>
       </c>
     </row>
     <row r="20">
@@ -5397,19 +5397,19 @@
         <v>19</v>
       </c>
       <c r="F20" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G20" t="n">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="H20" t="n">
-        <v>-9.082246599412928</v>
+        <v>-9.093649247953991</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0002634822194884516</v>
+        <v>0.003383537952972054</v>
       </c>
       <c r="J20" t="n">
-        <v>0.01282192719564129</v>
+        <v>0.01388508155263614</v>
       </c>
     </row>
     <row r="21">
@@ -5423,19 +5423,19 @@
         <v>20</v>
       </c>
       <c r="F21" t="n">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G21" t="n">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="H21" t="n">
-        <v>-9.082408159524388</v>
+        <v>-9.093748907215414</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0002871026196866519</v>
+        <v>0.003338253718139878</v>
       </c>
       <c r="J21" t="n">
-        <v>0.01578214532393193</v>
+        <v>0.003270569722067655</v>
       </c>
     </row>
     <row r="22">
@@ -5449,19 +5449,19 @@
         <v>21</v>
       </c>
       <c r="F22" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G22" t="n">
-        <v>559</v>
+        <v>564</v>
       </c>
       <c r="H22" t="n">
-        <v>-9.082569949639479</v>
+        <v>-9.094453238107786</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0003465392486870578</v>
+        <v>0.0021953677132086</v>
       </c>
       <c r="J22" t="n">
-        <v>0.01313543255874142</v>
+        <v>0.05085854259632471</v>
       </c>
     </row>
     <row r="23">
@@ -5475,19 +5475,19 @@
         <v>22</v>
       </c>
       <c r="F23" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G23" t="n">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="H23" t="n">
-        <v>-9.082769402139686</v>
+        <v>-9.094976637302402</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0004168500989024224</v>
+        <v>0.002228415660775126</v>
       </c>
       <c r="J23" t="n">
-        <v>0.01422813365634195</v>
+        <v>0.02535134124030124</v>
       </c>
     </row>
     <row r="24">
@@ -5501,19 +5501,19 @@
         <v>23</v>
       </c>
       <c r="F24" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G24" t="n">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="H24" t="n">
-        <v>-9.083014622853554</v>
+        <v>-9.095369378572407</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0004768834418942844</v>
+        <v>0.00227008453603086</v>
       </c>
       <c r="J24" t="n">
-        <v>0.01274373436523665</v>
+        <v>0.0173880978420327</v>
       </c>
     </row>
     <row r="25">
@@ -5527,19 +5527,19 @@
         <v>24</v>
       </c>
       <c r="F25" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G25" t="n">
-        <v>642</v>
+        <v>648</v>
       </c>
       <c r="H25" t="n">
-        <v>-9.083238511961669</v>
+        <v>-9.095615313436644</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0004066109234916906</v>
+        <v>0.00225309963148512</v>
       </c>
       <c r="J25" t="n">
-        <v>0.01658070655874211</v>
+        <v>0.006653505788788408</v>
       </c>
     </row>
     <row r="26">
@@ -5553,19 +5553,19 @@
         <v>25</v>
       </c>
       <c r="F26" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G26" t="n">
-        <v>670</v>
+        <v>675</v>
       </c>
       <c r="H26" t="n">
-        <v>-9.08334541165566</v>
+        <v>-9.097522046629724</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0004172497670762339</v>
+        <v>0.001532497540545373</v>
       </c>
       <c r="J26" t="n">
-        <v>0.00614461473853484</v>
+        <v>0.02508431395830646</v>
       </c>
     </row>
     <row r="27">
@@ -5579,19 +5579,19 @@
         <v>26</v>
       </c>
       <c r="F27" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G27" t="n">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="H27" t="n">
-        <v>-9.08336925076874</v>
+        <v>-9.096637655546465</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0004070688553406457</v>
+        <v>0.0007940574642495569</v>
       </c>
       <c r="J27" t="n">
-        <v>0.001282374122382684</v>
+        <v>0.01273055300187943</v>
       </c>
     </row>
     <row r="28">
@@ -5605,19 +5605,19 @@
         <v>27</v>
       </c>
       <c r="F28" t="n">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G28" t="n">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="H28" t="n">
-        <v>-9.083439105361558</v>
+        <v>-9.096101241833038</v>
       </c>
       <c r="I28" t="n">
-        <v>1.070180232903839e-06</v>
+        <v>0.0001381687141435066</v>
       </c>
       <c r="J28" t="n">
-        <v>0.00574989523083606</v>
+        <v>0.01565537983999782</v>
       </c>
     </row>
     <row r="29">
@@ -5631,19 +5631,19 @@
         <v>28</v>
       </c>
       <c r="F29" t="n">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G29" t="n">
-        <v>752</v>
+        <v>756</v>
       </c>
       <c r="H29" t="n">
-        <v>-9.083665407261968</v>
+        <v>-9.096393514862584</v>
       </c>
       <c r="I29" t="n">
-        <v>3.184987008920948e-05</v>
+        <v>0.0001158676477887318</v>
       </c>
       <c r="J29" t="n">
-        <v>0.01543794457007689</v>
+        <v>0.003093657506161159</v>
       </c>
     </row>
     <row r="30">
@@ -5657,19 +5657,19 @@
         <v>29</v>
       </c>
       <c r="F30" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G30" t="n">
-        <v>778</v>
+        <v>782</v>
       </c>
       <c r="H30" t="n">
-        <v>-9.083535232719674</v>
+        <v>-9.096014893381966</v>
       </c>
       <c r="I30" t="n">
-        <v>2.19970531423197e-06</v>
+        <v>1.787399433339498e-05</v>
       </c>
       <c r="J30" t="n">
-        <v>0.007324279260261699</v>
+        <v>0.007623377666189066</v>
       </c>
     </row>
     <row r="31">
@@ -5683,19 +5683,19 @@
         <v>30</v>
       </c>
       <c r="F31" t="n">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G31" t="n">
-        <v>804</v>
+        <v>809</v>
       </c>
       <c r="H31" t="n">
-        <v>-9.083672363841837</v>
+        <v>-9.096003924192033</v>
       </c>
       <c r="I31" t="n">
-        <v>2.770028558428395e-05</v>
+        <v>1.615283925761324e-05</v>
       </c>
       <c r="J31" t="n">
-        <v>0.02394207299141612</v>
+        <v>0.002533466140196182</v>
       </c>
     </row>
     <row r="32">
@@ -5709,19 +5709,19 @@
         <v>31</v>
       </c>
       <c r="F32" t="n">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G32" t="n">
-        <v>830</v>
+        <v>836</v>
       </c>
       <c r="H32" t="n">
-        <v>-9.083616478679565</v>
+        <v>-9.095978452662774</v>
       </c>
       <c r="I32" t="n">
-        <v>5.43856616505578e-07</v>
+        <v>8.282510081905614e-06</v>
       </c>
       <c r="J32" t="n">
-        <v>0.003100851469937611</v>
+        <v>0.0006994250033431103</v>
       </c>
     </row>
     <row r="33">
@@ -5735,19 +5735,19 @@
         <v>32</v>
       </c>
       <c r="F33" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G33" t="n">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="H33" t="n">
-        <v>-9.083616479147675</v>
+        <v>-9.095975160391889</v>
       </c>
       <c r="I33" t="n">
-        <v>5.438444161121048e-07</v>
+        <v>8.43503152620471e-06</v>
       </c>
       <c r="J33" t="n">
-        <v>1.551025206175806e-07</v>
+        <v>0.001041808901190885</v>
       </c>
     </row>
     <row r="34">
@@ -5761,19 +5761,19 @@
         <v>33</v>
       </c>
       <c r="F34" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G34" t="n">
-        <v>888</v>
+        <v>892</v>
       </c>
       <c r="H34" t="n">
-        <v>-9.732843571512268</v>
+        <v>-9.095977735418831</v>
       </c>
       <c r="I34" t="n">
-        <v>0.144434172252016</v>
+        <v>8.148653669774849e-06</v>
       </c>
       <c r="J34" t="n">
-        <v>0.2375421917851947</v>
+        <v>0.0001854080707795143</v>
       </c>
     </row>
     <row r="35">
@@ -5787,19 +5787,19 @@
         <v>34</v>
       </c>
       <c r="F35" t="n">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="G35" t="n">
-        <v>914</v>
+        <v>924</v>
       </c>
       <c r="H35" t="n">
-        <v>-9.117530334469242</v>
+        <v>-9.095978171011788</v>
       </c>
       <c r="I35" t="n">
-        <v>0.02255177478702066</v>
+        <v>8.036339746926536e-06</v>
       </c>
       <c r="J35" t="n">
-        <v>0.2788665945867921</v>
+        <v>5.271416797787628e-05</v>
       </c>
     </row>
     <row r="36">
@@ -5813,19 +5813,19 @@
         <v>35</v>
       </c>
       <c r="F36" t="n">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G36" t="n">
-        <v>941</v>
+        <v>950</v>
       </c>
       <c r="H36" t="n">
-        <v>-9.107688063423769</v>
+        <v>-9.095963063275995</v>
       </c>
       <c r="I36" t="n">
-        <v>0.01395344405971485</v>
+        <v>6.275958443352492e-07</v>
       </c>
       <c r="J36" t="n">
-        <v>0.1797553805133415</v>
+        <v>0.002506039004703238</v>
       </c>
     </row>
     <row r="37">
@@ -5839,19 +5839,19 @@
         <v>36</v>
       </c>
       <c r="F37" t="n">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="G37" t="n">
-        <v>967</v>
+        <v>977</v>
       </c>
       <c r="H37" t="n">
-        <v>-9.097459315225183</v>
+        <v>-9.095995645159885</v>
       </c>
       <c r="I37" t="n">
-        <v>0.01284823643320517</v>
+        <v>1.031688616426329e-06</v>
       </c>
       <c r="J37" t="n">
-        <v>0.06063376458664391</v>
+        <v>0.003794430927013315</v>
       </c>
     </row>
     <row r="38">
@@ -5865,19 +5865,19 @@
         <v>37</v>
       </c>
       <c r="F38" t="n">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="G38" t="n">
-        <v>993</v>
+        <v>1005</v>
       </c>
       <c r="H38" t="n">
-        <v>-9.084479828153999</v>
+        <v>-9.096000767550072</v>
       </c>
       <c r="I38" t="n">
-        <v>0.000482898925693505</v>
+        <v>1.022634071687345e-06</v>
       </c>
       <c r="J38" t="n">
-        <v>0.01798458190849382</v>
+        <v>0.0005004136524344271</v>
       </c>
     </row>
     <row r="39">
@@ -5891,19 +5891,19 @@
         <v>38</v>
       </c>
       <c r="F39" t="n">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="G39" t="n">
-        <v>1019</v>
+        <v>1035</v>
       </c>
       <c r="H39" t="n">
-        <v>-9.084193180411106</v>
+        <v>-9.096001137022503</v>
       </c>
       <c r="I39" t="n">
-        <v>0.0001181464120189046</v>
+        <v>1.064625459581969e-06</v>
       </c>
       <c r="J39" t="n">
-        <v>0.01675343240250649</v>
+        <v>3.090884234407413e-05</v>
       </c>
     </row>
     <row r="40">
@@ -5917,19 +5917,19 @@
         <v>39</v>
       </c>
       <c r="F40" t="n">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="G40" t="n">
-        <v>1045</v>
+        <v>1061</v>
       </c>
       <c r="H40" t="n">
-        <v>-9.083944531093127</v>
+        <v>-9.096013189538182</v>
       </c>
       <c r="I40" t="n">
-        <v>2.226940050099879e-05</v>
+        <v>1.064179953325084e-06</v>
       </c>
       <c r="J40" t="n">
-        <v>0.02458814978882919</v>
+        <v>0.001150335597515673</v>
       </c>
     </row>
     <row r="41">
@@ -5943,19 +5943,19 @@
         <v>40</v>
       </c>
       <c r="F41" t="n">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="G41" t="n">
-        <v>1072</v>
+        <v>1087</v>
       </c>
       <c r="H41" t="n">
-        <v>-9.08401171099854</v>
+        <v>-9.096021684611049</v>
       </c>
       <c r="I41" t="n">
-        <v>1.852559133454224e-05</v>
+        <v>6.227453297202867e-07</v>
       </c>
       <c r="J41" t="n">
-        <v>0.0119387803431142</v>
+        <v>0.002369828290658145</v>
       </c>
     </row>
     <row r="42">
@@ -5969,19 +5969,19 @@
         <v>41</v>
       </c>
       <c r="F42" t="n">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="G42" t="n">
-        <v>1100</v>
+        <v>1114</v>
       </c>
       <c r="H42" t="n">
-        <v>-9.084018733975931</v>
+        <v>-9.09602333252176</v>
       </c>
       <c r="I42" t="n">
-        <v>1.682621054362177e-05</v>
+        <v>7.078089467454918e-07</v>
       </c>
       <c r="J42" t="n">
-        <v>0.001848148665591283</v>
+        <v>0.0008189999136877914</v>
       </c>
     </row>
     <row r="43">
@@ -5995,19 +5995,19 @@
         <v>42</v>
       </c>
       <c r="F43" t="n">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="G43" t="n">
-        <v>1129</v>
+        <v>1141</v>
       </c>
       <c r="H43" t="n">
-        <v>-9.084019894523855</v>
+        <v>-9.096024374444724</v>
       </c>
       <c r="I43" t="n">
-        <v>1.657391141361708e-05</v>
+        <v>6.938351490709538e-07</v>
       </c>
       <c r="J43" t="n">
-        <v>0.0001891616384545366</v>
+        <v>0.0006630550048367174</v>
       </c>
     </row>
     <row r="44">
@@ -6021,19 +6021,19 @@
         <v>43</v>
       </c>
       <c r="F44" t="n">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G44" t="n">
-        <v>1155</v>
+        <v>1167</v>
       </c>
       <c r="H44" t="n">
-        <v>-9.083993497256534</v>
+        <v>-9.096022570562324</v>
       </c>
       <c r="I44" t="n">
-        <v>1.191697099903188e-06</v>
+        <v>2.140032434178041e-07</v>
       </c>
       <c r="J44" t="n">
-        <v>0.002133605762493981</v>
+        <v>0.0001301758959302501</v>
       </c>
     </row>
     <row r="45">
@@ -6044,177 +6044,21 @@
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F45" t="n">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="G45" t="n">
-        <v>1181</v>
+        <v>1169</v>
       </c>
       <c r="H45" t="n">
-        <v>-9.084013294140009</v>
+        <v>-9.096022570562324</v>
       </c>
       <c r="I45" t="n">
-        <v>2.849347304692504e-06</v>
+        <v>2.140032434178041e-07</v>
       </c>
       <c r="J45" t="n">
-        <v>0.002147951568342412</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="n">
-        <v>45</v>
-      </c>
-      <c r="F46" t="n">
-        <v>82</v>
-      </c>
-      <c r="G46" t="n">
-        <v>1207</v>
-      </c>
-      <c r="H46" t="n">
-        <v>-9.084017210274235</v>
-      </c>
-      <c r="I46" t="n">
-        <v>7.551696224877835e-07</v>
-      </c>
-      <c r="J46" t="n">
-        <v>0.001119833865891155</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="n">
-        <v>46</v>
-      </c>
-      <c r="F47" t="n">
-        <v>83</v>
-      </c>
-      <c r="G47" t="n">
-        <v>1233</v>
-      </c>
-      <c r="H47" t="n">
-        <v>-9.084023801589989</v>
-      </c>
-      <c r="I47" t="n">
-        <v>5.044237878504276e-07</v>
-      </c>
-      <c r="J47" t="n">
-        <v>0.002163701717047986</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="inlineStr"/>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="n">
-        <v>47</v>
-      </c>
-      <c r="F48" t="n">
-        <v>85</v>
-      </c>
-      <c r="G48" t="n">
-        <v>1260</v>
-      </c>
-      <c r="H48" t="n">
-        <v>-9.084042119394896</v>
-      </c>
-      <c r="I48" t="n">
-        <v>2.443342505598078e-06</v>
-      </c>
-      <c r="J48" t="n">
-        <v>0.003881622795160715</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="n">
-        <v>48</v>
-      </c>
-      <c r="F49" t="n">
-        <v>86</v>
-      </c>
-      <c r="G49" t="n">
-        <v>1286</v>
-      </c>
-      <c r="H49" t="n">
-        <v>-9.084033201173645</v>
-      </c>
-      <c r="I49" t="n">
-        <v>6.732448429164206e-07</v>
-      </c>
-      <c r="J49" t="n">
-        <v>0.002768131726134983</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="n">
-        <v>49</v>
-      </c>
-      <c r="F50" t="n">
-        <v>87</v>
-      </c>
-      <c r="G50" t="n">
-        <v>1312</v>
-      </c>
-      <c r="H50" t="n">
-        <v>-9.084031265372248</v>
-      </c>
-      <c r="I50" t="n">
-        <v>1.000865281208796e-07</v>
-      </c>
-      <c r="J50" t="n">
-        <v>0.0008758053270857481</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="n">
-        <v>49</v>
-      </c>
-      <c r="F51" t="n">
-        <v>91</v>
-      </c>
-      <c r="G51" t="n">
-        <v>1316</v>
-      </c>
-      <c r="H51" t="n">
-        <v>-9.084031265372248</v>
-      </c>
-      <c r="I51" t="n">
-        <v>1.000865281208796e-07</v>
-      </c>
-      <c r="J51" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>